<commit_message>
Changes of 10th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755"/>
+    <workbookView windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
+    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>FileName</t>
   </si>
@@ -32,6 +32,12 @@
     <t>RT00002183</t>
   </si>
   <si>
+    <t>RTE Job Creation ForCrud</t>
+  </si>
+  <si>
+    <t>RT00002194</t>
+  </si>
+  <si>
     <t>JobID</t>
   </si>
   <si>
@@ -39,12 +45,37 @@
   </si>
   <si>
     <t>BOLNo</t>
+  </si>
+  <si>
+    <t>125960302</t>
+  </si>
+  <si>
+    <t>125960324</t>
+  </si>
+  <si>
+    <t>32391789</t>
+  </si>
+  <si>
+    <t>3397027</t>
+  </si>
+  <si>
+    <t>125960313</t>
+  </si>
+  <si>
+    <t>32391790</t>
+  </si>
+  <si>
+    <t>3397028</t>
+  </si>
+  <si>
+    <t>125960335</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,100 +484,100 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -628,10 +659,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -789,7 +820,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -798,13 +829,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -814,7 +845,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -823,7 +854,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -832,7 +863,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -842,12 +873,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -878,7 +909,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -897,7 +928,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -909,18 +940,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -941,28 +972,38 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>125928131</v>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -970,31 +1011,45 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>125928131</v>
-      </c>
-      <c r="B2">
-        <v>32388271</v>
-      </c>
-      <c r="C2">
-        <v>3393509</v>
-      </c>
-      <c r="D2">
-        <v>125928142</v>
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes of 11th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>FileName</t>
   </si>
@@ -69,6 +69,30 @@
   </si>
   <si>
     <t>125960335</t>
+  </si>
+  <si>
+    <t>125980979</t>
+  </si>
+  <si>
+    <t>125980991</t>
+  </si>
+  <si>
+    <t>32393886</t>
+  </si>
+  <si>
+    <t>3399124</t>
+  </si>
+  <si>
+    <t>125980980</t>
+  </si>
+  <si>
+    <t>32393887</t>
+  </si>
+  <si>
+    <t>3399125</t>
+  </si>
+  <si>
+    <t>125981002</t>
   </si>
 </sst>
 </file>
@@ -973,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,7 +1008,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1022,30 +1046,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes of 12th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>FileName</t>
   </si>
@@ -47,30 +50,6 @@
     <t>BOLNo</t>
   </si>
   <si>
-    <t>125960302</t>
-  </si>
-  <si>
-    <t>125960324</t>
-  </si>
-  <si>
-    <t>32391789</t>
-  </si>
-  <si>
-    <t>3397027</t>
-  </si>
-  <si>
-    <t>125960313</t>
-  </si>
-  <si>
-    <t>32391790</t>
-  </si>
-  <si>
-    <t>3397028</t>
-  </si>
-  <si>
-    <t>125960335</t>
-  </si>
-  <si>
     <t>125980979</t>
   </si>
   <si>
@@ -93,13 +72,159 @@
   </si>
   <si>
     <t>125981002</t>
+  </si>
+  <si>
+    <t>PickUpID</t>
+  </si>
+  <si>
+    <t>ChargeName</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>RateProgramID</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>BR - Base Rate</t>
+  </si>
+  <si>
+    <t>$520.00</t>
+  </si>
+  <si>
+    <t>764 Minute(s)</t>
+  </si>
+  <si>
+    <t>Scheduler</t>
+  </si>
+  <si>
+    <t>228927</t>
+  </si>
+  <si>
+    <t>Total :US$520.00</t>
+  </si>
+  <si>
+    <t>Total Revenue :</t>
+  </si>
+  <si>
+    <t>US$520.00</t>
+  </si>
+  <si>
+    <t>Total Cost :</t>
+  </si>
+  <si>
+    <t>US$0.00</t>
+  </si>
+  <si>
+    <t>Margin($) :</t>
+  </si>
+  <si>
+    <t>Margin(%) :</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>Stop#</t>
+  </si>
+  <si>
+    <t>PU/DEL</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Miles</t>
+  </si>
+  <si>
+    <t>Est.Minutes</t>
+  </si>
+  <si>
+    <t>ETA/POD</t>
+  </si>
+  <si>
+    <t>Shipment</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PUStop</t>
+  </si>
+  <si>
+    <t>DelStop</t>
+  </si>
+  <si>
+    <t>PCs.</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2/0</t>
+  </si>
+  <si>
+    <t>Test company order 1</t>
+  </si>
+  <si>
+    <t>Test company order 1, 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2022-05-11 00:30</t>
+  </si>
+  <si>
+    <t>CDT</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0/2</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
+  </si>
+  <si>
+    <t>824</t>
+  </si>
+  <si>
+    <t>764</t>
+  </si>
+  <si>
+    <t>2022-05-11 13:14</t>
+  </si>
+  <si>
+    <t>Received</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +498,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -508,100 +639,114 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -683,10 +828,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -844,7 +989,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -853,13 +998,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -869,7 +1014,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -878,7 +1023,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -887,7 +1032,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -897,12 +1042,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -933,7 +1078,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -952,7 +1097,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -964,18 +1109,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -997,7 +1142,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1008,26 +1153,26 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,35 +1191,619 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="8"/>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8"/>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 13th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" activeTab="4"/>
+    <workbookView activeTab="4" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
-    <sheet name="Rate" sheetId="3" r:id="rId3"/>
-    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
-    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
+    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
+    <sheet name="Rate" r:id="rId3" sheetId="3"/>
+    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
+    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>FileName</t>
   </si>
@@ -219,12 +219,37 @@
   </si>
   <si>
     <t>Received</t>
+  </si>
+  <si>
+    <t>125999607</t>
+  </si>
+  <si>
+    <t>125999629</t>
+  </si>
+  <si>
+    <t>32395765</t>
+  </si>
+  <si>
+    <t>3401003</t>
+  </si>
+  <si>
+    <t>125999618</t>
+  </si>
+  <si>
+    <t>32395766</t>
+  </si>
+  <si>
+    <t>3401004</t>
+  </si>
+  <si>
+    <t>125999630</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,114 +664,114 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -828,10 +853,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -989,7 +1014,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -998,13 +1023,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1014,7 +1039,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1023,7 +1048,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1032,7 +1057,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1042,12 +1067,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1078,7 +1103,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1097,7 +1122,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1109,8 +1134,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1118,9 +1143,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1142,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1153,18 +1178,18 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1172,7 +1197,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1191,42 +1216,42 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1234,15 +1259,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1286,10 +1311,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1444,14 +1469,14 @@
       <c r="M10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -1459,16 +1484,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1503,9 +1528,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="8"/>
+    <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
@@ -1534,7 +1563,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="C3" t="s">
@@ -1670,13 +1699,13 @@
       <c r="K11" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
@@ -1684,11 +1713,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1804,6 +1833,6 @@
       <c r="F11" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 18th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="4" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>FileName</t>
   </si>
@@ -50,24 +51,6 @@
     <t>BOLNo</t>
   </si>
   <si>
-    <t>125980979</t>
-  </si>
-  <si>
-    <t>125980991</t>
-  </si>
-  <si>
-    <t>32393886</t>
-  </si>
-  <si>
-    <t>3399124</t>
-  </si>
-  <si>
-    <t>125980980</t>
-  </si>
-  <si>
-    <t>32393887</t>
-  </si>
-  <si>
     <t>3399125</t>
   </si>
   <si>
@@ -221,59 +204,34 @@
     <t>Received</t>
   </si>
   <si>
-    <t>125999607</t>
-  </si>
-  <si>
-    <t>125999629</t>
-  </si>
-  <si>
-    <t>32395765</t>
-  </si>
-  <si>
-    <t>3401003</t>
-  </si>
-  <si>
-    <t>125999618</t>
-  </si>
-  <si>
-    <t>32395766</t>
-  </si>
-  <si>
-    <t>3401004</t>
-  </si>
-  <si>
-    <t>125999630</t>
-  </si>
-  <si>
-    <t>126040034</t>
-  </si>
-  <si>
-    <t>126040056</t>
-  </si>
-  <si>
-    <t>32399896</t>
-  </si>
-  <si>
-    <t>3405134</t>
-  </si>
-  <si>
-    <t>126040045</t>
-  </si>
-  <si>
-    <t>32399897</t>
-  </si>
-  <si>
-    <t>3405135</t>
-  </si>
-  <si>
-    <t>126040067</t>
+    <t>126092907</t>
+  </si>
+  <si>
+    <t>126092929</t>
+  </si>
+  <si>
+    <t>32404842</t>
+  </si>
+  <si>
+    <t>3410080</t>
+  </si>
+  <si>
+    <t>126092918</t>
+  </si>
+  <si>
+    <t>32404843</t>
+  </si>
+  <si>
+    <t>3410081</t>
+  </si>
+  <si>
+    <t>126092930</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -688,114 +646,114 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -877,10 +835,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1038,7 +996,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1047,13 +1005,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1063,7 +1021,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1072,7 +1030,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1081,7 +1039,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1091,12 +1049,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1127,7 +1085,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1146,7 +1104,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1158,8 +1116,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1167,9 +1125,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1191,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1202,26 +1160,27 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,42 +1199,42 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1283,15 +1242,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1299,76 +1258,76 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="M2" s="2"/>
     </row>
@@ -1493,14 +1452,14 @@
       <c r="M10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -1508,114 +1467,114 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="K2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1723,65 +1682,63 @@
       <c r="K11" s="8"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,6 +1814,32 @@
       <c r="F11" s="6"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 27th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,22 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
-    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
+    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
+    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
+    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
   <si>
     <t>FileName</t>
   </si>
@@ -279,53 +282,127 @@
     <t>RT00002274</t>
   </si>
   <si>
-    <t>126194993</t>
-  </si>
-  <si>
-    <t>126195015</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>126212514</t>
-  </si>
-  <si>
-    <t>126212536</t>
-  </si>
-  <si>
-    <t>32417000</t>
-  </si>
-  <si>
-    <t>3422238</t>
-  </si>
-  <si>
-    <t>126212525</t>
-  </si>
-  <si>
-    <t>32417001</t>
-  </si>
-  <si>
-    <t>3422239</t>
-  </si>
-  <si>
-    <t>126212547</t>
-  </si>
-  <si>
-    <t>2022-05-26 00:30</t>
-  </si>
-  <si>
-    <t>2022-05-26 13:14</t>
-  </si>
-  <si>
-    <t>3422774</t>
+    <t>32418774</t>
+  </si>
+  <si>
+    <t>3424011</t>
+  </si>
+  <si>
+    <t>126229662</t>
+  </si>
+  <si>
+    <t>32418880</t>
+  </si>
+  <si>
+    <t>3424117</t>
+  </si>
+  <si>
+    <t>126230752</t>
+  </si>
+  <si>
+    <t>32418683</t>
+  </si>
+  <si>
+    <t>3423920</t>
+  </si>
+  <si>
+    <t>126228986</t>
+  </si>
+  <si>
+    <t>32418779</t>
+  </si>
+  <si>
+    <t>3424016</t>
+  </si>
+  <si>
+    <t>126229710</t>
+  </si>
+  <si>
+    <t>32418778</t>
+  </si>
+  <si>
+    <t>3424015</t>
+  </si>
+  <si>
+    <t>126229709</t>
+  </si>
+  <si>
+    <t>32418777</t>
+  </si>
+  <si>
+    <t>3424014</t>
+  </si>
+  <si>
+    <t>126229695</t>
+  </si>
+  <si>
+    <t>32418776</t>
+  </si>
+  <si>
+    <t>3424013</t>
+  </si>
+  <si>
+    <t>126229684</t>
+  </si>
+  <si>
+    <t>32418775</t>
+  </si>
+  <si>
+    <t>3424012</t>
+  </si>
+  <si>
+    <t>126229673</t>
+  </si>
+  <si>
+    <t>32418883</t>
+  </si>
+  <si>
+    <t>3424120</t>
+  </si>
+  <si>
+    <t>126230785</t>
+  </si>
+  <si>
+    <t>32418882</t>
+  </si>
+  <si>
+    <t>3424119</t>
+  </si>
+  <si>
+    <t>126230774</t>
+  </si>
+  <si>
+    <t>32418881</t>
+  </si>
+  <si>
+    <t>3424118</t>
+  </si>
+  <si>
+    <t>126230763</t>
+  </si>
+  <si>
+    <t>32418685</t>
+  </si>
+  <si>
+    <t>3423922</t>
+  </si>
+  <si>
+    <t>126229008</t>
+  </si>
+  <si>
+    <t>32418684</t>
+  </si>
+  <si>
+    <t>3423921</t>
+  </si>
+  <si>
+    <t>126228997</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -740,116 +817,116 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -931,10 +1008,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1092,7 +1169,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1101,13 +1178,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1117,7 +1194,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1126,7 +1203,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1135,7 +1212,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1145,12 +1222,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1181,7 +1258,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1200,7 +1277,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1212,19 +1289,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,8 +1325,8 @@
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>89</v>
+      <c r="C2" s="5">
+        <v>126229617</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>75</v>
@@ -1262,8 +1339,8 @@
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>90</v>
+      <c r="C3" s="5">
+        <v>126229639</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>75</v>
@@ -1276,8 +1353,8 @@
       <c r="B4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C4" t="s">
-        <v>88</v>
+      <c r="C4" s="5">
+        <v>126229651</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>76</v>
@@ -1290,8 +1367,8 @@
       <c r="B5" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C5" t="s">
-        <v>88</v>
+      <c r="C5" s="5">
+        <v>126230741</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>77</v>
@@ -1304,8 +1381,8 @@
       <c r="B6" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
-        <v>88</v>
+      <c r="C6" s="5">
+        <v>126228975</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>78</v>
@@ -1324,24 +1401,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1359,79 +1436,49 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s">
-        <v>93</v>
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" t="s">
-        <v>96</v>
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1439,15 +1486,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1491,10 +1538,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1659,14 +1706,14 @@
       <c r="M10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -1674,16 +1721,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1718,12 +1765,12 @@
         <v>40</v>
       </c>
     </row>
-    <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -1747,13 +1794,13 @@
         <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" t="s">
@@ -1778,7 +1825,7 @@
         <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="K3" t="s">
         <v>46</v>
@@ -1889,23 +1936,23 @@
       <c r="K11" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1930,10 +1977,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
@@ -2021,13 +2068,13 @@
       <c r="F11" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
@@ -2035,7 +2082,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="10" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2045,10 +2092,458 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
         <v>99</v>
       </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>126229651</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>126230741</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 31st May 2022 OneToMany
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
   <si>
     <t>FileName</t>
   </si>
@@ -210,21 +210,9 @@
     <t>US$520.00</t>
   </si>
   <si>
-    <t>126175286</t>
-  </si>
-  <si>
     <t>126175301</t>
   </si>
   <si>
-    <t>32413152</t>
-  </si>
-  <si>
-    <t>3418390</t>
-  </si>
-  <si>
-    <t>126175297</t>
-  </si>
-  <si>
     <t>3418391</t>
   </si>
   <si>
@@ -282,121 +270,142 @@
     <t>RT00002274</t>
   </si>
   <si>
-    <t>32418774</t>
-  </si>
-  <si>
-    <t>3424011</t>
-  </si>
-  <si>
-    <t>126229662</t>
-  </si>
-  <si>
-    <t>32418880</t>
-  </si>
-  <si>
-    <t>3424117</t>
-  </si>
-  <si>
-    <t>126230752</t>
-  </si>
-  <si>
-    <t>32418683</t>
-  </si>
-  <si>
-    <t>3423920</t>
-  </si>
-  <si>
-    <t>126228986</t>
-  </si>
-  <si>
-    <t>32418779</t>
-  </si>
-  <si>
-    <t>3424016</t>
-  </si>
-  <si>
-    <t>126229710</t>
-  </si>
-  <si>
-    <t>32418778</t>
-  </si>
-  <si>
-    <t>3424015</t>
-  </si>
-  <si>
-    <t>126229709</t>
-  </si>
-  <si>
-    <t>32418777</t>
-  </si>
-  <si>
-    <t>3424014</t>
-  </si>
-  <si>
-    <t>126229695</t>
-  </si>
-  <si>
-    <t>32418776</t>
-  </si>
-  <si>
-    <t>3424013</t>
-  </si>
-  <si>
-    <t>126229684</t>
-  </si>
-  <si>
-    <t>32418775</t>
-  </si>
-  <si>
-    <t>3424012</t>
-  </si>
-  <si>
-    <t>126229673</t>
-  </si>
-  <si>
-    <t>32418883</t>
-  </si>
-  <si>
-    <t>3424120</t>
-  </si>
-  <si>
-    <t>126230785</t>
-  </si>
-  <si>
-    <t>32418882</t>
-  </si>
-  <si>
-    <t>3424119</t>
-  </si>
-  <si>
-    <t>126230774</t>
-  </si>
-  <si>
-    <t>32418881</t>
-  </si>
-  <si>
-    <t>3424118</t>
-  </si>
-  <si>
-    <t>126230763</t>
-  </si>
-  <si>
-    <t>32418685</t>
-  </si>
-  <si>
-    <t>3423922</t>
-  </si>
-  <si>
-    <t>126229008</t>
-  </si>
-  <si>
-    <t>32418684</t>
-  </si>
-  <si>
-    <t>3423921</t>
-  </si>
-  <si>
-    <t>126228997</t>
+    <t>126269622</t>
+  </si>
+  <si>
+    <t>126269644</t>
+  </si>
+  <si>
+    <t>126269666</t>
+  </si>
+  <si>
+    <t>126254257</t>
+  </si>
+  <si>
+    <t>126269367</t>
+  </si>
+  <si>
+    <t>32422988</t>
+  </si>
+  <si>
+    <t>126269725</t>
+  </si>
+  <si>
+    <t>32422987</t>
+  </si>
+  <si>
+    <t>3428223</t>
+  </si>
+  <si>
+    <t>126269714</t>
+  </si>
+  <si>
+    <t>32422986</t>
+  </si>
+  <si>
+    <t>3428222</t>
+  </si>
+  <si>
+    <t>126269703</t>
+  </si>
+  <si>
+    <t>32422985</t>
+  </si>
+  <si>
+    <t>3428221</t>
+  </si>
+  <si>
+    <t>126269699</t>
+  </si>
+  <si>
+    <t>32422984</t>
+  </si>
+  <si>
+    <t>3428220</t>
+  </si>
+  <si>
+    <t>126269688</t>
+  </si>
+  <si>
+    <t>32422983</t>
+  </si>
+  <si>
+    <t>3428219</t>
+  </si>
+  <si>
+    <t>126269677</t>
+  </si>
+  <si>
+    <t>32421179</t>
+  </si>
+  <si>
+    <t>3426416</t>
+  </si>
+  <si>
+    <t>126254291</t>
+  </si>
+  <si>
+    <t>32421178</t>
+  </si>
+  <si>
+    <t>3426415</t>
+  </si>
+  <si>
+    <t>126254280</t>
+  </si>
+  <si>
+    <t>32421177</t>
+  </si>
+  <si>
+    <t>3426414</t>
+  </si>
+  <si>
+    <t>126254279</t>
+  </si>
+  <si>
+    <t>32421176</t>
+  </si>
+  <si>
+    <t>3426413</t>
+  </si>
+  <si>
+    <t>126254268</t>
+  </si>
+  <si>
+    <t>32422961</t>
+  </si>
+  <si>
+    <t>3428197</t>
+  </si>
+  <si>
+    <t>126269390</t>
+  </si>
+  <si>
+    <t>32422982</t>
+  </si>
+  <si>
+    <t>3428218</t>
+  </si>
+  <si>
+    <t>126269655</t>
+  </si>
+  <si>
+    <t>32422960</t>
+  </si>
+  <si>
+    <t>3428196</t>
+  </si>
+  <si>
+    <t>126269389</t>
+  </si>
+  <si>
+    <t>32422959</t>
+  </si>
+  <si>
+    <t>3428195</t>
+  </si>
+  <si>
+    <t>126269378</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1324,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,11 +1334,11 @@
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
-        <v>126229617</v>
+      <c r="C2" t="s">
+        <v>82</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1339,65 +1348,65 @@
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5">
-        <v>126229639</v>
+      <c r="C3" t="s">
+        <v>83</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="5">
-        <v>126229651</v>
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5">
-        <v>126230741</v>
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="5">
-        <v>126228975</v>
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1436,31 +1445,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,10 +1547,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1767,10 +1776,10 @@
     </row>
     <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -1794,7 +1803,7 @@
         <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
         <v>46</v>
@@ -1825,7 +1834,7 @@
         <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
         <v>46</v>
@@ -1977,10 +1986,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
@@ -2092,7 +2101,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2104,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,27 +2139,29 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
       <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" t="s">
-        <v>96</v>
+        <v>87</v>
+      </c>
+      <c r="C2">
+        <v>3426393</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,49 +2169,49 @@
         <v>126229651</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,6 +2270,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2266,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2291,39 +2303,41 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2331,13 +2345,13 @@
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2439,15 +2453,17 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2465,13 +2481,13 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes of 1st June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
@@ -270,149 +270,149 @@
     <t>RT00002274</t>
   </si>
   <si>
-    <t>126269622</t>
-  </si>
-  <si>
-    <t>126269644</t>
-  </si>
-  <si>
-    <t>126269666</t>
-  </si>
-  <si>
-    <t>126254257</t>
-  </si>
-  <si>
-    <t>126269367</t>
-  </si>
-  <si>
-    <t>32422988</t>
-  </si>
-  <si>
-    <t>126269725</t>
-  </si>
-  <si>
-    <t>32422987</t>
-  </si>
-  <si>
-    <t>3428223</t>
-  </si>
-  <si>
-    <t>126269714</t>
-  </si>
-  <si>
-    <t>32422986</t>
-  </si>
-  <si>
-    <t>3428222</t>
-  </si>
-  <si>
-    <t>126269703</t>
-  </si>
-  <si>
-    <t>32422985</t>
-  </si>
-  <si>
-    <t>3428221</t>
-  </si>
-  <si>
-    <t>126269699</t>
-  </si>
-  <si>
-    <t>32422984</t>
-  </si>
-  <si>
-    <t>3428220</t>
-  </si>
-  <si>
-    <t>126269688</t>
-  </si>
-  <si>
-    <t>32422983</t>
-  </si>
-  <si>
-    <t>3428219</t>
-  </si>
-  <si>
-    <t>126269677</t>
-  </si>
-  <si>
-    <t>32421179</t>
-  </si>
-  <si>
-    <t>3426416</t>
-  </si>
-  <si>
-    <t>126254291</t>
-  </si>
-  <si>
-    <t>32421178</t>
-  </si>
-  <si>
-    <t>3426415</t>
-  </si>
-  <si>
-    <t>126254280</t>
-  </si>
-  <si>
-    <t>32421177</t>
-  </si>
-  <si>
-    <t>3426414</t>
-  </si>
-  <si>
-    <t>126254279</t>
-  </si>
-  <si>
-    <t>32421176</t>
-  </si>
-  <si>
-    <t>3426413</t>
-  </si>
-  <si>
-    <t>126254268</t>
-  </si>
-  <si>
-    <t>32422961</t>
-  </si>
-  <si>
-    <t>3428197</t>
-  </si>
-  <si>
-    <t>126269390</t>
-  </si>
-  <si>
-    <t>32422982</t>
-  </si>
-  <si>
-    <t>3428218</t>
-  </si>
-  <si>
-    <t>126269655</t>
-  </si>
-  <si>
-    <t>32422960</t>
-  </si>
-  <si>
-    <t>3428196</t>
-  </si>
-  <si>
-    <t>126269389</t>
-  </si>
-  <si>
-    <t>32422959</t>
-  </si>
-  <si>
-    <t>3428195</t>
-  </si>
-  <si>
-    <t>126269378</t>
+    <t>126270011</t>
+  </si>
+  <si>
+    <t>126289990</t>
+  </si>
+  <si>
+    <t>32423043</t>
+  </si>
+  <si>
+    <t>126270055</t>
+  </si>
+  <si>
+    <t>32423042</t>
+  </si>
+  <si>
+    <t>126270044</t>
+  </si>
+  <si>
+    <t>32423041</t>
+  </si>
+  <si>
+    <t>126270033</t>
+  </si>
+  <si>
+    <t>32423040</t>
+  </si>
+  <si>
+    <t>126270022</t>
+  </si>
+  <si>
+    <t>32424988</t>
+  </si>
+  <si>
+    <t>126290024</t>
+  </si>
+  <si>
+    <t>32424987</t>
+  </si>
+  <si>
+    <t>3430223</t>
+  </si>
+  <si>
+    <t>126290013</t>
+  </si>
+  <si>
+    <t>32424986</t>
+  </si>
+  <si>
+    <t>3430222</t>
+  </si>
+  <si>
+    <t>126290002</t>
+  </si>
+  <si>
+    <t>126291054</t>
+  </si>
+  <si>
+    <t>126291076</t>
+  </si>
+  <si>
+    <t>126291098</t>
+  </si>
+  <si>
+    <t>32425100</t>
+  </si>
+  <si>
+    <t>3430336</t>
+  </si>
+  <si>
+    <t>126291087</t>
+  </si>
+  <si>
+    <t>32425106</t>
+  </si>
+  <si>
+    <t>3430342</t>
+  </si>
+  <si>
+    <t>126291157</t>
+  </si>
+  <si>
+    <t>32425105</t>
+  </si>
+  <si>
+    <t>3430341</t>
+  </si>
+  <si>
+    <t>126291146</t>
+  </si>
+  <si>
+    <t>32425104</t>
+  </si>
+  <si>
+    <t>3430340</t>
+  </si>
+  <si>
+    <t>126291135</t>
+  </si>
+  <si>
+    <t>32425103</t>
+  </si>
+  <si>
+    <t>3430339</t>
+  </si>
+  <si>
+    <t>126291124</t>
+  </si>
+  <si>
+    <t>32425102</t>
+  </si>
+  <si>
+    <t>3430338</t>
+  </si>
+  <si>
+    <t>126291113</t>
+  </si>
+  <si>
+    <t>32425101</t>
+  </si>
+  <si>
+    <t>3430337</t>
+  </si>
+  <si>
+    <t>126291102</t>
+  </si>
+  <si>
+    <t>3428279</t>
+  </si>
+  <si>
+    <t>3428278</t>
+  </si>
+  <si>
+    <t>3428277</t>
+  </si>
+  <si>
+    <t>3428276</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,6 +556,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="27">
     <fill>
@@ -694,7 +700,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -824,6 +830,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -869,7 +888,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -889,6 +908,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1302,7 +1327,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,7 +1360,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>71</v>
@@ -1349,7 +1374,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>71</v>
@@ -1363,7 +1388,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>72</v>
@@ -1377,7 +1402,7 @@
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>73</v>
@@ -1391,7 +1416,7 @@
         <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>74</v>
@@ -1421,7 +1446,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,21 +1471,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>68</v>
@@ -1487,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,75 +1556,75 @@
       <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="3"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="2"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H3" s="2"/>
@@ -1607,7 +1632,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1622,7 +1647,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -1637,7 +1662,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -1652,7 +1677,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="M6" s="12"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -1667,7 +1692,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1682,7 +1707,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1697,7 +1722,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -1712,7 +1737,301 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1722,10 +2041,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,68 +2094,68 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1944,6 +2263,266 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1951,9 +2530,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1965,7 +2546,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1985,27 +2566,27 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -2013,7 +2594,7 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2021,7 +2602,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2029,7 +2610,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2037,7 +2618,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2045,7 +2626,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2053,7 +2634,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2061,7 +2642,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2069,12 +2650,164 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2113,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,28 +2873,28 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2">
-        <v>3426393</v>
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2169,49 +2902,49 @@
         <v>126229651</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2279,7 +3012,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,54 +3037,54 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="10">
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,6 +3155,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2429,8 +3163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,40 +3188,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="C2">
+        <v>3426383</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2498,6 +3232,9 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
Changes if 2nd Jun 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="8"/>
+    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
-    <sheet name="Rate" sheetId="3" r:id="rId3"/>
-    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
-    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
-    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
-    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
-    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
-    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
+    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
+    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
+    <sheet name="Rate" r:id="rId3" sheetId="3"/>
+    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
+    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
+    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
+    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
+    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
+    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="143">
   <si>
     <t>FileName</t>
   </si>
@@ -270,149 +270,195 @@
     <t>RT00002274</t>
   </si>
   <si>
-    <t>126270011</t>
-  </si>
-  <si>
-    <t>126289990</t>
-  </si>
-  <si>
-    <t>32423043</t>
-  </si>
-  <si>
-    <t>126270055</t>
-  </si>
-  <si>
-    <t>32423042</t>
-  </si>
-  <si>
-    <t>126270044</t>
-  </si>
-  <si>
-    <t>32423041</t>
-  </si>
-  <si>
-    <t>126270033</t>
-  </si>
-  <si>
-    <t>32423040</t>
-  </si>
-  <si>
-    <t>126270022</t>
-  </si>
-  <si>
-    <t>32424988</t>
-  </si>
-  <si>
-    <t>126290024</t>
-  </si>
-  <si>
-    <t>32424987</t>
-  </si>
-  <si>
-    <t>3430223</t>
-  </si>
-  <si>
-    <t>126290013</t>
-  </si>
-  <si>
-    <t>32424986</t>
-  </si>
-  <si>
-    <t>3430222</t>
-  </si>
-  <si>
-    <t>126290002</t>
-  </si>
-  <si>
-    <t>126291054</t>
-  </si>
-  <si>
-    <t>126291076</t>
-  </si>
-  <si>
-    <t>126291098</t>
-  </si>
-  <si>
-    <t>32425100</t>
-  </si>
-  <si>
-    <t>3430336</t>
-  </si>
-  <si>
-    <t>126291087</t>
-  </si>
-  <si>
-    <t>32425106</t>
-  </si>
-  <si>
-    <t>3430342</t>
-  </si>
-  <si>
-    <t>126291157</t>
-  </si>
-  <si>
-    <t>32425105</t>
-  </si>
-  <si>
-    <t>3430341</t>
-  </si>
-  <si>
-    <t>126291146</t>
-  </si>
-  <si>
-    <t>32425104</t>
-  </si>
-  <si>
-    <t>3430340</t>
-  </si>
-  <si>
-    <t>126291135</t>
-  </si>
-  <si>
-    <t>32425103</t>
-  </si>
-  <si>
-    <t>3430339</t>
-  </si>
-  <si>
-    <t>126291124</t>
-  </si>
-  <si>
-    <t>32425102</t>
-  </si>
-  <si>
-    <t>3430338</t>
-  </si>
-  <si>
-    <t>126291113</t>
-  </si>
-  <si>
-    <t>32425101</t>
-  </si>
-  <si>
-    <t>3430337</t>
-  </si>
-  <si>
-    <t>126291102</t>
-  </si>
-  <si>
-    <t>3428279</t>
-  </si>
-  <si>
-    <t>3428278</t>
-  </si>
-  <si>
-    <t>3428277</t>
-  </si>
-  <si>
-    <t>3428276</t>
+    <t>RTE Automation NegFlow</t>
+  </si>
+  <si>
+    <t>RT00002335</t>
+  </si>
+  <si>
+    <t>126308828</t>
+  </si>
+  <si>
+    <t>126308415</t>
+  </si>
+  <si>
+    <t>126308840</t>
+  </si>
+  <si>
+    <t>126308862</t>
+  </si>
+  <si>
+    <t>126310177</t>
+  </si>
+  <si>
+    <t>126308149</t>
+  </si>
+  <si>
+    <t>32426785</t>
+  </si>
+  <si>
+    <t>126308921</t>
+  </si>
+  <si>
+    <t>32426784</t>
+  </si>
+  <si>
+    <t>3432020</t>
+  </si>
+  <si>
+    <t>126308910</t>
+  </si>
+  <si>
+    <t>32426783</t>
+  </si>
+  <si>
+    <t>3432019</t>
+  </si>
+  <si>
+    <t>126308909</t>
+  </si>
+  <si>
+    <t>32426782</t>
+  </si>
+  <si>
+    <t>3432018</t>
+  </si>
+  <si>
+    <t>126308895</t>
+  </si>
+  <si>
+    <t>32426781</t>
+  </si>
+  <si>
+    <t>3432017</t>
+  </si>
+  <si>
+    <t>126308884</t>
+  </si>
+  <si>
+    <t>32426780</t>
+  </si>
+  <si>
+    <t>3432016</t>
+  </si>
+  <si>
+    <t>126308873</t>
+  </si>
+  <si>
+    <t>32426931</t>
+  </si>
+  <si>
+    <t>126310214</t>
+  </si>
+  <si>
+    <t>32426930</t>
+  </si>
+  <si>
+    <t>3432166</t>
+  </si>
+  <si>
+    <t>126310203</t>
+  </si>
+  <si>
+    <t>32426929</t>
+  </si>
+  <si>
+    <t>3432165</t>
+  </si>
+  <si>
+    <t>126310199</t>
+  </si>
+  <si>
+    <t>32426928</t>
+  </si>
+  <si>
+    <t>3432164</t>
+  </si>
+  <si>
+    <t>126310188</t>
+  </si>
+  <si>
+    <t>32426718</t>
+  </si>
+  <si>
+    <t>126308172</t>
+  </si>
+  <si>
+    <t>32426717</t>
+  </si>
+  <si>
+    <t>3431953</t>
+  </si>
+  <si>
+    <t>126308161</t>
+  </si>
+  <si>
+    <t>32426716</t>
+  </si>
+  <si>
+    <t>3431952</t>
+  </si>
+  <si>
+    <t>126308150</t>
+  </si>
+  <si>
+    <t>3432014</t>
+  </si>
+  <si>
+    <t>126308839</t>
+  </si>
+  <si>
+    <t>32426741</t>
+  </si>
+  <si>
+    <t>3432021</t>
+  </si>
+  <si>
+    <t>3432167</t>
+  </si>
+  <si>
+    <t>3431954</t>
+  </si>
+  <si>
+    <t>32426778</t>
+  </si>
+  <si>
+    <t>3431977</t>
+  </si>
+  <si>
+    <t>126308426</t>
+  </si>
+  <si>
+    <t>32426779</t>
+  </si>
+  <si>
+    <t>3432015</t>
+  </si>
+  <si>
+    <t>126308851</t>
+  </si>
+  <si>
+    <t>2022-06-02 00:00</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
+  </si>
+  <si>
+    <t>2022-06-02 12:44</t>
+  </si>
+  <si>
+    <t>3432499</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,8 +608,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,6 +749,18 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -845,122 +909,128 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="28" fontId="21" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1042,10 +1112,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1203,7 +1273,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1212,13 +1282,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1228,7 +1298,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1237,7 +1307,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1246,7 +1316,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1256,12 +1326,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1292,7 +1362,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1311,7 +1381,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1323,19 +1393,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,21 +1430,21 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
+      <c r="A3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>71</v>
@@ -1382,77 +1452,91 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="8" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="8" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1471,48 +1555,62 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>64</v>
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1520,15 +1618,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1556,55 +1654,55 @@
       <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
       <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
       <c r="M2" s="12"/>
@@ -2034,14 +2132,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -2049,16 +2147,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2093,69 +2191,69 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="E3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2524,13 +2622,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -2538,11 +2636,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2566,22 +2664,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2810,13 +2908,13 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
@@ -2824,7 +2922,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2834,27 +2932,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2873,28 +2971,28 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2902,49 +3000,49 @@
         <v>126229651</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3002,23 +3100,23 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3037,40 +3135,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3078,13 +3176,13 @@
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3154,22 +3252,22 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3188,40 +3286,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2">
-        <v>3426383</v>
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3297,6 +3395,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changesof 3rd June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="153">
   <si>
     <t>FileName</t>
   </si>
@@ -195,12 +195,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>14101 Seeley Ave.</t>
-  </si>
-  <si>
-    <t>14101 Seeley Ave., 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
-  </si>
-  <si>
     <t>Scheduler</t>
   </si>
   <si>
@@ -210,27 +204,6 @@
     <t>US$520.00</t>
   </si>
   <si>
-    <t>126175301</t>
-  </si>
-  <si>
-    <t>3418391</t>
-  </si>
-  <si>
-    <t>126175312</t>
-  </si>
-  <si>
-    <t>2022-05-24 00:30</t>
-  </si>
-  <si>
-    <t>2022-05-24 13:14</t>
-  </si>
-  <si>
-    <t>3418490</t>
-  </si>
-  <si>
-    <t>32413153</t>
-  </si>
-  <si>
     <t>RTE Job Creation Manual</t>
   </si>
   <si>
@@ -276,75 +249,15 @@
     <t>RT00002335</t>
   </si>
   <si>
-    <t>126308828</t>
-  </si>
-  <si>
     <t>126308415</t>
   </si>
   <si>
-    <t>126308840</t>
-  </si>
-  <si>
     <t>126308862</t>
   </si>
   <si>
     <t>126310177</t>
   </si>
   <si>
-    <t>126308149</t>
-  </si>
-  <si>
-    <t>32426785</t>
-  </si>
-  <si>
-    <t>126308921</t>
-  </si>
-  <si>
-    <t>32426784</t>
-  </si>
-  <si>
-    <t>3432020</t>
-  </si>
-  <si>
-    <t>126308910</t>
-  </si>
-  <si>
-    <t>32426783</t>
-  </si>
-  <si>
-    <t>3432019</t>
-  </si>
-  <si>
-    <t>126308909</t>
-  </si>
-  <si>
-    <t>32426782</t>
-  </si>
-  <si>
-    <t>3432018</t>
-  </si>
-  <si>
-    <t>126308895</t>
-  </si>
-  <si>
-    <t>32426781</t>
-  </si>
-  <si>
-    <t>3432017</t>
-  </si>
-  <si>
-    <t>126308884</t>
-  </si>
-  <si>
-    <t>32426780</t>
-  </si>
-  <si>
-    <t>3432016</t>
-  </si>
-  <si>
-    <t>126308873</t>
-  </si>
-  <si>
     <t>32426931</t>
   </si>
   <si>
@@ -378,66 +291,15 @@
     <t>126310188</t>
   </si>
   <si>
-    <t>32426718</t>
-  </si>
-  <si>
-    <t>126308172</t>
-  </si>
-  <si>
-    <t>32426717</t>
-  </si>
-  <si>
-    <t>3431953</t>
-  </si>
-  <si>
-    <t>126308161</t>
-  </si>
-  <si>
-    <t>32426716</t>
-  </si>
-  <si>
-    <t>3431952</t>
-  </si>
-  <si>
-    <t>126308150</t>
-  </si>
-  <si>
-    <t>3432014</t>
-  </si>
-  <si>
-    <t>126308839</t>
-  </si>
-  <si>
-    <t>32426741</t>
-  </si>
-  <si>
-    <t>3432021</t>
-  </si>
-  <si>
     <t>3432167</t>
   </si>
   <si>
-    <t>3431954</t>
-  </si>
-  <si>
-    <t>32426778</t>
-  </si>
-  <si>
     <t>3431977</t>
   </si>
   <si>
     <t>126308426</t>
   </si>
   <si>
-    <t>32426779</t>
-  </si>
-  <si>
-    <t>3432015</t>
-  </si>
-  <si>
-    <t>126308851</t>
-  </si>
-  <si>
     <t>2022-06-02 00:00</t>
   </si>
   <si>
@@ -451,6 +313,174 @@
   </si>
   <si>
     <t>3432499</t>
+  </si>
+  <si>
+    <t>126326125</t>
+  </si>
+  <si>
+    <t>126326000</t>
+  </si>
+  <si>
+    <t>126326147</t>
+  </si>
+  <si>
+    <t>126326169</t>
+  </si>
+  <si>
+    <t>126325829</t>
+  </si>
+  <si>
+    <t>32428562</t>
+  </si>
+  <si>
+    <t>3433798</t>
+  </si>
+  <si>
+    <t>126326136</t>
+  </si>
+  <si>
+    <t>32428540</t>
+  </si>
+  <si>
+    <t>3433776</t>
+  </si>
+  <si>
+    <t>126326011</t>
+  </si>
+  <si>
+    <t>32428563</t>
+  </si>
+  <si>
+    <t>126326158</t>
+  </si>
+  <si>
+    <t>32428569</t>
+  </si>
+  <si>
+    <t>3433805</t>
+  </si>
+  <si>
+    <t>126326228</t>
+  </si>
+  <si>
+    <t>32428568</t>
+  </si>
+  <si>
+    <t>3433804</t>
+  </si>
+  <si>
+    <t>126326217</t>
+  </si>
+  <si>
+    <t>32428567</t>
+  </si>
+  <si>
+    <t>3433803</t>
+  </si>
+  <si>
+    <t>126326206</t>
+  </si>
+  <si>
+    <t>32428566</t>
+  </si>
+  <si>
+    <t>3433802</t>
+  </si>
+  <si>
+    <t>126326192</t>
+  </si>
+  <si>
+    <t>32428565</t>
+  </si>
+  <si>
+    <t>3433801</t>
+  </si>
+  <si>
+    <t>126326181</t>
+  </si>
+  <si>
+    <t>32428564</t>
+  </si>
+  <si>
+    <t>3433800</t>
+  </si>
+  <si>
+    <t>126326170</t>
+  </si>
+  <si>
+    <t>32428511</t>
+  </si>
+  <si>
+    <t>3433747</t>
+  </si>
+  <si>
+    <t>126325852</t>
+  </si>
+  <si>
+    <t>32428510</t>
+  </si>
+  <si>
+    <t>3433746</t>
+  </si>
+  <si>
+    <t>126325841</t>
+  </si>
+  <si>
+    <t>32428509</t>
+  </si>
+  <si>
+    <t>3433745</t>
+  </si>
+  <si>
+    <t>126325830</t>
+  </si>
+  <si>
+    <t>$150.00</t>
+  </si>
+  <si>
+    <t>Fix Route Base Rate is applied</t>
+  </si>
+  <si>
+    <t>Total :US$150.00</t>
+  </si>
+  <si>
+    <t>US$150.00</t>
+  </si>
+  <si>
+    <t>NYU OTHO HOSPTIAL</t>
+  </si>
+  <si>
+    <t>NYU OTHO HOSPTIAL, 301 E 17TH STREET, MANHATTAN, NY, 10003, USA</t>
+  </si>
+  <si>
+    <t>2022-06-03 00:30</t>
+  </si>
+  <si>
+    <t>EDT</t>
+  </si>
+  <si>
+    <t>STORAGE AMERICA</t>
+  </si>
+  <si>
+    <t>STORAGE AMERICA, 211 DENTON AVE, NEW HYDE PARK, NY, 11040, USA</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>2022-06-03 01:14</t>
+  </si>
+  <si>
+    <t>126325818</t>
+  </si>
+  <si>
+    <t>3433744</t>
+  </si>
+  <si>
+    <t>3434190</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,24 +1460,24 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,64 +1488,66 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
       <c r="D8" s="8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1530,12 +1562,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
@@ -1555,48 +1588,50 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" t="s">
-        <v>136</v>
+        <v>108</v>
+      </c>
+      <c r="C4">
+        <v>3433744</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1670,37 +1705,37 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
       <c r="L2" t="s">
         <v>26</v>
@@ -2193,10 +2228,10 @@
     </row>
     <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -2205,10 +2240,10 @@
         <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="G2" t="s">
         <v>45</v>
@@ -2220,10 +2255,10 @@
         <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>144</v>
       </c>
     </row>
     <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2236,25 +2271,25 @@
         <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="G3" t="s">
         <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="J3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2665,10 +2700,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
@@ -2932,7 +2967,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2971,28 +3006,28 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3000,49 +3035,49 @@
         <v>126229651</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3135,40 +3170,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3176,13 +3211,13 @@
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3286,40 +3321,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes of 7th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="137">
   <si>
     <t>FileName</t>
   </si>
@@ -249,238 +249,190 @@
     <t>RT00002335</t>
   </si>
   <si>
-    <t>126308415</t>
-  </si>
-  <si>
     <t>126308862</t>
   </si>
   <si>
-    <t>126310177</t>
-  </si>
-  <si>
-    <t>32426931</t>
-  </si>
-  <si>
-    <t>126310214</t>
-  </si>
-  <si>
-    <t>32426930</t>
-  </si>
-  <si>
-    <t>3432166</t>
-  </si>
-  <si>
-    <t>126310203</t>
-  </si>
-  <si>
-    <t>32426929</t>
-  </si>
-  <si>
-    <t>3432165</t>
-  </si>
-  <si>
-    <t>126310199</t>
-  </si>
-  <si>
-    <t>32426928</t>
-  </si>
-  <si>
-    <t>3432164</t>
-  </si>
-  <si>
-    <t>126310188</t>
-  </si>
-  <si>
-    <t>3432167</t>
-  </si>
-  <si>
-    <t>3431977</t>
-  </si>
-  <si>
-    <t>126308426</t>
-  </si>
-  <si>
-    <t>2022-06-02 00:00</t>
-  </si>
-  <si>
     <t>ST FRANCIS MEDICAL CENTER</t>
   </si>
   <si>
     <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
   </si>
   <si>
-    <t>2022-06-02 12:44</t>
-  </si>
-  <si>
-    <t>3432499</t>
-  </si>
-  <si>
-    <t>126326125</t>
-  </si>
-  <si>
-    <t>126326000</t>
-  </si>
-  <si>
-    <t>126326147</t>
-  </si>
-  <si>
-    <t>126326169</t>
-  </si>
-  <si>
-    <t>126325829</t>
-  </si>
-  <si>
-    <t>32428562</t>
-  </si>
-  <si>
-    <t>3433798</t>
-  </si>
-  <si>
-    <t>126326136</t>
-  </si>
-  <si>
-    <t>32428540</t>
-  </si>
-  <si>
-    <t>3433776</t>
-  </si>
-  <si>
-    <t>126326011</t>
-  </si>
-  <si>
-    <t>32428563</t>
-  </si>
-  <si>
-    <t>126326158</t>
-  </si>
-  <si>
-    <t>32428569</t>
-  </si>
-  <si>
-    <t>3433805</t>
-  </si>
-  <si>
-    <t>126326228</t>
-  </si>
-  <si>
-    <t>32428568</t>
-  </si>
-  <si>
-    <t>3433804</t>
-  </si>
-  <si>
-    <t>126326217</t>
-  </si>
-  <si>
-    <t>32428567</t>
-  </si>
-  <si>
-    <t>3433803</t>
-  </si>
-  <si>
-    <t>126326206</t>
-  </si>
-  <si>
-    <t>32428566</t>
-  </si>
-  <si>
-    <t>3433802</t>
-  </si>
-  <si>
-    <t>126326192</t>
-  </si>
-  <si>
-    <t>32428565</t>
-  </si>
-  <si>
-    <t>3433801</t>
-  </si>
-  <si>
-    <t>126326181</t>
-  </si>
-  <si>
-    <t>32428564</t>
-  </si>
-  <si>
-    <t>3433800</t>
-  </si>
-  <si>
-    <t>126326170</t>
-  </si>
-  <si>
-    <t>32428511</t>
-  </si>
-  <si>
-    <t>3433747</t>
-  </si>
-  <si>
-    <t>126325852</t>
-  </si>
-  <si>
-    <t>32428510</t>
-  </si>
-  <si>
-    <t>3433746</t>
-  </si>
-  <si>
-    <t>126325841</t>
-  </si>
-  <si>
-    <t>32428509</t>
-  </si>
-  <si>
-    <t>3433745</t>
-  </si>
-  <si>
-    <t>126325830</t>
-  </si>
-  <si>
-    <t>$150.00</t>
-  </si>
-  <si>
-    <t>Fix Route Base Rate is applied</t>
-  </si>
-  <si>
-    <t>Total :US$150.00</t>
-  </si>
-  <si>
-    <t>US$150.00</t>
-  </si>
-  <si>
-    <t>NYU OTHO HOSPTIAL</t>
-  </si>
-  <si>
-    <t>NYU OTHO HOSPTIAL, 301 E 17TH STREET, MANHATTAN, NY, 10003, USA</t>
-  </si>
-  <si>
-    <t>2022-06-03 00:30</t>
-  </si>
-  <si>
-    <t>EDT</t>
-  </si>
-  <si>
-    <t>STORAGE AMERICA</t>
-  </si>
-  <si>
-    <t>STORAGE AMERICA, 211 DENTON AVE, NEW HYDE PARK, NY, 11040, USA</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>2022-06-03 01:14</t>
-  </si>
-  <si>
-    <t>126325818</t>
-  </si>
-  <si>
-    <t>3433744</t>
-  </si>
-  <si>
-    <t>3434190</t>
+    <t>126361641</t>
+  </si>
+  <si>
+    <t>32432106</t>
+  </si>
+  <si>
+    <t>3437342</t>
+  </si>
+  <si>
+    <t>126361685</t>
+  </si>
+  <si>
+    <t>32432105</t>
+  </si>
+  <si>
+    <t>3437341</t>
+  </si>
+  <si>
+    <t>126361674</t>
+  </si>
+  <si>
+    <t>32432104</t>
+  </si>
+  <si>
+    <t>3437340</t>
+  </si>
+  <si>
+    <t>126361663</t>
+  </si>
+  <si>
+    <t>32432103</t>
+  </si>
+  <si>
+    <t>3437339</t>
+  </si>
+  <si>
+    <t>126361652</t>
+  </si>
+  <si>
+    <t>126383348</t>
+  </si>
+  <si>
+    <t>126382916</t>
+  </si>
+  <si>
+    <t>126383360</t>
+  </si>
+  <si>
+    <t>126383382</t>
+  </si>
+  <si>
+    <t>126382639</t>
+  </si>
+  <si>
+    <t>32434323</t>
+  </si>
+  <si>
+    <t>3439559</t>
+  </si>
+  <si>
+    <t>126383359</t>
+  </si>
+  <si>
+    <t>32434269</t>
+  </si>
+  <si>
+    <t>3439505</t>
+  </si>
+  <si>
+    <t>126382927</t>
+  </si>
+  <si>
+    <t>32434324</t>
+  </si>
+  <si>
+    <t>3439560</t>
+  </si>
+  <si>
+    <t>126383371</t>
+  </si>
+  <si>
+    <t>32434330</t>
+  </si>
+  <si>
+    <t>3439566</t>
+  </si>
+  <si>
+    <t>126383441</t>
+  </si>
+  <si>
+    <t>32434329</t>
+  </si>
+  <si>
+    <t>3439565</t>
+  </si>
+  <si>
+    <t>126383430</t>
+  </si>
+  <si>
+    <t>32434328</t>
+  </si>
+  <si>
+    <t>3439564</t>
+  </si>
+  <si>
+    <t>126383429</t>
+  </si>
+  <si>
+    <t>32434327</t>
+  </si>
+  <si>
+    <t>3439563</t>
+  </si>
+  <si>
+    <t>126383418</t>
+  </si>
+  <si>
+    <t>32434326</t>
+  </si>
+  <si>
+    <t>3439562</t>
+  </si>
+  <si>
+    <t>126383407</t>
+  </si>
+  <si>
+    <t>32434325</t>
+  </si>
+  <si>
+    <t>3439561</t>
+  </si>
+  <si>
+    <t>126383393</t>
+  </si>
+  <si>
+    <t>32434237</t>
+  </si>
+  <si>
+    <t>3439473</t>
+  </si>
+  <si>
+    <t>126382662</t>
+  </si>
+  <si>
+    <t>32434236</t>
+  </si>
+  <si>
+    <t>3439472</t>
+  </si>
+  <si>
+    <t>126382651</t>
+  </si>
+  <si>
+    <t>32434235</t>
+  </si>
+  <si>
+    <t>3439471</t>
+  </si>
+  <si>
+    <t>126382640</t>
+  </si>
+  <si>
+    <t>2022-06-07 00:30</t>
+  </si>
+  <si>
+    <t>2022-06-07 13:14</t>
+  </si>
+  <si>
+    <t>3439729</t>
+  </si>
+  <si>
+    <t>Automation Merge RTE with LOC Job</t>
+  </si>
+  <si>
+    <t>RT00002367.</t>
   </si>
 </sst>
 </file>
@@ -1424,15 +1376,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
@@ -1459,8 +1411,8 @@
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>97</v>
+      <c r="C2" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>62</v>
@@ -1473,8 +1425,8 @@
       <c r="B3" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C3" t="s">
-        <v>98</v>
+      <c r="C3" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>62</v>
@@ -1487,8 +1439,8 @@
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>99</v>
+      <c r="C4" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>62</v>
@@ -1501,8 +1453,8 @@
       <c r="B5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C5" t="s">
-        <v>100</v>
+      <c r="C5" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>63</v>
@@ -1515,8 +1467,8 @@
       <c r="B6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C6" t="s">
-        <v>77</v>
+      <c r="C6" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>64</v>
@@ -1529,8 +1481,8 @@
       <c r="B7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C7" t="s">
-        <v>101</v>
+      <c r="C7" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>65</v>
@@ -1543,10 +1495,22 @@
       <c r="B8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C8" t="s">
-        <v>76</v>
+      <c r="C8" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1561,15 +1525,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,49 +1551,49 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
         <v>97</v>
       </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4">
-        <v>3433744</v>
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1705,37 +1668,37 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>139</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>140</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>140</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
         <v>26</v>
@@ -2228,10 +2191,10 @@
     </row>
     <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -2240,10 +2203,10 @@
         <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>142</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
         <v>45</v>
@@ -2255,10 +2218,10 @@
         <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="K2" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
     </row>
     <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2271,25 +2234,25 @@
         <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
         <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>147</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="K3" t="s">
-        <v>144</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2700,10 +2663,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>51</v>
@@ -2967,7 +2930,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3006,28 +2969,28 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,49 +2998,49 @@
         <v>126229651</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3170,40 +3133,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3211,13 +3174,13 @@
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,40 +3284,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changes of 8th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="177">
   <si>
     <t>FileName</t>
   </si>
@@ -258,181 +258,301 @@
     <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
   </si>
   <si>
-    <t>126361641</t>
-  </si>
-  <si>
-    <t>32432106</t>
-  </si>
-  <si>
-    <t>3437342</t>
-  </si>
-  <si>
-    <t>126361685</t>
-  </si>
-  <si>
-    <t>32432105</t>
-  </si>
-  <si>
-    <t>3437341</t>
-  </si>
-  <si>
-    <t>126361674</t>
-  </si>
-  <si>
-    <t>32432104</t>
-  </si>
-  <si>
-    <t>3437340</t>
-  </si>
-  <si>
-    <t>126361663</t>
-  </si>
-  <si>
-    <t>32432103</t>
-  </si>
-  <si>
-    <t>3437339</t>
-  </si>
-  <si>
-    <t>126361652</t>
-  </si>
-  <si>
-    <t>126383348</t>
-  </si>
-  <si>
     <t>126382916</t>
   </si>
   <si>
-    <t>126383360</t>
-  </si>
-  <si>
-    <t>126383382</t>
-  </si>
-  <si>
-    <t>126382639</t>
-  </si>
-  <si>
-    <t>32434323</t>
-  </si>
-  <si>
-    <t>3439559</t>
-  </si>
-  <si>
-    <t>126383359</t>
-  </si>
-  <si>
-    <t>32434269</t>
-  </si>
-  <si>
     <t>3439505</t>
   </si>
   <si>
-    <t>126382927</t>
-  </si>
-  <si>
-    <t>32434324</t>
-  </si>
-  <si>
     <t>3439560</t>
   </si>
   <si>
     <t>126383371</t>
   </si>
   <si>
-    <t>32434330</t>
-  </si>
-  <si>
-    <t>3439566</t>
-  </si>
-  <si>
-    <t>126383441</t>
-  </si>
-  <si>
-    <t>32434329</t>
-  </si>
-  <si>
-    <t>3439565</t>
-  </si>
-  <si>
-    <t>126383430</t>
-  </si>
-  <si>
-    <t>32434328</t>
-  </si>
-  <si>
-    <t>3439564</t>
-  </si>
-  <si>
-    <t>126383429</t>
-  </si>
-  <si>
-    <t>32434327</t>
-  </si>
-  <si>
-    <t>3439563</t>
-  </si>
-  <si>
-    <t>126383418</t>
-  </si>
-  <si>
-    <t>32434326</t>
-  </si>
-  <si>
-    <t>3439562</t>
-  </si>
-  <si>
-    <t>126383407</t>
-  </si>
-  <si>
-    <t>32434325</t>
-  </si>
-  <si>
-    <t>3439561</t>
-  </si>
-  <si>
-    <t>126383393</t>
-  </si>
-  <si>
-    <t>32434237</t>
-  </si>
-  <si>
-    <t>3439473</t>
-  </si>
-  <si>
-    <t>126382662</t>
-  </si>
-  <si>
-    <t>32434236</t>
-  </si>
-  <si>
-    <t>3439472</t>
-  </si>
-  <si>
-    <t>126382651</t>
-  </si>
-  <si>
-    <t>32434235</t>
-  </si>
-  <si>
-    <t>3439471</t>
-  </si>
-  <si>
-    <t>126382640</t>
-  </si>
-  <si>
     <t>2022-06-07 00:30</t>
   </si>
   <si>
     <t>2022-06-07 13:14</t>
   </si>
   <si>
-    <t>3439729</t>
-  </si>
-  <si>
     <t>Automation Merge RTE with LOC Job</t>
   </si>
   <si>
     <t>RT00002367.</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>RT00001993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation RW </t>
+  </si>
+  <si>
+    <t>126404063</t>
+  </si>
+  <si>
+    <t>126403653</t>
+  </si>
+  <si>
+    <t>126404085</t>
+  </si>
+  <si>
+    <t>126404100</t>
+  </si>
+  <si>
+    <t>126384873</t>
+  </si>
+  <si>
+    <t>126403594</t>
+  </si>
+  <si>
+    <t>32436425</t>
+  </si>
+  <si>
+    <t>3441661</t>
+  </si>
+  <si>
+    <t>126404074</t>
+  </si>
+  <si>
+    <t>32436366</t>
+  </si>
+  <si>
+    <t>3441602</t>
+  </si>
+  <si>
+    <t>126403664</t>
+  </si>
+  <si>
+    <t>32436426</t>
+  </si>
+  <si>
+    <t>3441662</t>
+  </si>
+  <si>
+    <t>126404096</t>
+  </si>
+  <si>
+    <t>32436432</t>
+  </si>
+  <si>
+    <t>3441668</t>
+  </si>
+  <si>
+    <t>126404166</t>
+  </si>
+  <si>
+    <t>32436431</t>
+  </si>
+  <si>
+    <t>3441667</t>
+  </si>
+  <si>
+    <t>126404155</t>
+  </si>
+  <si>
+    <t>32436430</t>
+  </si>
+  <si>
+    <t>3441666</t>
+  </si>
+  <si>
+    <t>126404144</t>
+  </si>
+  <si>
+    <t>32436429</t>
+  </si>
+  <si>
+    <t>3441665</t>
+  </si>
+  <si>
+    <t>126404133</t>
+  </si>
+  <si>
+    <t>32436428</t>
+  </si>
+  <si>
+    <t>3441664</t>
+  </si>
+  <si>
+    <t>126404122</t>
+  </si>
+  <si>
+    <t>32436427</t>
+  </si>
+  <si>
+    <t>3441663</t>
+  </si>
+  <si>
+    <t>126404111</t>
+  </si>
+  <si>
+    <t>32434478</t>
+  </si>
+  <si>
+    <t>3439714</t>
+  </si>
+  <si>
+    <t>126384910</t>
+  </si>
+  <si>
+    <t>32434477</t>
+  </si>
+  <si>
+    <t>3439713</t>
+  </si>
+  <si>
+    <t>126384909</t>
+  </si>
+  <si>
+    <t>32434476</t>
+  </si>
+  <si>
+    <t>3439712</t>
+  </si>
+  <si>
+    <t>126384895</t>
+  </si>
+  <si>
+    <t>32434475</t>
+  </si>
+  <si>
+    <t>3439711</t>
+  </si>
+  <si>
+    <t>126384884</t>
+  </si>
+  <si>
+    <t>32436361</t>
+  </si>
+  <si>
+    <t>3441597</t>
+  </si>
+  <si>
+    <t>126403620</t>
+  </si>
+  <si>
+    <t>32436360</t>
+  </si>
+  <si>
+    <t>3441596</t>
+  </si>
+  <si>
+    <t>126403619</t>
+  </si>
+  <si>
+    <t>32436359</t>
+  </si>
+  <si>
+    <t>3441595</t>
+  </si>
+  <si>
+    <t>126403608</t>
+  </si>
+  <si>
+    <t>126405059</t>
+  </si>
+  <si>
+    <t>126403572</t>
+  </si>
+  <si>
+    <t>32436530</t>
+  </si>
+  <si>
+    <t>3441766</t>
+  </si>
+  <si>
+    <t>126405093</t>
+  </si>
+  <si>
+    <t>32436529</t>
+  </si>
+  <si>
+    <t>3441765</t>
+  </si>
+  <si>
+    <t>126405082</t>
+  </si>
+  <si>
+    <t>32436528</t>
+  </si>
+  <si>
+    <t>3441764</t>
+  </si>
+  <si>
+    <t>126405071</t>
+  </si>
+  <si>
+    <t>32436527</t>
+  </si>
+  <si>
+    <t>3441763</t>
+  </si>
+  <si>
+    <t>126405060</t>
+  </si>
+  <si>
+    <t>32436358</t>
+  </si>
+  <si>
+    <t>3441594</t>
+  </si>
+  <si>
+    <t>126403583</t>
+  </si>
+  <si>
+    <t>2022-06-08 00:30</t>
+  </si>
+  <si>
+    <t>2022-06-08 13:14</t>
+  </si>
+  <si>
+    <t>3441866</t>
+  </si>
+  <si>
+    <t>3441881</t>
+  </si>
+  <si>
+    <t>$960.00</t>
+  </si>
+  <si>
+    <t>1395 Minute(s)</t>
+  </si>
+  <si>
+    <t>Total :US$985.00</t>
+  </si>
+  <si>
+    <t>US$985.00</t>
+  </si>
+  <si>
+    <t>Delivery instruction for Automation Testing</t>
+  </si>
+  <si>
+    <t>2022-06-09 22:03</t>
+  </si>
+  <si>
+    <t>RT00002368.</t>
+  </si>
+  <si>
+    <t>32436645</t>
+  </si>
+  <si>
+    <t>126406344</t>
+  </si>
+  <si>
+    <t>3442001</t>
+  </si>
+  <si>
+    <t>3442009</t>
+  </si>
+  <si>
+    <t>RT00002369.</t>
   </si>
 </sst>
 </file>
@@ -934,7 +1054,7 @@
     <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -965,6 +1085,9 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="28" fontId="21" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1376,10 +1499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,8 +1534,8 @@
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>91</v>
+      <c r="C2" t="s">
+        <v>90</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>62</v>
@@ -1425,8 +1548,8 @@
       <c r="B3" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>92</v>
+      <c r="C3" t="s">
+        <v>91</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>62</v>
@@ -1439,8 +1562,8 @@
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>93</v>
+      <c r="C4" t="s">
+        <v>92</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>62</v>
@@ -1453,8 +1576,8 @@
       <c r="B5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>94</v>
+      <c r="C5" t="s">
+        <v>93</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>63</v>
@@ -1467,8 +1590,8 @@
       <c r="B6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>78</v>
+      <c r="C6" t="s">
+        <v>144</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>64</v>
@@ -1481,7 +1604,7 @@
       <c r="B7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>95</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -1504,13 +1627,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1523,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,22 +1673,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>96</v>
@@ -1565,7 +1702,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
         <v>99</v>
@@ -1579,7 +1716,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>102</v>
@@ -1592,12 +1729,26 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1668,7 +1819,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>100</v>
@@ -1677,28 +1828,28 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>166</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="L2" t="s">
         <v>26</v>
@@ -1708,19 +1859,19 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>56</v>
       </c>
       <c r="H3" s="2"/>
@@ -2191,7 +2342,7 @@
     </row>
     <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>100</v>
@@ -2200,16 +2351,16 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="H2" t="s">
         <v>45</v>
@@ -2218,7 +2369,7 @@
         <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="K2" t="s">
         <v>46</v>
@@ -2249,7 +2400,7 @@
         <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="K3" t="s">
         <v>46</v>
@@ -2672,10 +2823,10 @@
         <v>51</v>
       </c>
       <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
         <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -2912,25 +3063,40 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>174</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2969,7 +3135,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
@@ -3133,40 +3299,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3174,13 +3340,13 @@
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,37 +3453,37 @@
         <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes of 9th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="152">
   <si>
     <t>FileName</t>
   </si>
@@ -78,15 +78,6 @@
     <t>BR - Base Rate</t>
   </si>
   <si>
-    <t>$520.00</t>
-  </si>
-  <si>
-    <t>764 Minute(s)</t>
-  </si>
-  <si>
-    <t>228927</t>
-  </si>
-  <si>
     <t>Total Revenue :</t>
   </si>
   <si>
@@ -150,409 +141,343 @@
     <t>1</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>ADV - ADVANCE FEES</t>
+  </si>
+  <si>
+    <t>$25.00</t>
+  </si>
+  <si>
+    <t>ADVANCE FEES</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>RTE Job Creation Manual</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>One To One</t>
+  </si>
+  <si>
+    <t>One To Many</t>
+  </si>
+  <si>
+    <t>Many to One</t>
+  </si>
+  <si>
+    <t>Many To Many</t>
+  </si>
+  <si>
+    <t>RTE Job Creation OneToMany</t>
+  </si>
+  <si>
+    <t>RTE Job Creation ManyToOne</t>
+  </si>
+  <si>
+    <t>RTE Job Creation ManyToMany</t>
+  </si>
+  <si>
+    <t>RT00002275</t>
+  </si>
+  <si>
+    <t>RT00002276</t>
+  </si>
+  <si>
+    <t>RT00002277</t>
+  </si>
+  <si>
+    <t>RT00002274</t>
+  </si>
+  <si>
+    <t>RTE Automation NegFlow</t>
+  </si>
+  <si>
+    <t>RT00002335</t>
+  </si>
+  <si>
+    <t>126308862</t>
+  </si>
+  <si>
+    <t>Automation Merge RTE with LOC Job</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>RT00001993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation RW </t>
+  </si>
+  <si>
+    <t>126405059</t>
+  </si>
+  <si>
+    <t>32436530</t>
+  </si>
+  <si>
+    <t>3441766</t>
+  </si>
+  <si>
+    <t>126405093</t>
+  </si>
+  <si>
+    <t>32436529</t>
+  </si>
+  <si>
+    <t>3441765</t>
+  </si>
+  <si>
+    <t>126405082</t>
+  </si>
+  <si>
+    <t>32436528</t>
+  </si>
+  <si>
+    <t>3441764</t>
+  </si>
+  <si>
+    <t>126405071</t>
+  </si>
+  <si>
+    <t>32436527</t>
+  </si>
+  <si>
+    <t>3441763</t>
+  </si>
+  <si>
+    <t>126405060</t>
+  </si>
+  <si>
+    <t>RT00002369.</t>
+  </si>
+  <si>
+    <t>126423194</t>
+  </si>
+  <si>
+    <t>126422636</t>
+  </si>
+  <si>
+    <t>126423219</t>
+  </si>
+  <si>
+    <t>126423231</t>
+  </si>
+  <si>
+    <t>126422142</t>
+  </si>
+  <si>
+    <t>126422120</t>
+  </si>
+  <si>
+    <t>32438401</t>
+  </si>
+  <si>
+    <t>3443637</t>
+  </si>
+  <si>
+    <t>126423208</t>
+  </si>
+  <si>
+    <t>32438324</t>
+  </si>
+  <si>
+    <t>3443560</t>
+  </si>
+  <si>
+    <t>126422647</t>
+  </si>
+  <si>
+    <t>32438402</t>
+  </si>
+  <si>
+    <t>126423220</t>
+  </si>
+  <si>
+    <t>32438408</t>
+  </si>
+  <si>
+    <t>3443644</t>
+  </si>
+  <si>
+    <t>126423297</t>
+  </si>
+  <si>
+    <t>32438407</t>
+  </si>
+  <si>
+    <t>3443643</t>
+  </si>
+  <si>
+    <t>126423286</t>
+  </si>
+  <si>
+    <t>32438406</t>
+  </si>
+  <si>
+    <t>3443642</t>
+  </si>
+  <si>
+    <t>126423275</t>
+  </si>
+  <si>
+    <t>32438405</t>
+  </si>
+  <si>
+    <t>3443641</t>
+  </si>
+  <si>
+    <t>126423264</t>
+  </si>
+  <si>
+    <t>32438404</t>
+  </si>
+  <si>
+    <t>3443640</t>
+  </si>
+  <si>
+    <t>126423253</t>
+  </si>
+  <si>
+    <t>32438403</t>
+  </si>
+  <si>
+    <t>3443639</t>
+  </si>
+  <si>
+    <t>126423242</t>
+  </si>
+  <si>
+    <t>32438280</t>
+  </si>
+  <si>
+    <t>3443516</t>
+  </si>
+  <si>
+    <t>126422175</t>
+  </si>
+  <si>
+    <t>32438279</t>
+  </si>
+  <si>
+    <t>3443515</t>
+  </si>
+  <si>
+    <t>126422164</t>
+  </si>
+  <si>
+    <t>32438278</t>
+  </si>
+  <si>
+    <t>3443514</t>
+  </si>
+  <si>
+    <t>126422153</t>
+  </si>
+  <si>
+    <t>32438277</t>
+  </si>
+  <si>
+    <t>3443513</t>
+  </si>
+  <si>
+    <t>126422131</t>
+  </si>
+  <si>
+    <t>Scheduler</t>
+  </si>
+  <si>
+    <t>0/2</t>
+  </si>
+  <si>
+    <t>Delivery instruction for Automation Testing</t>
+  </si>
+  <si>
+    <t>$150.00</t>
+  </si>
+  <si>
+    <t>Fix Route Base Rate is applied</t>
+  </si>
+  <si>
+    <t>Total :US$150.00</t>
+  </si>
+  <si>
+    <t>US$150.00</t>
+  </si>
+  <si>
+    <t>EDT</t>
+  </si>
+  <si>
+    <t>STORAGE AMERICA</t>
+  </si>
+  <si>
+    <t>STORAGE AMERICA, 211 DENTON AVE, NEW HYDE PARK, NY, 11040, USA</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>2022-06-02 01:14</t>
+  </si>
+  <si>
+    <t>126308138</t>
+  </si>
+  <si>
+    <t>3431951</t>
+  </si>
+  <si>
+    <t>2022-06-10 20:24</t>
+  </si>
+  <si>
+    <t>3443989</t>
+  </si>
+  <si>
+    <t>3443993</t>
+  </si>
+  <si>
     <t>2/0</t>
   </si>
   <si>
-    <t>Test company order 1</t>
-  </si>
-  <si>
-    <t>Test company order 1, 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>CDT</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0/2</t>
-  </si>
-  <si>
-    <t>824</t>
-  </si>
-  <si>
-    <t>764</t>
-  </si>
-  <si>
-    <t>Received</t>
-  </si>
-  <si>
-    <t>automation</t>
-  </si>
-  <si>
-    <t>ADV - ADVANCE FEES</t>
-  </si>
-  <si>
-    <t>$25.00</t>
-  </si>
-  <si>
-    <t>ADVANCE FEES</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Scheduler</t>
-  </si>
-  <si>
-    <t>Total :US$520.00</t>
-  </si>
-  <si>
-    <t>US$520.00</t>
-  </si>
-  <si>
-    <t>RTE Job Creation Manual</t>
-  </si>
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>One To One</t>
-  </si>
-  <si>
-    <t>One To Many</t>
-  </si>
-  <si>
-    <t>Many to One</t>
-  </si>
-  <si>
-    <t>Many To Many</t>
-  </si>
-  <si>
-    <t>RTE Job Creation OneToMany</t>
-  </si>
-  <si>
-    <t>RTE Job Creation ManyToOne</t>
-  </si>
-  <si>
-    <t>RTE Job Creation ManyToMany</t>
-  </si>
-  <si>
-    <t>RT00002275</t>
-  </si>
-  <si>
-    <t>RT00002276</t>
-  </si>
-  <si>
-    <t>RT00002277</t>
-  </si>
-  <si>
-    <t>RT00002274</t>
-  </si>
-  <si>
-    <t>RTE Automation NegFlow</t>
-  </si>
-  <si>
-    <t>RT00002335</t>
-  </si>
-  <si>
-    <t>126308862</t>
-  </si>
-  <si>
-    <t>ST FRANCIS MEDICAL CENTER</t>
-  </si>
-  <si>
-    <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
-  </si>
-  <si>
-    <t>126382916</t>
-  </si>
-  <si>
-    <t>3439505</t>
-  </si>
-  <si>
-    <t>3439560</t>
-  </si>
-  <si>
-    <t>126383371</t>
-  </si>
-  <si>
-    <t>2022-06-07 00:30</t>
-  </si>
-  <si>
-    <t>2022-06-07 13:14</t>
-  </si>
-  <si>
-    <t>Automation Merge RTE with LOC Job</t>
-  </si>
-  <si>
-    <t>RT00002367.</t>
-  </si>
-  <si>
-    <t>SVC</t>
-  </si>
-  <si>
-    <t>LOC</t>
-  </si>
-  <si>
-    <t>RT00001993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation RW </t>
-  </si>
-  <si>
-    <t>126404063</t>
-  </si>
-  <si>
-    <t>126403653</t>
-  </si>
-  <si>
-    <t>126404085</t>
-  </si>
-  <si>
-    <t>126404100</t>
-  </si>
-  <si>
-    <t>126384873</t>
-  </si>
-  <si>
-    <t>126403594</t>
-  </si>
-  <si>
-    <t>32436425</t>
-  </si>
-  <si>
-    <t>3441661</t>
-  </si>
-  <si>
-    <t>126404074</t>
-  </si>
-  <si>
-    <t>32436366</t>
-  </si>
-  <si>
-    <t>3441602</t>
-  </si>
-  <si>
-    <t>126403664</t>
-  </si>
-  <si>
-    <t>32436426</t>
-  </si>
-  <si>
-    <t>3441662</t>
-  </si>
-  <si>
-    <t>126404096</t>
-  </si>
-  <si>
-    <t>32436432</t>
-  </si>
-  <si>
-    <t>3441668</t>
-  </si>
-  <si>
-    <t>126404166</t>
-  </si>
-  <si>
-    <t>32436431</t>
-  </si>
-  <si>
-    <t>3441667</t>
-  </si>
-  <si>
-    <t>126404155</t>
-  </si>
-  <si>
-    <t>32436430</t>
-  </si>
-  <si>
-    <t>3441666</t>
-  </si>
-  <si>
-    <t>126404144</t>
-  </si>
-  <si>
-    <t>32436429</t>
-  </si>
-  <si>
-    <t>3441665</t>
-  </si>
-  <si>
-    <t>126404133</t>
-  </si>
-  <si>
-    <t>32436428</t>
-  </si>
-  <si>
-    <t>3441664</t>
-  </si>
-  <si>
-    <t>126404122</t>
-  </si>
-  <si>
-    <t>32436427</t>
-  </si>
-  <si>
-    <t>3441663</t>
-  </si>
-  <si>
-    <t>126404111</t>
-  </si>
-  <si>
-    <t>32434478</t>
-  </si>
-  <si>
-    <t>3439714</t>
-  </si>
-  <si>
-    <t>126384910</t>
-  </si>
-  <si>
-    <t>32434477</t>
-  </si>
-  <si>
-    <t>3439713</t>
-  </si>
-  <si>
-    <t>126384909</t>
-  </si>
-  <si>
-    <t>32434476</t>
-  </si>
-  <si>
-    <t>3439712</t>
-  </si>
-  <si>
-    <t>126384895</t>
-  </si>
-  <si>
-    <t>32434475</t>
-  </si>
-  <si>
-    <t>3439711</t>
-  </si>
-  <si>
-    <t>126384884</t>
-  </si>
-  <si>
-    <t>32436361</t>
-  </si>
-  <si>
-    <t>3441597</t>
-  </si>
-  <si>
-    <t>126403620</t>
-  </si>
-  <si>
-    <t>32436360</t>
-  </si>
-  <si>
-    <t>3441596</t>
-  </si>
-  <si>
-    <t>126403619</t>
-  </si>
-  <si>
-    <t>32436359</t>
-  </si>
-  <si>
-    <t>3441595</t>
-  </si>
-  <si>
-    <t>126403608</t>
-  </si>
-  <si>
-    <t>126405059</t>
-  </si>
-  <si>
-    <t>126403572</t>
-  </si>
-  <si>
-    <t>32436530</t>
-  </si>
-  <si>
-    <t>3441766</t>
-  </si>
-  <si>
-    <t>126405093</t>
-  </si>
-  <si>
-    <t>32436529</t>
-  </si>
-  <si>
-    <t>3441765</t>
-  </si>
-  <si>
-    <t>126405082</t>
-  </si>
-  <si>
-    <t>32436528</t>
-  </si>
-  <si>
-    <t>3441764</t>
-  </si>
-  <si>
-    <t>126405071</t>
-  </si>
-  <si>
-    <t>32436527</t>
-  </si>
-  <si>
-    <t>3441763</t>
-  </si>
-  <si>
-    <t>126405060</t>
-  </si>
-  <si>
-    <t>32436358</t>
-  </si>
-  <si>
-    <t>3441594</t>
-  </si>
-  <si>
-    <t>126403583</t>
-  </si>
-  <si>
-    <t>2022-06-08 00:30</t>
-  </si>
-  <si>
-    <t>2022-06-08 13:14</t>
-  </si>
-  <si>
-    <t>3441866</t>
-  </si>
-  <si>
-    <t>3441881</t>
-  </si>
-  <si>
-    <t>$960.00</t>
-  </si>
-  <si>
-    <t>1395 Minute(s)</t>
-  </si>
-  <si>
-    <t>Total :US$985.00</t>
-  </si>
-  <si>
-    <t>US$985.00</t>
-  </si>
-  <si>
-    <t>Delivery instruction for Automation Testing</t>
-  </si>
-  <si>
-    <t>2022-06-09 22:03</t>
-  </si>
-  <si>
-    <t>RT00002368.</t>
-  </si>
-  <si>
-    <t>32436645</t>
-  </si>
-  <si>
-    <t>126406344</t>
-  </si>
-  <si>
-    <t>3442001</t>
-  </si>
-  <si>
-    <t>3442009</t>
-  </si>
-  <si>
-    <t>RT00002369.</t>
+    <t>NYU OTHO HOSPTIAL</t>
+  </si>
+  <si>
+    <t>NYU OTHO HOSPTIAL, 301 E 17TH STREET, MANHATTAN, NY, 10003, USA</t>
+  </si>
+  <si>
+    <t>PickUp instruction for Automation Testing</t>
+  </si>
+  <si>
+    <t>2022-06-09 00:30</t>
+  </si>
+  <si>
+    <t>2022-06-09 01:14</t>
+  </si>
+  <si>
+    <t>3444051</t>
+  </si>
+  <si>
+    <t>3444054</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1535,24 +1460,24 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,92 +1488,92 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>68</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1663,7 +1588,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,49 +1613,49 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
         <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+      <c r="C4">
+        <v>3443513</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1738,16 +1663,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1804,55 +1729,55 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
       </c>
       <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" t="s">
         <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>168</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
       </c>
       <c r="M2" s="12"/>
     </row>
@@ -1860,19 +1785,19 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2305,7 +2230,7 @@
     <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2313,97 +2238,97 @@
         <v>10</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="K1" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="G2" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>136</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2797,39 +2722,39 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3066,7 +2991,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3080,23 +3005,23 @@
         <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3135,28 +3060,28 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3164,49 +3089,49 @@
         <v>126229651</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3299,40 +3224,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3340,13 +3265,13 @@
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3450,40 +3375,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final changes of 10th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
-    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
-    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
-    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
-    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
+    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
+    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
+    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="146">
   <si>
     <t>FileName</t>
   </si>
@@ -228,180 +228,6 @@
     <t xml:space="preserve">Automation RW </t>
   </si>
   <si>
-    <t>126405059</t>
-  </si>
-  <si>
-    <t>32436530</t>
-  </si>
-  <si>
-    <t>3441766</t>
-  </si>
-  <si>
-    <t>126405093</t>
-  </si>
-  <si>
-    <t>32436529</t>
-  </si>
-  <si>
-    <t>3441765</t>
-  </si>
-  <si>
-    <t>126405082</t>
-  </si>
-  <si>
-    <t>32436528</t>
-  </si>
-  <si>
-    <t>3441764</t>
-  </si>
-  <si>
-    <t>126405071</t>
-  </si>
-  <si>
-    <t>32436527</t>
-  </si>
-  <si>
-    <t>3441763</t>
-  </si>
-  <si>
-    <t>126405060</t>
-  </si>
-  <si>
-    <t>RT00002369.</t>
-  </si>
-  <si>
-    <t>126423194</t>
-  </si>
-  <si>
-    <t>126422636</t>
-  </si>
-  <si>
-    <t>126423219</t>
-  </si>
-  <si>
-    <t>126423231</t>
-  </si>
-  <si>
-    <t>126422142</t>
-  </si>
-  <si>
-    <t>126422120</t>
-  </si>
-  <si>
-    <t>32438401</t>
-  </si>
-  <si>
-    <t>3443637</t>
-  </si>
-  <si>
-    <t>126423208</t>
-  </si>
-  <si>
-    <t>32438324</t>
-  </si>
-  <si>
-    <t>3443560</t>
-  </si>
-  <si>
-    <t>126422647</t>
-  </si>
-  <si>
-    <t>32438402</t>
-  </si>
-  <si>
-    <t>126423220</t>
-  </si>
-  <si>
-    <t>32438408</t>
-  </si>
-  <si>
-    <t>3443644</t>
-  </si>
-  <si>
-    <t>126423297</t>
-  </si>
-  <si>
-    <t>32438407</t>
-  </si>
-  <si>
-    <t>3443643</t>
-  </si>
-  <si>
-    <t>126423286</t>
-  </si>
-  <si>
-    <t>32438406</t>
-  </si>
-  <si>
-    <t>3443642</t>
-  </si>
-  <si>
-    <t>126423275</t>
-  </si>
-  <si>
-    <t>32438405</t>
-  </si>
-  <si>
-    <t>3443641</t>
-  </si>
-  <si>
-    <t>126423264</t>
-  </si>
-  <si>
-    <t>32438404</t>
-  </si>
-  <si>
-    <t>3443640</t>
-  </si>
-  <si>
-    <t>126423253</t>
-  </si>
-  <si>
-    <t>32438403</t>
-  </si>
-  <si>
-    <t>3443639</t>
-  </si>
-  <si>
-    <t>126423242</t>
-  </si>
-  <si>
-    <t>32438280</t>
-  </si>
-  <si>
-    <t>3443516</t>
-  </si>
-  <si>
-    <t>126422175</t>
-  </si>
-  <si>
-    <t>32438279</t>
-  </si>
-  <si>
-    <t>3443515</t>
-  </si>
-  <si>
-    <t>126422164</t>
-  </si>
-  <si>
-    <t>32438278</t>
-  </si>
-  <si>
-    <t>3443514</t>
-  </si>
-  <si>
-    <t>126422153</t>
-  </si>
-  <si>
-    <t>32438277</t>
-  </si>
-  <si>
-    <t>3443513</t>
-  </si>
-  <si>
-    <t>126422131</t>
-  </si>
-  <si>
     <t>Scheduler</t>
   </si>
   <si>
@@ -411,80 +237,235 @@
     <t>Delivery instruction for Automation Testing</t>
   </si>
   <si>
-    <t>$150.00</t>
-  </si>
-  <si>
-    <t>Fix Route Base Rate is applied</t>
-  </si>
-  <si>
-    <t>Total :US$150.00</t>
-  </si>
-  <si>
-    <t>US$150.00</t>
-  </si>
-  <si>
-    <t>EDT</t>
-  </si>
-  <si>
-    <t>STORAGE AMERICA</t>
-  </si>
-  <si>
-    <t>STORAGE AMERICA, 211 DENTON AVE, NEW HYDE PARK, NY, 11040, USA</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
     <t>2/0</t>
   </si>
   <si>
-    <t>NYU OTHO HOSPTIAL</t>
-  </si>
-  <si>
-    <t>NYU OTHO HOSPTIAL, 301 E 17TH STREET, MANHATTAN, NY, 10003, USA</t>
-  </si>
-  <si>
     <t>PickUp instruction for Automation Testing</t>
   </si>
   <si>
-    <t>2022-06-09 00:30</t>
-  </si>
-  <si>
-    <t>2022-06-09 01:14</t>
-  </si>
-  <si>
-    <t>3444051</t>
-  </si>
-  <si>
-    <t>3444054</t>
-  </si>
-  <si>
-    <t>2022-06-08 00:30</t>
-  </si>
-  <si>
-    <t>2022-06-08 01:14</t>
-  </si>
-  <si>
-    <t>126403583</t>
-  </si>
-  <si>
-    <t>3441594</t>
-  </si>
-  <si>
-    <t>3444462</t>
-  </si>
-  <si>
-    <t>3444471</t>
+    <t>126443060</t>
+  </si>
+  <si>
+    <t>126442605</t>
+  </si>
+  <si>
+    <t>126443082</t>
+  </si>
+  <si>
+    <t>126443118</t>
+  </si>
+  <si>
+    <t>126424456</t>
+  </si>
+  <si>
+    <t>126442100</t>
+  </si>
+  <si>
+    <t>126442085</t>
+  </si>
+  <si>
+    <t>32440301</t>
+  </si>
+  <si>
+    <t>3445537</t>
+  </si>
+  <si>
+    <t>126443071</t>
+  </si>
+  <si>
+    <t>32440238</t>
+  </si>
+  <si>
+    <t>3445474</t>
+  </si>
+  <si>
+    <t>126442616</t>
+  </si>
+  <si>
+    <t>32440302</t>
+  </si>
+  <si>
+    <t>3445538</t>
+  </si>
+  <si>
+    <t>126443093</t>
+  </si>
+  <si>
+    <t>32440309</t>
+  </si>
+  <si>
+    <t>3445545</t>
+  </si>
+  <si>
+    <t>126443174</t>
+  </si>
+  <si>
+    <t>32440308</t>
+  </si>
+  <si>
+    <t>3445544</t>
+  </si>
+  <si>
+    <t>126443163</t>
+  </si>
+  <si>
+    <t>32440307</t>
+  </si>
+  <si>
+    <t>3445543</t>
+  </si>
+  <si>
+    <t>126443152</t>
+  </si>
+  <si>
+    <t>32440306</t>
+  </si>
+  <si>
+    <t>3445542</t>
+  </si>
+  <si>
+    <t>126443141</t>
+  </si>
+  <si>
+    <t>32440305</t>
+  </si>
+  <si>
+    <t>3445541</t>
+  </si>
+  <si>
+    <t>126443130</t>
+  </si>
+  <si>
+    <t>32440304</t>
+  </si>
+  <si>
+    <t>3445540</t>
+  </si>
+  <si>
+    <t>126443129</t>
+  </si>
+  <si>
+    <t>32438523</t>
+  </si>
+  <si>
+    <t>3443759</t>
+  </si>
+  <si>
+    <t>126424490</t>
+  </si>
+  <si>
+    <t>32438522</t>
+  </si>
+  <si>
+    <t>3443758</t>
+  </si>
+  <si>
+    <t>126424489</t>
+  </si>
+  <si>
+    <t>32438521</t>
+  </si>
+  <si>
+    <t>3443757</t>
+  </si>
+  <si>
+    <t>126424478</t>
+  </si>
+  <si>
+    <t>32438520</t>
+  </si>
+  <si>
+    <t>3443756</t>
+  </si>
+  <si>
+    <t>126424467</t>
+  </si>
+  <si>
+    <t>32440196</t>
+  </si>
+  <si>
+    <t>3445432</t>
+  </si>
+  <si>
+    <t>126442133</t>
+  </si>
+  <si>
+    <t>32440195</t>
+  </si>
+  <si>
+    <t>3445431</t>
+  </si>
+  <si>
+    <t>126442122</t>
+  </si>
+  <si>
+    <t>32440194</t>
+  </si>
+  <si>
+    <t>3445430</t>
+  </si>
+  <si>
+    <t>126442111</t>
+  </si>
+  <si>
+    <t>32440193</t>
+  </si>
+  <si>
+    <t>3445429</t>
+  </si>
+  <si>
+    <t>126442096</t>
+  </si>
+  <si>
+    <t>$160.00</t>
+  </si>
+  <si>
+    <t>43 Minute(s)</t>
+  </si>
+  <si>
+    <t>228927</t>
+  </si>
+  <si>
+    <t>Total :US$160.00</t>
+  </si>
+  <si>
+    <t>US$160.00</t>
+  </si>
+  <si>
+    <t>Test company order 1</t>
+  </si>
+  <si>
+    <t>Test company order 1, 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
+  </si>
+  <si>
+    <t>2022-06-10 00:30</t>
+  </si>
+  <si>
+    <t>CDT</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>2022-06-10 01:13</t>
+  </si>
+  <si>
+    <t>RT00002399.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -936,131 +917,131 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="28" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1142,10 +1123,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1303,7 +1284,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1312,13 +1293,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1328,7 +1309,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1337,7 +1318,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1346,7 +1327,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1356,12 +1337,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1392,7 +1373,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1411,7 +1392,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1423,19 +1404,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1460,7 +1441,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>49</v>
@@ -1474,7 +1455,7 @@
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>49</v>
@@ -1488,7 +1469,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>49</v>
@@ -1502,7 +1483,7 @@
         <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>50</v>
@@ -1516,7 +1497,7 @@
         <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>51</v>
@@ -1530,7 +1511,7 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>52</v>
@@ -1555,7 +1536,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8" t="s">
@@ -1570,31 +1551,31 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1613,44 +1594,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
         <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
         <v>83</v>
       </c>
-      <c r="B3" t="s">
-        <v>91</v>
-      </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4">
-        <v>3441594</v>
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1663,28 +1644,28 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -1692,15 +1673,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1744,37 +1725,37 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -2206,14 +2187,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -2221,13 +2202,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2267,25 +2248,25 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G2" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
         <v>39</v>
@@ -2294,10 +2275,10 @@
         <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="K2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2307,28 +2288,28 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="G3" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="I3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="J3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K3" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2696,13 +2677,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -2710,11 +2691,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2739,10 +2720,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -2982,22 +2963,22 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3009,29 +2990,29 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>150</v>
+      <c r="A2" s="2">
+        <v>3444462</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>151</v>
+      <c r="A3" s="2">
+        <v>3443905</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3039,9 +3020,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3060,28 +3041,28 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3089,49 +3070,49 @@
         <v>126229651</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,14 +3170,14 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3204,8 +3185,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3224,40 +3205,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3265,13 +3246,13 @@
         <v>126230741</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,14 +3322,14 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3356,7 +3337,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3375,40 +3356,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,6 +3465,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 13th june 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="5"/>
+    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
-    <sheet name="Rate" sheetId="3" r:id="rId3"/>
-    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
-    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
-    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
-    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
-    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
-    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
+    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
+    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
+    <sheet name="Rate" r:id="rId3" sheetId="3"/>
+    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
+    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
+    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
+    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
+    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
+    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="127">
   <si>
     <t>FileName</t>
   </si>
@@ -243,180 +243,6 @@
     <t>PickUp instruction for Automation Testing</t>
   </si>
   <si>
-    <t>126443060</t>
-  </si>
-  <si>
-    <t>126442605</t>
-  </si>
-  <si>
-    <t>126443082</t>
-  </si>
-  <si>
-    <t>126443118</t>
-  </si>
-  <si>
-    <t>126424456</t>
-  </si>
-  <si>
-    <t>126442100</t>
-  </si>
-  <si>
-    <t>126442085</t>
-  </si>
-  <si>
-    <t>32440301</t>
-  </si>
-  <si>
-    <t>3445537</t>
-  </si>
-  <si>
-    <t>126443071</t>
-  </si>
-  <si>
-    <t>32440238</t>
-  </si>
-  <si>
-    <t>3445474</t>
-  </si>
-  <si>
-    <t>126442616</t>
-  </si>
-  <si>
-    <t>32440302</t>
-  </si>
-  <si>
-    <t>3445538</t>
-  </si>
-  <si>
-    <t>126443093</t>
-  </si>
-  <si>
-    <t>32440309</t>
-  </si>
-  <si>
-    <t>3445545</t>
-  </si>
-  <si>
-    <t>126443174</t>
-  </si>
-  <si>
-    <t>32440308</t>
-  </si>
-  <si>
-    <t>3445544</t>
-  </si>
-  <si>
-    <t>126443163</t>
-  </si>
-  <si>
-    <t>32440307</t>
-  </si>
-  <si>
-    <t>3445543</t>
-  </si>
-  <si>
-    <t>126443152</t>
-  </si>
-  <si>
-    <t>32440306</t>
-  </si>
-  <si>
-    <t>3445542</t>
-  </si>
-  <si>
-    <t>126443141</t>
-  </si>
-  <si>
-    <t>32440305</t>
-  </si>
-  <si>
-    <t>3445541</t>
-  </si>
-  <si>
-    <t>126443130</t>
-  </si>
-  <si>
-    <t>32440304</t>
-  </si>
-  <si>
-    <t>3445540</t>
-  </si>
-  <si>
-    <t>126443129</t>
-  </si>
-  <si>
-    <t>32438523</t>
-  </si>
-  <si>
-    <t>3443759</t>
-  </si>
-  <si>
-    <t>126424490</t>
-  </si>
-  <si>
-    <t>32438522</t>
-  </si>
-  <si>
-    <t>3443758</t>
-  </si>
-  <si>
-    <t>126424489</t>
-  </si>
-  <si>
-    <t>32438521</t>
-  </si>
-  <si>
-    <t>3443757</t>
-  </si>
-  <si>
-    <t>126424478</t>
-  </si>
-  <si>
-    <t>32438520</t>
-  </si>
-  <si>
-    <t>3443756</t>
-  </si>
-  <si>
-    <t>126424467</t>
-  </si>
-  <si>
-    <t>32440196</t>
-  </si>
-  <si>
-    <t>3445432</t>
-  </si>
-  <si>
-    <t>126442133</t>
-  </si>
-  <si>
-    <t>32440195</t>
-  </si>
-  <si>
-    <t>3445431</t>
-  </si>
-  <si>
-    <t>126442122</t>
-  </si>
-  <si>
-    <t>32440194</t>
-  </si>
-  <si>
-    <t>3445430</t>
-  </si>
-  <si>
-    <t>126442111</t>
-  </si>
-  <si>
-    <t>32440193</t>
-  </si>
-  <si>
-    <t>3445429</t>
-  </si>
-  <si>
-    <t>126442096</t>
-  </si>
-  <si>
     <t>$160.00</t>
   </si>
   <si>
@@ -438,9 +264,6 @@
     <t>Test company order 1, 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
   </si>
   <si>
-    <t>2022-06-10 00:30</t>
-  </si>
-  <si>
     <t>CDT</t>
   </si>
   <si>
@@ -456,17 +279,138 @@
     <t>43</t>
   </si>
   <si>
-    <t>2022-06-10 01:13</t>
-  </si>
-  <si>
     <t>RT00002399.</t>
+  </si>
+  <si>
+    <t>126477555</t>
+  </si>
+  <si>
+    <t>32443711</t>
+  </si>
+  <si>
+    <t>126477485</t>
+  </si>
+  <si>
+    <t>126477577</t>
+  </si>
+  <si>
+    <t>32443723</t>
+  </si>
+  <si>
+    <t>126477647</t>
+  </si>
+  <si>
+    <t>32443722</t>
+  </si>
+  <si>
+    <t>126477636</t>
+  </si>
+  <si>
+    <t>32443721</t>
+  </si>
+  <si>
+    <t>126477625</t>
+  </si>
+  <si>
+    <t>32443720</t>
+  </si>
+  <si>
+    <t>126477614</t>
+  </si>
+  <si>
+    <t>32443719</t>
+  </si>
+  <si>
+    <t>126477603</t>
+  </si>
+  <si>
+    <t>32443718</t>
+  </si>
+  <si>
+    <t>126477599</t>
+  </si>
+  <si>
+    <t>126477197</t>
+  </si>
+  <si>
+    <t>32443678</t>
+  </si>
+  <si>
+    <t>126477186</t>
+  </si>
+  <si>
+    <t>32443677</t>
+  </si>
+  <si>
+    <t>126477175</t>
+  </si>
+  <si>
+    <t>32443676</t>
+  </si>
+  <si>
+    <t>126477153</t>
+  </si>
+  <si>
+    <t>3449010</t>
+  </si>
+  <si>
+    <t>3449013</t>
+  </si>
+  <si>
+    <t>32443816</t>
+  </si>
+  <si>
+    <t>126478596</t>
+  </si>
+  <si>
+    <t>32443815</t>
+  </si>
+  <si>
+    <t>126478585</t>
+  </si>
+  <si>
+    <t>32443814</t>
+  </si>
+  <si>
+    <t>126478574</t>
+  </si>
+  <si>
+    <t>32443813</t>
+  </si>
+  <si>
+    <t>126478563</t>
+  </si>
+  <si>
+    <t>126459856</t>
+  </si>
+  <si>
+    <t>3447167</t>
+  </si>
+  <si>
+    <t>2022-06-11 00:30</t>
+  </si>
+  <si>
+    <t>2022-06-11 01:13</t>
+  </si>
+  <si>
+    <t>126460027</t>
+  </si>
+  <si>
+    <t>3447180</t>
+  </si>
+  <si>
+    <t>3449973</t>
+  </si>
+  <si>
+    <t>3449980</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,6 +565,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto-Regular"/>
     </font>
   </fonts>
   <fills count="29">
@@ -917,131 +866,132 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="17">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="28" fontId="21" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1123,10 +1073,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1284,7 +1234,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1293,13 +1243,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1309,7 +1259,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1318,7 +1268,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1327,7 +1277,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1337,12 +1287,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1373,7 +1323,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1392,7 +1342,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1404,22 +1354,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1433,91 +1383,91 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
+      <c r="C2">
+        <v>126459993</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="13" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C3" t="s">
-        <v>74</v>
+      <c r="C3">
+        <v>126459856</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>75</v>
+      <c r="C4">
+        <v>126460016</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C5" t="s">
-        <v>76</v>
+      <c r="C5">
+        <v>126460038</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>77</v>
+      <c r="C6">
+        <v>126460393</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C7" t="s">
-        <v>78</v>
+      <c r="C7">
+        <v>126459579</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
         <v>47</v>
       </c>
@@ -1531,54 +1481,54 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C10" t="s">
-        <v>79</v>
+      <c r="C10">
+        <v>126459557</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
@@ -1592,49 +1542,49 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>126459993</v>
+      </c>
+      <c r="B2">
+        <v>32443716</v>
+      </c>
+      <c r="C2">
+        <v>3447179</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>74</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>126459856</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="C3">
+        <v>3447167</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>126460016</v>
+      </c>
+      <c r="B4">
+        <v>3449872</v>
+      </c>
+      <c r="C4">
+        <v>3449872</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>62</v>
       </c>
@@ -1642,49 +1592,49 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>79</v>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>126459557</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" t="s">
-        <v>129</v>
+        <v>107</v>
+      </c>
+      <c r="C6">
+        <v>3447144</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1723,46 +1673,46 @@
       </c>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="F2" t="s">
         <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>133</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>134</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>135</v>
+        <v>77</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
       </c>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
@@ -1787,7 +1737,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1802,7 +1752,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1817,7 +1767,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1832,7 +1782,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1847,7 +1797,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1862,7 +1812,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1877,7 +1827,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1892,7 +1842,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1906,7 +1856,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1920,7 +1870,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1934,7 +1884,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1948,7 +1898,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1962,7 +1912,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1976,7 +1926,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1990,7 +1940,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2004,7 +1954,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2018,7 +1968,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2032,7 +1982,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2046,7 +1996,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2060,7 +2010,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2074,7 +2024,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2088,7 +2038,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2102,7 +2052,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2116,7 +2066,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2130,7 +2080,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2144,7 +2094,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2158,7 +2108,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2172,7 +2122,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2187,31 +2137,31 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2246,12 +2196,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -2260,10 +2210,10 @@
         <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -2275,13 +2225,13 @@
         <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="K2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" t="s">
@@ -2291,28 +2241,28 @@
         <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
         <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>143</v>
+        <v>84</v>
       </c>
       <c r="J3" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="K3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="2"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -2325,7 +2275,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="2"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2338,7 +2288,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="2"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2351,7 +2301,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2364,7 +2314,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2377,7 +2327,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="2"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2390,7 +2340,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="2"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2403,7 +2353,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="2"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2416,7 +2366,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2429,7 +2379,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2442,7 +2392,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2455,7 +2405,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2468,7 +2418,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2481,7 +2431,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2494,7 +2444,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2507,7 +2457,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2520,7 +2470,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2533,7 +2483,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2546,7 +2496,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2559,7 +2509,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2572,7 +2522,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2585,7 +2535,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2598,7 +2548,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2611,7 +2561,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2624,7 +2574,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2637,7 +2587,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2650,7 +2600,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2663,7 +2613,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2677,28 +2627,28 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -2718,12 +2668,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -2738,7 +2688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2746,7 +2696,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2754,7 +2704,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2762,7 +2712,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2770,7 +2720,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2778,7 +2728,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2786,7 +2736,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2794,7 +2744,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2802,7 +2752,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2810,7 +2760,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2818,7 +2768,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2826,7 +2776,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2834,7 +2784,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2842,7 +2792,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2850,7 +2800,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2858,7 +2808,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2866,7 +2816,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2874,7 +2824,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2882,7 +2832,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -2890,7 +2840,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2898,7 +2848,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -2906,7 +2856,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2914,7 +2864,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -2922,7 +2872,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -2930,7 +2880,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2938,7 +2888,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2946,7 +2896,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2954,7 +2904,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2963,25 +2913,25 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -2989,43 +2939,43 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>3444462</v>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>125</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>3443905</v>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>126</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3039,157 +2989,155 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>76</v>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>126460038</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
         <v>90</v>
+      </c>
+      <c r="C2">
+        <v>3447181</v>
       </c>
       <c r="D2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="16">
+        <v>3447182</v>
+      </c>
+      <c r="D3" t="s">
         <v>93</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>126229651</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>3447183</v>
+      </c>
+      <c r="D4" t="s">
         <v>95</v>
       </c>
-      <c r="C4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="C5" s="16">
+        <v>3447184</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="C6">
+        <v>3447185</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" t="s">
-        <v>105</v>
+        <v>100</v>
+      </c>
+      <c r="C7" s="16">
+        <v>3447186</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3203,144 +3151,142 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>77</v>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>126460393</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>3447216</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="C3">
+        <v>3447217</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="C4">
+        <v>3447218</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>126230741</v>
-      </c>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" t="s">
         <v>117</v>
+      </c>
+      <c r="C5">
+        <v>3447219</v>
       </c>
       <c r="D5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3354,117 +3300,117 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" t="s">
-        <v>120</v>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>126459579</v>
+      </c>
+      <c r="B2">
+        <v>32443679</v>
+      </c>
+      <c r="C2">
+        <v>3447145</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" t="s">
-        <v>123</v>
+        <v>103</v>
+      </c>
+      <c r="C3">
+        <v>3447146</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
+        <v>105</v>
+      </c>
+      <c r="C4">
+        <v>3447147</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final changes of 15th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="192">
   <si>
     <t>FileName</t>
   </si>
@@ -403,6 +403,201 @@
   </si>
   <si>
     <t>3449980</t>
+  </si>
+  <si>
+    <t>126515569</t>
+  </si>
+  <si>
+    <t>126515293</t>
+  </si>
+  <si>
+    <t>126515581</t>
+  </si>
+  <si>
+    <t>126515606</t>
+  </si>
+  <si>
+    <t>126516728</t>
+  </si>
+  <si>
+    <t>126514872</t>
+  </si>
+  <si>
+    <t>126514850</t>
+  </si>
+  <si>
+    <t>32447844</t>
+  </si>
+  <si>
+    <t>3453080</t>
+  </si>
+  <si>
+    <t>126515570</t>
+  </si>
+  <si>
+    <t>32447816</t>
+  </si>
+  <si>
+    <t>3453052</t>
+  </si>
+  <si>
+    <t>126515307</t>
+  </si>
+  <si>
+    <t>32447845</t>
+  </si>
+  <si>
+    <t>3453081</t>
+  </si>
+  <si>
+    <t>126515592</t>
+  </si>
+  <si>
+    <t>32447851</t>
+  </si>
+  <si>
+    <t>3453087</t>
+  </si>
+  <si>
+    <t>126515662</t>
+  </si>
+  <si>
+    <t>32447850</t>
+  </si>
+  <si>
+    <t>3453086</t>
+  </si>
+  <si>
+    <t>126515651</t>
+  </si>
+  <si>
+    <t>32447849</t>
+  </si>
+  <si>
+    <t>3453085</t>
+  </si>
+  <si>
+    <t>126515640</t>
+  </si>
+  <si>
+    <t>32447848</t>
+  </si>
+  <si>
+    <t>3453084</t>
+  </si>
+  <si>
+    <t>126515639</t>
+  </si>
+  <si>
+    <t>32447847</t>
+  </si>
+  <si>
+    <t>3453083</t>
+  </si>
+  <si>
+    <t>126515628</t>
+  </si>
+  <si>
+    <t>32447846</t>
+  </si>
+  <si>
+    <t>3453082</t>
+  </si>
+  <si>
+    <t>126515617</t>
+  </si>
+  <si>
+    <t>32447963</t>
+  </si>
+  <si>
+    <t>3453199</t>
+  </si>
+  <si>
+    <t>126516762</t>
+  </si>
+  <si>
+    <t>32447962</t>
+  </si>
+  <si>
+    <t>3453198</t>
+  </si>
+  <si>
+    <t>126516751</t>
+  </si>
+  <si>
+    <t>32447961</t>
+  </si>
+  <si>
+    <t>3453197</t>
+  </si>
+  <si>
+    <t>126516740</t>
+  </si>
+  <si>
+    <t>32447960</t>
+  </si>
+  <si>
+    <t>3453196</t>
+  </si>
+  <si>
+    <t>126516739</t>
+  </si>
+  <si>
+    <t>32447780</t>
+  </si>
+  <si>
+    <t>3453016</t>
+  </si>
+  <si>
+    <t>126514908</t>
+  </si>
+  <si>
+    <t>32447779</t>
+  </si>
+  <si>
+    <t>3453015</t>
+  </si>
+  <si>
+    <t>126514894</t>
+  </si>
+  <si>
+    <t>32447778</t>
+  </si>
+  <si>
+    <t>3453014</t>
+  </si>
+  <si>
+    <t>126514883</t>
+  </si>
+  <si>
+    <t>32447777</t>
+  </si>
+  <si>
+    <t>3453013</t>
+  </si>
+  <si>
+    <t>126514861</t>
+  </si>
+  <si>
+    <t>14101 Seeley Ave.</t>
+  </si>
+  <si>
+    <t>14101 Seeley Ave., 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
+  </si>
+  <si>
+    <t>2022-06-15 00:30</t>
+  </si>
+  <si>
+    <t>2022-06-15 01:13</t>
+  </si>
+  <si>
+    <t>3453863</t>
+  </si>
+  <si>
+    <t>3453870</t>
+  </si>
+  <si>
+    <t>RT00002411</t>
   </si>
 </sst>
 </file>
@@ -1390,8 +1585,8 @@
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>126459993</v>
+      <c r="C2" t="s">
+        <v>127</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>49</v>
@@ -1404,8 +1599,8 @@
       <c r="B3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C3">
-        <v>126459856</v>
+      <c r="C3" t="s">
+        <v>128</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>49</v>
@@ -1418,8 +1613,8 @@
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>126460016</v>
+      <c r="C4" t="s">
+        <v>129</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>49</v>
@@ -1432,8 +1627,8 @@
       <c r="B5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C5">
-        <v>126460038</v>
+      <c r="C5" t="s">
+        <v>130</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>50</v>
@@ -1446,8 +1641,8 @@
       <c r="B6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C6">
-        <v>126460393</v>
+      <c r="C6" t="s">
+        <v>131</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>51</v>
@@ -1460,8 +1655,8 @@
       <c r="B7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C7">
-        <v>126459579</v>
+      <c r="C7" t="s">
+        <v>132</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>52</v>
@@ -1486,7 +1681,7 @@
         <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>191</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8" t="s">
@@ -1500,8 +1695,8 @@
       <c r="B10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C10">
-        <v>126459557</v>
+      <c r="C10" t="s">
+        <v>133</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>49</v>
@@ -1543,45 +1738,45 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>126459993</v>
-      </c>
-      <c r="B2">
-        <v>32443716</v>
-      </c>
-      <c r="C2">
-        <v>3447179</v>
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>126459856</v>
+      <c r="A3" t="s">
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3">
-        <v>3447167</v>
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>126460016</v>
-      </c>
-      <c r="B4">
-        <v>3449872</v>
-      </c>
-      <c r="C4">
-        <v>3449872</v>
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1593,17 +1788,17 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>126459557</v>
+      <c r="A6" t="s">
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6">
-        <v>3447144</v>
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1675,10 +1870,10 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -2198,10 +2393,10 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
@@ -2210,10 +2405,10 @@
         <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>185</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>186</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -2225,7 +2420,7 @@
         <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="K2" t="s">
         <v>80</v>
@@ -2256,7 +2451,7 @@
         <v>84</v>
       </c>
       <c r="J3" t="s">
-        <v>122</v>
+        <v>188</v>
       </c>
       <c r="K3" t="s">
         <v>80</v>
@@ -2670,10 +2865,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -2941,7 +3136,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>65</v>
@@ -2949,7 +3144,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>65</v>
@@ -2990,77 +3185,77 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>126460038</v>
+      <c r="A2" t="s">
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2">
-        <v>3447181</v>
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="16">
-        <v>3447182</v>
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4">
-        <v>3447183</v>
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="16">
-        <v>3447184</v>
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6">
-        <v>3447185</v>
+        <v>155</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="16">
-        <v>3447186</v>
+        <v>158</v>
+      </c>
+      <c r="C7" t="s">
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3152,53 +3347,53 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>126460393</v>
+      <c r="A2" t="s">
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2">
-        <v>3447216</v>
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>162</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3">
-        <v>3447217</v>
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4">
-        <v>3447218</v>
+        <v>167</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5">
-        <v>3447219</v>
+        <v>170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3301,41 +3496,41 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>126459579</v>
-      </c>
-      <c r="B2">
-        <v>32443679</v>
-      </c>
-      <c r="C2">
-        <v>3447145</v>
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3">
-        <v>3447146</v>
+        <v>176</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4">
-        <v>3447147</v>
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>

<commit_message>
Final changes of 23rd Jun 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="222">
   <si>
     <t>FileName</t>
   </si>
@@ -482,6 +482,213 @@
   </si>
   <si>
     <t>RT00002207</t>
+  </si>
+  <si>
+    <t>126110090</t>
+  </si>
+  <si>
+    <t>126110115</t>
+  </si>
+  <si>
+    <t>126110137</t>
+  </si>
+  <si>
+    <t>126110159</t>
+  </si>
+  <si>
+    <t>126110757</t>
+  </si>
+  <si>
+    <t>126110229</t>
+  </si>
+  <si>
+    <t>126110263</t>
+  </si>
+  <si>
+    <t>126110034</t>
+  </si>
+  <si>
+    <t>32403512</t>
+  </si>
+  <si>
+    <t>3408749</t>
+  </si>
+  <si>
+    <t>126110104</t>
+  </si>
+  <si>
+    <t>32403513</t>
+  </si>
+  <si>
+    <t>3408750</t>
+  </si>
+  <si>
+    <t>126110126</t>
+  </si>
+  <si>
+    <t>32403514</t>
+  </si>
+  <si>
+    <t>3408751</t>
+  </si>
+  <si>
+    <t>126110148</t>
+  </si>
+  <si>
+    <t>32403520</t>
+  </si>
+  <si>
+    <t>3408757</t>
+  </si>
+  <si>
+    <t>126110218</t>
+  </si>
+  <si>
+    <t>32403519</t>
+  </si>
+  <si>
+    <t>3408756</t>
+  </si>
+  <si>
+    <t>126110207</t>
+  </si>
+  <si>
+    <t>32403518</t>
+  </si>
+  <si>
+    <t>3408755</t>
+  </si>
+  <si>
+    <t>126110193</t>
+  </si>
+  <si>
+    <t>32403517</t>
+  </si>
+  <si>
+    <t>3408754</t>
+  </si>
+  <si>
+    <t>126110182</t>
+  </si>
+  <si>
+    <t>32403516</t>
+  </si>
+  <si>
+    <t>3408753</t>
+  </si>
+  <si>
+    <t>126110171</t>
+  </si>
+  <si>
+    <t>32403515</t>
+  </si>
+  <si>
+    <t>3408752</t>
+  </si>
+  <si>
+    <t>126110160</t>
+  </si>
+  <si>
+    <t>32403671</t>
+  </si>
+  <si>
+    <t>3408908</t>
+  </si>
+  <si>
+    <t>126110791</t>
+  </si>
+  <si>
+    <t>32403670</t>
+  </si>
+  <si>
+    <t>3408907</t>
+  </si>
+  <si>
+    <t>126110780</t>
+  </si>
+  <si>
+    <t>32403669</t>
+  </si>
+  <si>
+    <t>3408906</t>
+  </si>
+  <si>
+    <t>126110779</t>
+  </si>
+  <si>
+    <t>32403668</t>
+  </si>
+  <si>
+    <t>3408905</t>
+  </si>
+  <si>
+    <t>126110768</t>
+  </si>
+  <si>
+    <t>32403523</t>
+  </si>
+  <si>
+    <t>3408760</t>
+  </si>
+  <si>
+    <t>126110252</t>
+  </si>
+  <si>
+    <t>32403522</t>
+  </si>
+  <si>
+    <t>3408759</t>
+  </si>
+  <si>
+    <t>126110241</t>
+  </si>
+  <si>
+    <t>32403521</t>
+  </si>
+  <si>
+    <t>3408758</t>
+  </si>
+  <si>
+    <t>126110230</t>
+  </si>
+  <si>
+    <t>32403524</t>
+  </si>
+  <si>
+    <t>3408761</t>
+  </si>
+  <si>
+    <t>126110274</t>
+  </si>
+  <si>
+    <t>$160.00</t>
+  </si>
+  <si>
+    <t>3408942</t>
+  </si>
+  <si>
+    <t>3408946</t>
+  </si>
+  <si>
+    <t>3408948</t>
+  </si>
+  <si>
+    <t>RT00002211</t>
+  </si>
+  <si>
+    <t>$760.00</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>3409019</t>
+  </si>
+  <si>
+    <t>3409036</t>
+  </si>
+  <si>
+    <t>RT00002212</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1683,7 @@
         <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1490,7 +1697,7 @@
         <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1503,8 +1710,8 @@
       <c r="B4" t="s">
         <v>148</v>
       </c>
-      <c r="C4">
-        <v>126066463</v>
+      <c r="C4" t="s">
+        <v>155</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1518,7 +1725,7 @@
         <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1532,7 +1739,7 @@
         <v>150</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1546,7 +1753,7 @@
         <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1560,7 +1767,7 @@
         <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1574,7 +1781,7 @@
         <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>160</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1585,7 +1792,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1638,20 +1845,24 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>126096592</v>
+      <c r="A2" t="s">
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="16">
-        <v>150</v>
+        <v>215</v>
+      </c>
+      <c r="C2" t="s">
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+        <v>217</v>
+      </c>
+      <c r="E2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -1793,63 +2004,63 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>126066463</v>
+      <c r="A4" t="s">
+        <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4">
-        <v>3404435</v>
+        <v>167</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5">
-        <v>3407299</v>
+        <v>209</v>
+      </c>
+      <c r="C5" t="s">
+        <v>210</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>160</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1924,10 +2135,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2447,10 +2658,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -3189,8 +3400,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3408088</v>
+      <c r="A2" t="s">
+        <v>219</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3198,7 +3409,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>220</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
@@ -3240,76 +3451,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3402,52 +3613,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3551,40 +3762,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>201</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>204</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>206</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>207</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes of 29th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView activeTab="7" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="168">
   <si>
     <t>FileName</t>
   </si>
@@ -289,183 +289,6 @@
     <t>RT00002207</t>
   </si>
   <si>
-    <t>126110090</t>
-  </si>
-  <si>
-    <t>126110115</t>
-  </si>
-  <si>
-    <t>126110137</t>
-  </si>
-  <si>
-    <t>126110159</t>
-  </si>
-  <si>
-    <t>126110757</t>
-  </si>
-  <si>
-    <t>126110229</t>
-  </si>
-  <si>
-    <t>126110263</t>
-  </si>
-  <si>
-    <t>126110034</t>
-  </si>
-  <si>
-    <t>32403512</t>
-  </si>
-  <si>
-    <t>3408749</t>
-  </si>
-  <si>
-    <t>126110104</t>
-  </si>
-  <si>
-    <t>32403513</t>
-  </si>
-  <si>
-    <t>3408750</t>
-  </si>
-  <si>
-    <t>126110126</t>
-  </si>
-  <si>
-    <t>32403514</t>
-  </si>
-  <si>
-    <t>3408751</t>
-  </si>
-  <si>
-    <t>126110148</t>
-  </si>
-  <si>
-    <t>32403520</t>
-  </si>
-  <si>
-    <t>3408757</t>
-  </si>
-  <si>
-    <t>126110218</t>
-  </si>
-  <si>
-    <t>32403519</t>
-  </si>
-  <si>
-    <t>3408756</t>
-  </si>
-  <si>
-    <t>126110207</t>
-  </si>
-  <si>
-    <t>32403518</t>
-  </si>
-  <si>
-    <t>3408755</t>
-  </si>
-  <si>
-    <t>126110193</t>
-  </si>
-  <si>
-    <t>32403517</t>
-  </si>
-  <si>
-    <t>3408754</t>
-  </si>
-  <si>
-    <t>126110182</t>
-  </si>
-  <si>
-    <t>32403516</t>
-  </si>
-  <si>
-    <t>3408753</t>
-  </si>
-  <si>
-    <t>126110171</t>
-  </si>
-  <si>
-    <t>32403515</t>
-  </si>
-  <si>
-    <t>3408752</t>
-  </si>
-  <si>
-    <t>126110160</t>
-  </si>
-  <si>
-    <t>32403671</t>
-  </si>
-  <si>
-    <t>3408908</t>
-  </si>
-  <si>
-    <t>126110791</t>
-  </si>
-  <si>
-    <t>32403670</t>
-  </si>
-  <si>
-    <t>3408907</t>
-  </si>
-  <si>
-    <t>126110780</t>
-  </si>
-  <si>
-    <t>32403669</t>
-  </si>
-  <si>
-    <t>3408906</t>
-  </si>
-  <si>
-    <t>126110779</t>
-  </si>
-  <si>
-    <t>32403668</t>
-  </si>
-  <si>
-    <t>3408905</t>
-  </si>
-  <si>
-    <t>126110768</t>
-  </si>
-  <si>
-    <t>32403523</t>
-  </si>
-  <si>
-    <t>3408760</t>
-  </si>
-  <si>
-    <t>126110252</t>
-  </si>
-  <si>
-    <t>32403522</t>
-  </si>
-  <si>
-    <t>3408759</t>
-  </si>
-  <si>
-    <t>126110241</t>
-  </si>
-  <si>
-    <t>32403521</t>
-  </si>
-  <si>
-    <t>3408758</t>
-  </si>
-  <si>
-    <t>126110230</t>
-  </si>
-  <si>
-    <t>32403524</t>
-  </si>
-  <si>
-    <t>3408761</t>
-  </si>
-  <si>
-    <t>126110274</t>
-  </si>
-  <si>
     <t>$160.00</t>
   </si>
   <si>
@@ -478,279 +301,12 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>3409019</t>
-  </si>
-  <si>
-    <t>RT00002212</t>
-  </si>
-  <si>
-    <t>3409918</t>
-  </si>
-  <si>
-    <t>3409919</t>
-  </si>
-  <si>
-    <t>RT00002215</t>
-  </si>
-  <si>
-    <t>3409966</t>
-  </si>
-  <si>
-    <t>3409968</t>
-  </si>
-  <si>
-    <t>RT00002216</t>
-  </si>
-  <si>
-    <t>126132328</t>
-  </si>
-  <si>
-    <t>126132340</t>
-  </si>
-  <si>
-    <t>126132362</t>
-  </si>
-  <si>
-    <t>126132384</t>
-  </si>
-  <si>
-    <t>126133842</t>
-  </si>
-  <si>
-    <t>126132281</t>
-  </si>
-  <si>
-    <t>126132454</t>
-  </si>
-  <si>
-    <t>126133440</t>
-  </si>
-  <si>
-    <t>3411675</t>
-  </si>
-  <si>
-    <t>3411679</t>
-  </si>
-  <si>
-    <t>126139693</t>
-  </si>
-  <si>
     <t>126139718</t>
   </si>
   <si>
-    <t>126139730</t>
-  </si>
-  <si>
-    <t>126139752</t>
-  </si>
-  <si>
-    <t>126139659</t>
-  </si>
-  <si>
-    <t>126139822</t>
-  </si>
-  <si>
-    <t>126140808</t>
-  </si>
-  <si>
-    <t>32407042</t>
-  </si>
-  <si>
-    <t>3412279</t>
-  </si>
-  <si>
-    <t>126139707</t>
-  </si>
-  <si>
-    <t>3412395</t>
-  </si>
-  <si>
-    <t>3412399</t>
-  </si>
-  <si>
-    <t>32407043</t>
-  </si>
-  <si>
     <t>3412280</t>
   </si>
   <si>
-    <t>126139729</t>
-  </si>
-  <si>
-    <t>3412410</t>
-  </si>
-  <si>
-    <t>3412412</t>
-  </si>
-  <si>
-    <t>3412416</t>
-  </si>
-  <si>
-    <t>3412418</t>
-  </si>
-  <si>
-    <t>3412429</t>
-  </si>
-  <si>
-    <t>3412432</t>
-  </si>
-  <si>
-    <t>3412437</t>
-  </si>
-  <si>
-    <t>3412438</t>
-  </si>
-  <si>
-    <t>126141241</t>
-  </si>
-  <si>
-    <t>32407044</t>
-  </si>
-  <si>
-    <t>3412281</t>
-  </si>
-  <si>
-    <t>126139741</t>
-  </si>
-  <si>
-    <t>32407050</t>
-  </si>
-  <si>
-    <t>3412287</t>
-  </si>
-  <si>
-    <t>126139811</t>
-  </si>
-  <si>
-    <t>32407049</t>
-  </si>
-  <si>
-    <t>3412286</t>
-  </si>
-  <si>
-    <t>126139800</t>
-  </si>
-  <si>
-    <t>32407048</t>
-  </si>
-  <si>
-    <t>3412285</t>
-  </si>
-  <si>
-    <t>126139796</t>
-  </si>
-  <si>
-    <t>32407047</t>
-  </si>
-  <si>
-    <t>3412284</t>
-  </si>
-  <si>
-    <t>126139785</t>
-  </si>
-  <si>
-    <t>32407046</t>
-  </si>
-  <si>
-    <t>3412283</t>
-  </si>
-  <si>
-    <t>126139774</t>
-  </si>
-  <si>
-    <t>32407045</t>
-  </si>
-  <si>
-    <t>3412282</t>
-  </si>
-  <si>
-    <t>126139763</t>
-  </si>
-  <si>
-    <t>32407190</t>
-  </si>
-  <si>
-    <t>3412427</t>
-  </si>
-  <si>
-    <t>126141285</t>
-  </si>
-  <si>
-    <t>32407189</t>
-  </si>
-  <si>
-    <t>3412426</t>
-  </si>
-  <si>
-    <t>126141274</t>
-  </si>
-  <si>
-    <t>32407188</t>
-  </si>
-  <si>
-    <t>3412425</t>
-  </si>
-  <si>
-    <t>126141263</t>
-  </si>
-  <si>
-    <t>32407187</t>
-  </si>
-  <si>
-    <t>3412424</t>
-  </si>
-  <si>
-    <t>126141252</t>
-  </si>
-  <si>
-    <t>32407041</t>
-  </si>
-  <si>
-    <t>3412278</t>
-  </si>
-  <si>
-    <t>126139682</t>
-  </si>
-  <si>
-    <t>32407040</t>
-  </si>
-  <si>
-    <t>3412277</t>
-  </si>
-  <si>
-    <t>126139671</t>
-  </si>
-  <si>
-    <t>32407039</t>
-  </si>
-  <si>
-    <t>3412276</t>
-  </si>
-  <si>
-    <t>126139660</t>
-  </si>
-  <si>
-    <t>32407051</t>
-  </si>
-  <si>
-    <t>3412288</t>
-  </si>
-  <si>
-    <t>126139833</t>
-  </si>
-  <si>
-    <t>3412457</t>
-  </si>
-  <si>
-    <t>3412458</t>
-  </si>
-  <si>
-    <t>3412498</t>
-  </si>
-  <si>
-    <t>3412499</t>
-  </si>
-  <si>
     <t>3412526</t>
   </si>
   <si>
@@ -758,6 +314,219 @@
   </si>
   <si>
     <t>RT00002246</t>
+  </si>
+  <si>
+    <t>126145607</t>
+  </si>
+  <si>
+    <t>126145629</t>
+  </si>
+  <si>
+    <t>126145663</t>
+  </si>
+  <si>
+    <t>126145560</t>
+  </si>
+  <si>
+    <t>126145733</t>
+  </si>
+  <si>
+    <t>126146604</t>
+  </si>
+  <si>
+    <t>32407906</t>
+  </si>
+  <si>
+    <t>3413143</t>
+  </si>
+  <si>
+    <t>126145618</t>
+  </si>
+  <si>
+    <t>32407907</t>
+  </si>
+  <si>
+    <t>3413144</t>
+  </si>
+  <si>
+    <t>126145630</t>
+  </si>
+  <si>
+    <t>32407908</t>
+  </si>
+  <si>
+    <t>126145652</t>
+  </si>
+  <si>
+    <t>32407914</t>
+  </si>
+  <si>
+    <t>3413151</t>
+  </si>
+  <si>
+    <t>126145722</t>
+  </si>
+  <si>
+    <t>32407913</t>
+  </si>
+  <si>
+    <t>3413150</t>
+  </si>
+  <si>
+    <t>126145711</t>
+  </si>
+  <si>
+    <t>32407912</t>
+  </si>
+  <si>
+    <t>3413149</t>
+  </si>
+  <si>
+    <t>126145700</t>
+  </si>
+  <si>
+    <t>32407911</t>
+  </si>
+  <si>
+    <t>3413148</t>
+  </si>
+  <si>
+    <t>126145696</t>
+  </si>
+  <si>
+    <t>32407910</t>
+  </si>
+  <si>
+    <t>3413147</t>
+  </si>
+  <si>
+    <t>126145685</t>
+  </si>
+  <si>
+    <t>32407909</t>
+  </si>
+  <si>
+    <t>3413146</t>
+  </si>
+  <si>
+    <t>126145674</t>
+  </si>
+  <si>
+    <t>32408166</t>
+  </si>
+  <si>
+    <t>126147140</t>
+  </si>
+  <si>
+    <t>32408165</t>
+  </si>
+  <si>
+    <t>126147139</t>
+  </si>
+  <si>
+    <t>32408164</t>
+  </si>
+  <si>
+    <t>126147128</t>
+  </si>
+  <si>
+    <t>32408163</t>
+  </si>
+  <si>
+    <t>126147117</t>
+  </si>
+  <si>
+    <t>32407905</t>
+  </si>
+  <si>
+    <t>3413142</t>
+  </si>
+  <si>
+    <t>126145593</t>
+  </si>
+  <si>
+    <t>32407904</t>
+  </si>
+  <si>
+    <t>3413141</t>
+  </si>
+  <si>
+    <t>126145582</t>
+  </si>
+  <si>
+    <t>32407903</t>
+  </si>
+  <si>
+    <t>3413140</t>
+  </si>
+  <si>
+    <t>126145571</t>
+  </si>
+  <si>
+    <t>32407915</t>
+  </si>
+  <si>
+    <t>3413152</t>
+  </si>
+  <si>
+    <t>126145744</t>
+  </si>
+  <si>
+    <t>43 Minute(s)</t>
+  </si>
+  <si>
+    <t>228927</t>
+  </si>
+  <si>
+    <t>Total :US$160.00</t>
+  </si>
+  <si>
+    <t>US$160.00</t>
+  </si>
+  <si>
+    <t>2/0</t>
+  </si>
+  <si>
+    <t>Test company order 1</t>
+  </si>
+  <si>
+    <t>Test company order 1, 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
+  </si>
+  <si>
+    <t>PickUp instruction for Automation Testing</t>
+  </si>
+  <si>
+    <t>2022-06-23 22:30</t>
+  </si>
+  <si>
+    <t>CDT</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>2022-06-23 23:13</t>
+  </si>
+  <si>
+    <t>126115165</t>
+  </si>
+  <si>
+    <t>3409634</t>
+  </si>
+  <si>
+    <t>3413625</t>
+  </si>
+  <si>
+    <t>3413642</t>
   </si>
 </sst>
 </file>
@@ -765,7 +534,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -920,6 +689,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto-Regular"/>
     </font>
   </fonts>
   <fills count="28">
@@ -1253,7 +1027,7 @@
     <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -1288,6 +1062,7 @@
     <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
@@ -1715,11 +1490,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
@@ -1727,7 +1502,7 @@
     <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1516,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1749,13 +1524,13 @@
         <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="14" t="s">
         <v>54</v>
       </c>
@@ -1763,27 +1538,27 @@
         <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
-        <v>171</v>
+      <c r="C4">
+        <v>126115154</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
@@ -1791,27 +1566,27 @@
         <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>99</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>85</v>
       </c>
-      <c r="C6" t="s">
-        <v>192</v>
+      <c r="C6">
+        <v>126128776</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -1819,13 +1594,13 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>100</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>80</v>
       </c>
@@ -1833,13 +1608,13 @@
         <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>101</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
@@ -1847,18 +1622,18 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>102</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>244</v>
+        <v>96</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1880,7 +1655,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
@@ -1890,7 +1665,7 @@
     <col min="6" max="8" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -1910,27 +1685,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1938,7 +1713,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1946,7 +1721,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1954,7 +1729,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1962,7 +1737,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1970,7 +1745,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1978,7 +1753,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1986,7 +1761,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1994,7 +1769,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2002,7 +1777,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2010,7 +1785,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2018,7 +1793,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2045,16 +1820,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
     <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -2068,65 +1843,65 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>171</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>126115154</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4" t="s">
-        <v>194</v>
+        <v>109</v>
+      </c>
+      <c r="C4">
+        <v>3409634</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>147</v>
       </c>
       <c r="D5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>102</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2147,7 +1922,7 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
@@ -2160,7 +1935,7 @@
     <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2199,46 +1974,46 @@
       </c>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="F2" t="s">
         <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
@@ -2263,7 +2038,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2278,7 +2053,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2293,7 +2068,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2308,7 +2083,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2323,7 +2098,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2338,7 +2113,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2353,7 +2128,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2368,7 +2143,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2382,7 +2157,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2396,7 +2171,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2410,7 +2185,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2424,7 +2199,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2438,7 +2213,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2452,7 +2227,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2466,7 +2241,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2480,7 +2255,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2494,7 +2269,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2508,7 +2283,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2522,7 +2297,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2536,7 +2311,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2550,7 +2325,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2564,7 +2339,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2578,7 +2353,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2592,7 +2367,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2606,7 +2381,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2620,7 +2395,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2634,7 +2409,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2648,7 +2423,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2676,7 +2451,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
@@ -2687,7 +2462,7 @@
     <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2722,27 +2497,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>154</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="H2" t="s">
         <v>37</v>
@@ -2751,13 +2526,13 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" t="s">
@@ -2767,28 +2542,28 @@
         <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>159</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
         <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="K3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="2"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -2801,7 +2576,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="2"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2814,7 +2589,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="2"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2827,7 +2602,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2840,7 +2615,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2853,7 +2628,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="2"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2866,7 +2641,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="2"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2879,7 +2654,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="2"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2892,7 +2667,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2905,7 +2680,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2918,7 +2693,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2931,7 +2706,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2944,7 +2719,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2957,7 +2732,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2970,7 +2745,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2983,7 +2758,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2996,7 +2771,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -3009,7 +2784,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -3022,7 +2797,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3035,7 +2810,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3048,7 +2823,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3061,7 +2836,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3074,7 +2849,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3087,7 +2862,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3100,7 +2875,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3113,7 +2888,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3126,7 +2901,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3139,7 +2914,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3165,7 +2940,7 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
@@ -3174,7 +2949,7 @@
     <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -3194,27 +2969,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
       </c>
       <c r="F2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -3222,7 +2997,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3230,7 +3005,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -3238,7 +3013,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3246,7 +3021,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -3254,7 +3029,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3262,7 +3037,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -3270,7 +3045,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3278,7 +3053,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3286,7 +3061,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -3294,7 +3069,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3302,7 +3077,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3310,7 +3085,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -3318,7 +3093,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -3326,7 +3101,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -3334,7 +3109,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -3342,7 +3117,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3350,7 +3125,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -3358,7 +3133,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3366,7 +3141,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3374,7 +3149,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3382,7 +3157,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3390,7 +3165,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3398,7 +3173,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3406,7 +3181,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -3414,7 +3189,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3422,7 +3197,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3430,7 +3205,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -3451,13 +3226,13 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -3465,17 +3240,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>166</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>167</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
@@ -3494,14 +3269,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3515,129 +3290,129 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3653,17 +3428,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3677,117 +3452,117 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>192</v>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>126128776</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" t="s">
-        <v>215</v>
+        <v>129</v>
+      </c>
+      <c r="C2">
+        <v>3411112</v>
       </c>
       <c r="D2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" t="s">
-        <v>218</v>
+        <v>131</v>
+      </c>
+      <c r="C3" s="16">
+        <v>3411113</v>
       </c>
       <c r="D3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" t="s">
-        <v>221</v>
+        <v>133</v>
+      </c>
+      <c r="C4">
+        <v>3411114</v>
       </c>
       <c r="D4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" t="s">
-        <v>224</v>
+        <v>135</v>
+      </c>
+      <c r="C5" s="16">
+        <v>3411115</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3807,12 +3582,12 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3826,111 +3601,111 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>232</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
Changes of 30th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="7" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
-    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
-    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
-    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
-    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
-    <sheet name="CompareCharges" r:id="rId10" sheetId="10"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
+    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
+    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
+    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
+    <sheet name="CompareCharges" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
   <si>
     <t>FileName</t>
   </si>
@@ -226,45 +226,6 @@
     <t>RT00002194</t>
   </si>
   <si>
-    <t>$150.00</t>
-  </si>
-  <si>
-    <t>Fix Route Base Rate is applied</t>
-  </si>
-  <si>
-    <t>Total :US$150.00</t>
-  </si>
-  <si>
-    <t>US$150.00</t>
-  </si>
-  <si>
-    <t>EDT</t>
-  </si>
-  <si>
-    <t>STORAGE AMERICA</t>
-  </si>
-  <si>
-    <t>STORAGE AMERICA, 211 DENTON AVE, NEW HYDE PARK, NY, 11040, USA</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>2022-06-19 01:14</t>
-  </si>
-  <si>
-    <t>126066474</t>
-  </si>
-  <si>
-    <t>3404435</t>
-  </si>
-  <si>
-    <t>2022-06-24 01:42</t>
-  </si>
-  <si>
     <t>RTE Job Creation_Automation RTE</t>
   </si>
   <si>
@@ -292,186 +253,12 @@
     <t>$160.00</t>
   </si>
   <si>
-    <t>3408948</t>
-  </si>
-  <si>
     <t>$760.00</t>
   </si>
   <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t>126139718</t>
-  </si>
-  <si>
-    <t>3412280</t>
-  </si>
-  <si>
-    <t>3412526</t>
-  </si>
-  <si>
-    <t>3412527</t>
-  </si>
-  <si>
-    <t>RT00002246</t>
-  </si>
-  <si>
-    <t>126145607</t>
-  </si>
-  <si>
-    <t>126145629</t>
-  </si>
-  <si>
-    <t>126145663</t>
-  </si>
-  <si>
-    <t>126145560</t>
-  </si>
-  <si>
-    <t>126145733</t>
-  </si>
-  <si>
-    <t>126146604</t>
-  </si>
-  <si>
-    <t>32407906</t>
-  </si>
-  <si>
-    <t>3413143</t>
-  </si>
-  <si>
-    <t>126145618</t>
-  </si>
-  <si>
-    <t>32407907</t>
-  </si>
-  <si>
-    <t>3413144</t>
-  </si>
-  <si>
-    <t>126145630</t>
-  </si>
-  <si>
-    <t>32407908</t>
-  </si>
-  <si>
-    <t>126145652</t>
-  </si>
-  <si>
-    <t>32407914</t>
-  </si>
-  <si>
-    <t>3413151</t>
-  </si>
-  <si>
-    <t>126145722</t>
-  </si>
-  <si>
-    <t>32407913</t>
-  </si>
-  <si>
-    <t>3413150</t>
-  </si>
-  <si>
-    <t>126145711</t>
-  </si>
-  <si>
-    <t>32407912</t>
-  </si>
-  <si>
-    <t>3413149</t>
-  </si>
-  <si>
-    <t>126145700</t>
-  </si>
-  <si>
-    <t>32407911</t>
-  </si>
-  <si>
-    <t>3413148</t>
-  </si>
-  <si>
-    <t>126145696</t>
-  </si>
-  <si>
-    <t>32407910</t>
-  </si>
-  <si>
-    <t>3413147</t>
-  </si>
-  <si>
-    <t>126145685</t>
-  </si>
-  <si>
-    <t>32407909</t>
-  </si>
-  <si>
-    <t>3413146</t>
-  </si>
-  <si>
-    <t>126145674</t>
-  </si>
-  <si>
-    <t>32408166</t>
-  </si>
-  <si>
-    <t>126147140</t>
-  </si>
-  <si>
-    <t>32408165</t>
-  </si>
-  <si>
-    <t>126147139</t>
-  </si>
-  <si>
-    <t>32408164</t>
-  </si>
-  <si>
-    <t>126147128</t>
-  </si>
-  <si>
-    <t>32408163</t>
-  </si>
-  <si>
-    <t>126147117</t>
-  </si>
-  <si>
-    <t>32407905</t>
-  </si>
-  <si>
-    <t>3413142</t>
-  </si>
-  <si>
-    <t>126145593</t>
-  </si>
-  <si>
-    <t>32407904</t>
-  </si>
-  <si>
-    <t>3413141</t>
-  </si>
-  <si>
-    <t>126145582</t>
-  </si>
-  <si>
-    <t>32407903</t>
-  </si>
-  <si>
-    <t>3413140</t>
-  </si>
-  <si>
-    <t>126145571</t>
-  </si>
-  <si>
-    <t>32407915</t>
-  </si>
-  <si>
-    <t>3413152</t>
-  </si>
-  <si>
-    <t>126145744</t>
-  </si>
-  <si>
     <t>43 Minute(s)</t>
   </si>
   <si>
@@ -496,9 +283,6 @@
     <t>PickUp instruction for Automation Testing</t>
   </si>
   <si>
-    <t>2022-06-23 22:30</t>
-  </si>
-  <si>
     <t>CDT</t>
   </si>
   <si>
@@ -514,27 +298,203 @@
     <t>43</t>
   </si>
   <si>
-    <t>2022-06-23 23:13</t>
-  </si>
-  <si>
-    <t>126115165</t>
-  </si>
-  <si>
-    <t>3409634</t>
-  </si>
-  <si>
-    <t>3413625</t>
-  </si>
-  <si>
-    <t>3413642</t>
+    <t>126150371</t>
+  </si>
+  <si>
+    <t>126150393</t>
+  </si>
+  <si>
+    <t>126150418</t>
+  </si>
+  <si>
+    <t>126150430</t>
+  </si>
+  <si>
+    <t>126151873</t>
+  </si>
+  <si>
+    <t>126150337</t>
+  </si>
+  <si>
+    <t>126150500</t>
+  </si>
+  <si>
+    <t>126151459</t>
+  </si>
+  <si>
+    <t>32408646</t>
+  </si>
+  <si>
+    <t>3413883</t>
+  </si>
+  <si>
+    <t>126150360</t>
+  </si>
+  <si>
+    <t>32408645</t>
+  </si>
+  <si>
+    <t>3413882</t>
+  </si>
+  <si>
+    <t>126150359</t>
+  </si>
+  <si>
+    <t>32408644</t>
+  </si>
+  <si>
+    <t>3413881</t>
+  </si>
+  <si>
+    <t>126150348</t>
+  </si>
+  <si>
+    <t>32408656</t>
+  </si>
+  <si>
+    <t>3413893</t>
+  </si>
+  <si>
+    <t>126150511</t>
+  </si>
+  <si>
+    <t>32408647</t>
+  </si>
+  <si>
+    <t>3413884</t>
+  </si>
+  <si>
+    <t>126150382</t>
+  </si>
+  <si>
+    <t>32408648</t>
+  </si>
+  <si>
+    <t>3413885</t>
+  </si>
+  <si>
+    <t>126150407</t>
+  </si>
+  <si>
+    <t>32408649</t>
+  </si>
+  <si>
+    <t>3413886</t>
+  </si>
+  <si>
+    <t>126150429</t>
+  </si>
+  <si>
+    <t>32408655</t>
+  </si>
+  <si>
+    <t>3413892</t>
+  </si>
+  <si>
+    <t>126150496</t>
+  </si>
+  <si>
+    <t>32408654</t>
+  </si>
+  <si>
+    <t>3413891</t>
+  </si>
+  <si>
+    <t>126150485</t>
+  </si>
+  <si>
+    <t>32408653</t>
+  </si>
+  <si>
+    <t>3413890</t>
+  </si>
+  <si>
+    <t>126150474</t>
+  </si>
+  <si>
+    <t>32408652</t>
+  </si>
+  <si>
+    <t>3413889</t>
+  </si>
+  <si>
+    <t>126150463</t>
+  </si>
+  <si>
+    <t>32408651</t>
+  </si>
+  <si>
+    <t>3413888</t>
+  </si>
+  <si>
+    <t>126150452</t>
+  </si>
+  <si>
+    <t>32408650</t>
+  </si>
+  <si>
+    <t>3413887</t>
+  </si>
+  <si>
+    <t>126150441</t>
+  </si>
+  <si>
+    <t>32408777</t>
+  </si>
+  <si>
+    <t>3414014</t>
+  </si>
+  <si>
+    <t>126151910</t>
+  </si>
+  <si>
+    <t>32408776</t>
+  </si>
+  <si>
+    <t>3414013</t>
+  </si>
+  <si>
+    <t>126151909</t>
+  </si>
+  <si>
+    <t>32408775</t>
+  </si>
+  <si>
+    <t>3414012</t>
+  </si>
+  <si>
+    <t>126151895</t>
+  </si>
+  <si>
+    <t>32408774</t>
+  </si>
+  <si>
+    <t>3414011</t>
+  </si>
+  <si>
+    <t>126151884</t>
+  </si>
+  <si>
+    <t>2022-06-29 22:30</t>
+  </si>
+  <si>
+    <t>2022-06-29 23:13</t>
+  </si>
+  <si>
+    <t>3414119</t>
+  </si>
+  <si>
+    <t>3414120</t>
+  </si>
+  <si>
+    <t>RT00002267</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="23">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,11 +649,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto-Regular"/>
     </font>
   </fonts>
   <fills count="28">
@@ -984,129 +939,128 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1124,7 +1078,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1206,10 +1160,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1367,7 +1321,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1376,13 +1330,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1392,7 +1346,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1401,7 +1355,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1410,7 +1364,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1420,12 +1374,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1456,7 +1410,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1475,7 +1429,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1487,22 +1441,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1516,105 +1470,105 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4">
-        <v>126115154</v>
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6">
-        <v>126128776</v>
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
@@ -1622,18 +1576,18 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>154</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1641,31 +1595,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -1685,27 +1639,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" t="s">
-        <v>89</v>
+        <v>97</v>
+      </c>
+      <c r="B2">
+        <v>3414120</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1713,7 +1667,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1721,7 +1675,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1729,7 +1683,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1737,7 +1691,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1745,7 +1699,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1753,7 +1707,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1761,7 +1715,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1769,7 +1723,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1777,7 +1731,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1785,7 +1739,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1793,7 +1747,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1803,33 +1757,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -1843,99 +1797,99 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>97</v>
       </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>98</v>
-      </c>
-      <c r="B3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>126115154</v>
-      </c>
-      <c r="B4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4">
-        <v>3409634</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>102</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1974,46 +1928,46 @@
       </c>
       <c r="M1" s="11"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
@@ -2038,7 +1992,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2053,7 +2007,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2068,7 +2022,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2083,7 +2037,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2098,7 +2052,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2113,7 +2067,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2128,7 +2082,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2143,7 +2097,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2157,7 +2111,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2171,7 +2125,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2185,7 +2139,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2199,7 +2153,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2213,7 +2167,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2227,7 +2181,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2241,7 +2195,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2255,7 +2209,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2269,7 +2223,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2283,7 +2237,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2297,7 +2251,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2311,7 +2265,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2325,7 +2279,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2339,7 +2293,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2353,7 +2307,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2367,7 +2321,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2381,7 +2335,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2395,7 +2349,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2409,7 +2363,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2423,7 +2377,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2438,31 +2392,31 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2497,27 +2451,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
         <v>37</v>
@@ -2526,13 +2480,13 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="7"/>
       <c r="C3" t="s">
@@ -2542,28 +2496,28 @@
         <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
         <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>161</v>
+        <v>89</v>
       </c>
       <c r="I3" t="s">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="K3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -2576,7 +2530,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2589,7 +2543,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2602,7 +2556,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2615,7 +2569,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2628,7 +2582,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2641,7 +2595,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2654,7 +2608,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2667,7 +2621,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2680,7 +2634,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2693,7 +2647,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2706,7 +2660,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2719,7 +2673,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2732,7 +2686,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2745,7 +2699,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2758,7 +2712,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2771,7 +2725,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2784,7 +2738,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2797,7 +2751,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2810,7 +2764,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2823,7 +2777,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2836,7 +2790,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2849,7 +2803,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2862,7 +2816,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2875,7 +2829,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2888,7 +2842,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2901,7 +2855,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2914,7 +2868,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2928,28 +2882,28 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -2969,12 +2923,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -2989,7 +2943,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2997,7 +2951,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3005,7 +2959,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -3013,7 +2967,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3021,7 +2975,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -3029,7 +2983,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3037,7 +2991,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -3045,7 +2999,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3053,7 +3007,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3061,7 +3015,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -3069,7 +3023,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3077,7 +3031,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3085,7 +3039,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -3093,7 +3047,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -3101,7 +3055,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -3109,7 +3063,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -3117,7 +3071,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3125,7 +3079,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -3133,7 +3087,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3141,7 +3095,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3149,7 +3103,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3157,7 +3111,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3165,7 +3119,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -3173,7 +3127,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -3181,7 +3135,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -3189,7 +3143,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3197,7 +3151,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3205,7 +3159,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -3214,25 +3168,25 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -3240,43 +3194,43 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3290,155 +3244,155 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3452,142 +3406,142 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>126128776</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2">
-        <v>3411112</v>
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="16">
-        <v>3411113</v>
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4">
-        <v>3411114</v>
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="16">
-        <v>3411115</v>
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3601,117 +3555,117 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>100</v>
       </c>
-      <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>138</v>
-      </c>
       <c r="D2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of PU and Del stop enable disable 7th July
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="1"/>
+    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
-    <sheet name="Rate" sheetId="3" r:id="rId3"/>
-    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
-    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
-    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
-    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
-    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
-    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
-    <sheet name="CompareCharges" sheetId="10" r:id="rId10"/>
+    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
+    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
+    <sheet name="Rate" r:id="rId3" sheetId="3"/>
+    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
+    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
+    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
+    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
+    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
+    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
+    <sheet name="CompareCharges" r:id="rId10" sheetId="10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="165">
   <si>
     <t>FileName</t>
   </si>
@@ -298,202 +298,233 @@
     <t>43</t>
   </si>
   <si>
-    <t>126150371</t>
-  </si>
-  <si>
-    <t>126150393</t>
-  </si>
-  <si>
-    <t>126150418</t>
-  </si>
-  <si>
-    <t>126150430</t>
-  </si>
-  <si>
-    <t>126151873</t>
-  </si>
-  <si>
-    <t>126150337</t>
-  </si>
-  <si>
-    <t>126150500</t>
-  </si>
-  <si>
-    <t>126151459</t>
-  </si>
-  <si>
-    <t>32408646</t>
-  </si>
-  <si>
-    <t>3413883</t>
-  </si>
-  <si>
-    <t>126150360</t>
-  </si>
-  <si>
-    <t>32408645</t>
-  </si>
-  <si>
-    <t>3413882</t>
-  </si>
-  <si>
-    <t>126150359</t>
-  </si>
-  <si>
-    <t>32408644</t>
-  </si>
-  <si>
-    <t>3413881</t>
-  </si>
-  <si>
-    <t>126150348</t>
-  </si>
-  <si>
-    <t>32408656</t>
-  </si>
-  <si>
-    <t>3413893</t>
-  </si>
-  <si>
-    <t>126150511</t>
-  </si>
-  <si>
-    <t>32408647</t>
-  </si>
-  <si>
-    <t>3413884</t>
-  </si>
-  <si>
-    <t>126150382</t>
-  </si>
-  <si>
-    <t>32408648</t>
-  </si>
-  <si>
-    <t>3413885</t>
-  </si>
-  <si>
-    <t>126150407</t>
-  </si>
-  <si>
-    <t>32408649</t>
-  </si>
-  <si>
-    <t>3413886</t>
-  </si>
-  <si>
-    <t>126150429</t>
-  </si>
-  <si>
-    <t>32408655</t>
-  </si>
-  <si>
-    <t>3413892</t>
-  </si>
-  <si>
-    <t>126150496</t>
-  </si>
-  <si>
-    <t>32408654</t>
-  </si>
-  <si>
-    <t>3413891</t>
-  </si>
-  <si>
-    <t>126150485</t>
-  </si>
-  <si>
-    <t>32408653</t>
-  </si>
-  <si>
-    <t>3413890</t>
-  </si>
-  <si>
-    <t>126150474</t>
-  </si>
-  <si>
-    <t>32408652</t>
-  </si>
-  <si>
-    <t>3413889</t>
-  </si>
-  <si>
-    <t>126150463</t>
-  </si>
-  <si>
-    <t>32408651</t>
-  </si>
-  <si>
-    <t>3413888</t>
-  </si>
-  <si>
-    <t>126150452</t>
-  </si>
-  <si>
-    <t>32408650</t>
-  </si>
-  <si>
-    <t>3413887</t>
-  </si>
-  <si>
-    <t>126150441</t>
-  </si>
-  <si>
-    <t>32408777</t>
-  </si>
-  <si>
-    <t>3414014</t>
-  </si>
-  <si>
-    <t>126151910</t>
-  </si>
-  <si>
-    <t>32408776</t>
-  </si>
-  <si>
-    <t>3414013</t>
-  </si>
-  <si>
-    <t>126151909</t>
-  </si>
-  <si>
-    <t>32408775</t>
-  </si>
-  <si>
-    <t>3414012</t>
-  </si>
-  <si>
-    <t>126151895</t>
-  </si>
-  <si>
-    <t>32408774</t>
-  </si>
-  <si>
-    <t>3414011</t>
-  </si>
-  <si>
-    <t>126151884</t>
-  </si>
-  <si>
-    <t>2022-06-29 22:30</t>
-  </si>
-  <si>
-    <t>2022-06-29 23:13</t>
-  </si>
-  <si>
-    <t>3414119</t>
-  </si>
-  <si>
-    <t>3414120</t>
-  </si>
-  <si>
-    <t>RT00002267</t>
+    <t>ADD - ADDITIONAL STOP</t>
+  </si>
+  <si>
+    <t>$15.00</t>
+  </si>
+  <si>
+    <t>ADDITIONAL STOP</t>
+  </si>
+  <si>
+    <t>228540</t>
+  </si>
+  <si>
+    <t>$30.00</t>
+  </si>
+  <si>
+    <t>Base Rate</t>
+  </si>
+  <si>
+    <t>SAP - Saturday Pickup</t>
+  </si>
+  <si>
+    <t>Saturday Pickup</t>
+  </si>
+  <si>
+    <t>XML - Excess Mileage</t>
+  </si>
+  <si>
+    <t>$9.90</t>
+  </si>
+  <si>
+    <t>26 Mile(s)</t>
+  </si>
+  <si>
+    <t>126206485</t>
+  </si>
+  <si>
+    <t>126206500</t>
+  </si>
+  <si>
+    <t>126206522</t>
+  </si>
+  <si>
+    <t>126206544</t>
+  </si>
+  <si>
+    <t>126208467</t>
+  </si>
+  <si>
+    <t>126205983</t>
+  </si>
+  <si>
+    <t>126206614</t>
+  </si>
+  <si>
+    <t>126207921</t>
+  </si>
+  <si>
+    <t>32414440</t>
+  </si>
+  <si>
+    <t>3419674</t>
+  </si>
+  <si>
+    <t>126206496</t>
+  </si>
+  <si>
+    <t>32414441</t>
+  </si>
+  <si>
+    <t>3419675</t>
+  </si>
+  <si>
+    <t>126206511</t>
+  </si>
+  <si>
+    <t>32414442</t>
+  </si>
+  <si>
+    <t>3419676</t>
+  </si>
+  <si>
+    <t>126206533</t>
+  </si>
+  <si>
+    <t>32414448</t>
+  </si>
+  <si>
+    <t>3419682</t>
+  </si>
+  <si>
+    <t>126206603</t>
+  </si>
+  <si>
+    <t>32414447</t>
+  </si>
+  <si>
+    <t>3419681</t>
+  </si>
+  <si>
+    <t>126206599</t>
+  </si>
+  <si>
+    <t>32414446</t>
+  </si>
+  <si>
+    <t>3419680</t>
+  </si>
+  <si>
+    <t>126206588</t>
+  </si>
+  <si>
+    <t>32414445</t>
+  </si>
+  <si>
+    <t>3419679</t>
+  </si>
+  <si>
+    <t>126206577</t>
+  </si>
+  <si>
+    <t>32414444</t>
+  </si>
+  <si>
+    <t>3419678</t>
+  </si>
+  <si>
+    <t>126206566</t>
+  </si>
+  <si>
+    <t>32414443</t>
+  </si>
+  <si>
+    <t>3419677</t>
+  </si>
+  <si>
+    <t>126206555</t>
+  </si>
+  <si>
+    <t>32414622</t>
+  </si>
+  <si>
+    <t>3419856</t>
+  </si>
+  <si>
+    <t>126208504</t>
+  </si>
+  <si>
+    <t>32414621</t>
+  </si>
+  <si>
+    <t>3419855</t>
+  </si>
+  <si>
+    <t>126208490</t>
+  </si>
+  <si>
+    <t>32414620</t>
+  </si>
+  <si>
+    <t>3419854</t>
+  </si>
+  <si>
+    <t>126208489</t>
+  </si>
+  <si>
+    <t>32414619</t>
+  </si>
+  <si>
+    <t>3419853</t>
+  </si>
+  <si>
+    <t>126208478</t>
+  </si>
+  <si>
+    <t>32414394</t>
+  </si>
+  <si>
+    <t>3419628</t>
+  </si>
+  <si>
+    <t>126206016</t>
+  </si>
+  <si>
+    <t>32414393</t>
+  </si>
+  <si>
+    <t>3419627</t>
+  </si>
+  <si>
+    <t>126206005</t>
+  </si>
+  <si>
+    <t>32414392</t>
+  </si>
+  <si>
+    <t>3419626</t>
+  </si>
+  <si>
+    <t>126205994</t>
+  </si>
+  <si>
+    <t>32414449</t>
+  </si>
+  <si>
+    <t>126206625</t>
+  </si>
+  <si>
+    <t>2022-07-06 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-06 23:13</t>
+  </si>
+  <si>
+    <t>3419932</t>
+  </si>
+  <si>
+    <t>3419933</t>
+  </si>
+  <si>
+    <t>RT00002329</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -939,128 +970,128 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1078,7 +1109,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1160,10 +1191,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1321,7 +1352,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1330,13 +1361,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1346,7 +1377,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1355,7 +1386,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1364,7 +1395,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1374,12 +1405,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1410,7 +1441,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1429,7 +1460,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1441,19 +1472,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1478,7 +1509,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1492,7 +1523,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1506,7 +1537,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1520,7 +1551,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1534,7 +1565,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1548,7 +1579,7 @@
         <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1561,8 +1592,8 @@
       <c r="B8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" t="s">
-        <v>97</v>
+      <c r="C8">
+        <v>126173695</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1576,7 +1607,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1587,7 +1618,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1595,15 +1626,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
@@ -1611,12 +1642,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,10 +1672,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2">
-        <v>3414120</v>
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -1757,30 +1788,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,78 +1830,78 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
         <v>111</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
         <v>114</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>115</v>
-      </c>
-      <c r="D3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4">
+        <v>3419676</v>
+      </c>
+      <c r="D4" t="s">
         <v>118</v>
       </c>
-      <c r="D4" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>97</v>
+      <c r="A5">
+        <v>126173695</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
+        <v>158</v>
+      </c>
+      <c r="C5">
+        <v>3415612</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -1878,15 +1909,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1930,10 +1961,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -1995,11 +2026,21 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -2010,11 +2051,21 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -2025,11 +2076,21 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -2040,11 +2101,21 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -2392,14 +2463,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -2407,13 +2478,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2453,10 +2524,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2480,7 +2551,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K2" t="s">
         <v>86</v>
@@ -2511,7 +2582,7 @@
         <v>90</v>
       </c>
       <c r="J3" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="K3" t="s">
         <v>86</v>
@@ -2882,13 +2953,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -2896,11 +2967,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2925,10 +2996,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
         <v>118</v>
-      </c>
-      <c r="B2" t="s">
-        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3168,13 +3239,13 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -3182,8 +3253,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3196,7 +3267,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3204,20 +3275,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -3225,9 +3296,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3246,76 +3317,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
         <v>120</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>121</v>
-      </c>
-      <c r="D2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>124</v>
-      </c>
-      <c r="D3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
         <v>126</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>127</v>
-      </c>
-      <c r="D4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
         <v>129</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>130</v>
-      </c>
-      <c r="D5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
         <v>132</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>133</v>
-      </c>
-      <c r="D6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" t="s">
         <v>135</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>136</v>
-      </c>
-      <c r="D7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3373,14 +3444,14 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
@@ -3388,8 +3459,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3408,52 +3479,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
         <v>138</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>139</v>
-      </c>
-      <c r="D2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
         <v>141</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
         <v>144</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>145</v>
-      </c>
-      <c r="D4" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
         <v>147</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>148</v>
-      </c>
-      <c r="D5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3523,14 +3594,14 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
@@ -3538,7 +3609,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3557,40 +3628,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3666,6 +3737,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 8th July 2022 for Copy all and Copy Next
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView activeTab="7" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="166">
   <si>
     <t>FileName</t>
   </si>
@@ -331,180 +331,18 @@
     <t>26 Mile(s)</t>
   </si>
   <si>
-    <t>126206485</t>
-  </si>
-  <si>
     <t>126206500</t>
   </si>
   <si>
-    <t>126206522</t>
-  </si>
-  <si>
-    <t>126206544</t>
-  </si>
-  <si>
-    <t>126208467</t>
-  </si>
-  <si>
-    <t>126205983</t>
-  </si>
-  <si>
-    <t>126206614</t>
-  </si>
-  <si>
-    <t>126207921</t>
-  </si>
-  <si>
-    <t>32414440</t>
-  </si>
-  <si>
-    <t>3419674</t>
-  </si>
-  <si>
-    <t>126206496</t>
-  </si>
-  <si>
-    <t>32414441</t>
-  </si>
-  <si>
     <t>3419675</t>
   </si>
   <si>
-    <t>126206511</t>
-  </si>
-  <si>
-    <t>32414442</t>
-  </si>
-  <si>
     <t>3419676</t>
   </si>
   <si>
     <t>126206533</t>
   </si>
   <si>
-    <t>32414448</t>
-  </si>
-  <si>
-    <t>3419682</t>
-  </si>
-  <si>
-    <t>126206603</t>
-  </si>
-  <si>
-    <t>32414447</t>
-  </si>
-  <si>
-    <t>3419681</t>
-  </si>
-  <si>
-    <t>126206599</t>
-  </si>
-  <si>
-    <t>32414446</t>
-  </si>
-  <si>
-    <t>3419680</t>
-  </si>
-  <si>
-    <t>126206588</t>
-  </si>
-  <si>
-    <t>32414445</t>
-  </si>
-  <si>
-    <t>3419679</t>
-  </si>
-  <si>
-    <t>126206577</t>
-  </si>
-  <si>
-    <t>32414444</t>
-  </si>
-  <si>
-    <t>3419678</t>
-  </si>
-  <si>
-    <t>126206566</t>
-  </si>
-  <si>
-    <t>32414443</t>
-  </si>
-  <si>
-    <t>3419677</t>
-  </si>
-  <si>
-    <t>126206555</t>
-  </si>
-  <si>
-    <t>32414622</t>
-  </si>
-  <si>
-    <t>3419856</t>
-  </si>
-  <si>
-    <t>126208504</t>
-  </si>
-  <si>
-    <t>32414621</t>
-  </si>
-  <si>
-    <t>3419855</t>
-  </si>
-  <si>
-    <t>126208490</t>
-  </si>
-  <si>
-    <t>32414620</t>
-  </si>
-  <si>
-    <t>3419854</t>
-  </si>
-  <si>
-    <t>126208489</t>
-  </si>
-  <si>
-    <t>32414619</t>
-  </si>
-  <si>
-    <t>3419853</t>
-  </si>
-  <si>
-    <t>126208478</t>
-  </si>
-  <si>
-    <t>32414394</t>
-  </si>
-  <si>
-    <t>3419628</t>
-  </si>
-  <si>
-    <t>126206016</t>
-  </si>
-  <si>
-    <t>32414393</t>
-  </si>
-  <si>
-    <t>3419627</t>
-  </si>
-  <si>
-    <t>126206005</t>
-  </si>
-  <si>
-    <t>32414392</t>
-  </si>
-  <si>
-    <t>3419626</t>
-  </si>
-  <si>
-    <t>126205994</t>
-  </si>
-  <si>
-    <t>32414449</t>
-  </si>
-  <si>
-    <t>126206625</t>
-  </si>
-  <si>
     <t>2022-07-06 22:30</t>
   </si>
   <si>
@@ -518,6 +356,171 @@
   </si>
   <si>
     <t>RT00002329</t>
+  </si>
+  <si>
+    <t>126223958</t>
+  </si>
+  <si>
+    <t>126223970</t>
+  </si>
+  <si>
+    <t>126223992</t>
+  </si>
+  <si>
+    <t>126224014</t>
+  </si>
+  <si>
+    <t>126224081</t>
+  </si>
+  <si>
+    <t>126225099</t>
+  </si>
+  <si>
+    <t>32416358</t>
+  </si>
+  <si>
+    <t>3421592</t>
+  </si>
+  <si>
+    <t>126223969</t>
+  </si>
+  <si>
+    <t>32416359</t>
+  </si>
+  <si>
+    <t>3421593</t>
+  </si>
+  <si>
+    <t>126223981</t>
+  </si>
+  <si>
+    <t>32416360</t>
+  </si>
+  <si>
+    <t>3421594</t>
+  </si>
+  <si>
+    <t>126224003</t>
+  </si>
+  <si>
+    <t>32416366</t>
+  </si>
+  <si>
+    <t>3421600</t>
+  </si>
+  <si>
+    <t>126224070</t>
+  </si>
+  <si>
+    <t>32416365</t>
+  </si>
+  <si>
+    <t>3421599</t>
+  </si>
+  <si>
+    <t>126224069</t>
+  </si>
+  <si>
+    <t>32416364</t>
+  </si>
+  <si>
+    <t>3421598</t>
+  </si>
+  <si>
+    <t>126224058</t>
+  </si>
+  <si>
+    <t>32416363</t>
+  </si>
+  <si>
+    <t>3421597</t>
+  </si>
+  <si>
+    <t>126224047</t>
+  </si>
+  <si>
+    <t>32416362</t>
+  </si>
+  <si>
+    <t>3421596</t>
+  </si>
+  <si>
+    <t>126224036</t>
+  </si>
+  <si>
+    <t>32416361</t>
+  </si>
+  <si>
+    <t>3421595</t>
+  </si>
+  <si>
+    <t>126224025</t>
+  </si>
+  <si>
+    <t>32416534</t>
+  </si>
+  <si>
+    <t>126226029</t>
+  </si>
+  <si>
+    <t>32416533</t>
+  </si>
+  <si>
+    <t>126226018</t>
+  </si>
+  <si>
+    <t>32416532</t>
+  </si>
+  <si>
+    <t>126226007</t>
+  </si>
+  <si>
+    <t>32416531</t>
+  </si>
+  <si>
+    <t>126225996</t>
+  </si>
+  <si>
+    <t>32416323</t>
+  </si>
+  <si>
+    <t>126223590</t>
+  </si>
+  <si>
+    <t>32416322</t>
+  </si>
+  <si>
+    <t>126223589</t>
+  </si>
+  <si>
+    <t>32416321</t>
+  </si>
+  <si>
+    <t>126223578</t>
+  </si>
+  <si>
+    <t>32416367</t>
+  </si>
+  <si>
+    <t>3421601</t>
+  </si>
+  <si>
+    <t>126224092</t>
+  </si>
+  <si>
+    <t>2022-07-07 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-07 23:13</t>
+  </si>
+  <si>
+    <t>3421947</t>
+  </si>
+  <si>
+    <t>3421952</t>
+  </si>
+  <si>
+    <t>RT00002344</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1479,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,7 +1512,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1523,7 +1526,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1537,7 +1540,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1551,7 +1554,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1564,8 +1567,8 @@
       <c r="B6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
-        <v>106</v>
+      <c r="C6">
+        <v>126184475</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1578,8 +1581,8 @@
       <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" t="s">
-        <v>107</v>
+      <c r="C7">
+        <v>126173651</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1592,8 +1595,8 @@
       <c r="B8" t="s">
         <v>74</v>
       </c>
-      <c r="C8">
-        <v>126173695</v>
+      <c r="C8" t="s">
+        <v>115</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1607,7 +1610,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1618,7 +1621,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1672,10 +1675,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -1804,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,63 +1833,63 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4">
-        <v>3419676</v>
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>126173695</v>
+      <c r="A5" t="s">
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>158</v>
       </c>
-      <c r="C5">
-        <v>3415612</v>
+      <c r="C5" t="s">
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1961,10 +1964,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2524,10 +2527,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2551,7 +2554,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K2" t="s">
         <v>86</v>
@@ -2582,7 +2585,7 @@
         <v>90</v>
       </c>
       <c r="J3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K3" t="s">
         <v>86</v>
@@ -2996,10 +2999,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3267,7 +3270,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3275,7 +3278,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
@@ -3291,7 +3294,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,76 +3320,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3453,8 +3456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3478,53 +3481,53 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>106</v>
+      <c r="A2">
+        <v>126184475</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>138</v>
+        <v>144</v>
+      </c>
+      <c r="C2">
+        <v>3417266</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C3" t="s">
-        <v>141</v>
+        <v>146</v>
+      </c>
+      <c r="C3">
+        <v>3417267</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" t="s">
-        <v>144</v>
+        <v>148</v>
+      </c>
+      <c r="C4">
+        <v>3417268</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <v>3417269</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3604,7 +3607,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3627,40 +3630,40 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" t="s">
-        <v>151</v>
+      <c r="A2" s="2">
+        <v>126173651</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3416137</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="2" t="s">
         <v>154</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3416138</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="2">
+        <v>3416139</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes of 12th July for ManyTo One Many To Manya ANd AGent charges and driver
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="7" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
-    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
-    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
-    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
-    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
-    <sheet name="CompareCharges" r:id="rId10" sheetId="10"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
+    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
+    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
+    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
+    <sheet name="CompareCharges" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="164">
   <si>
     <t>FileName</t>
   </si>
@@ -331,203 +331,196 @@
     <t>26 Mile(s)</t>
   </si>
   <si>
-    <t>126206500</t>
-  </si>
-  <si>
-    <t>3419675</t>
-  </si>
-  <si>
-    <t>3419676</t>
-  </si>
-  <si>
-    <t>126206533</t>
-  </si>
-  <si>
-    <t>2022-07-06 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-06 23:13</t>
-  </si>
-  <si>
-    <t>3419932</t>
-  </si>
-  <si>
     <t>3419933</t>
   </si>
   <si>
-    <t>RT00002329</t>
-  </si>
-  <si>
-    <t>126223958</t>
-  </si>
-  <si>
-    <t>126223970</t>
-  </si>
-  <si>
-    <t>126223992</t>
-  </si>
-  <si>
-    <t>126224014</t>
-  </si>
-  <si>
-    <t>126224081</t>
-  </si>
-  <si>
-    <t>126225099</t>
-  </si>
-  <si>
-    <t>32416358</t>
-  </si>
-  <si>
-    <t>3421592</t>
-  </si>
-  <si>
-    <t>126223969</t>
-  </si>
-  <si>
-    <t>32416359</t>
-  </si>
-  <si>
-    <t>3421593</t>
-  </si>
-  <si>
-    <t>126223981</t>
-  </si>
-  <si>
-    <t>32416360</t>
-  </si>
-  <si>
-    <t>3421594</t>
-  </si>
-  <si>
-    <t>126224003</t>
-  </si>
-  <si>
-    <t>32416366</t>
-  </si>
-  <si>
-    <t>3421600</t>
-  </si>
-  <si>
-    <t>126224070</t>
-  </si>
-  <si>
-    <t>32416365</t>
-  </si>
-  <si>
-    <t>3421599</t>
-  </si>
-  <si>
-    <t>126224069</t>
-  </si>
-  <si>
-    <t>32416364</t>
-  </si>
-  <si>
-    <t>3421598</t>
-  </si>
-  <si>
-    <t>126224058</t>
-  </si>
-  <si>
-    <t>32416363</t>
-  </si>
-  <si>
-    <t>3421597</t>
-  </si>
-  <si>
-    <t>126224047</t>
-  </si>
-  <si>
-    <t>32416362</t>
-  </si>
-  <si>
-    <t>3421596</t>
-  </si>
-  <si>
-    <t>126224036</t>
-  </si>
-  <si>
-    <t>32416361</t>
-  </si>
-  <si>
-    <t>3421595</t>
-  </si>
-  <si>
-    <t>126224025</t>
-  </si>
-  <si>
-    <t>32416534</t>
-  </si>
-  <si>
-    <t>126226029</t>
-  </si>
-  <si>
-    <t>32416533</t>
-  </si>
-  <si>
-    <t>126226018</t>
-  </si>
-  <si>
-    <t>32416532</t>
-  </si>
-  <si>
-    <t>126226007</t>
-  </si>
-  <si>
-    <t>32416531</t>
-  </si>
-  <si>
-    <t>126225996</t>
-  </si>
-  <si>
-    <t>32416323</t>
-  </si>
-  <si>
-    <t>126223590</t>
-  </si>
-  <si>
-    <t>32416322</t>
-  </si>
-  <si>
-    <t>126223589</t>
-  </si>
-  <si>
-    <t>32416321</t>
-  </si>
-  <si>
-    <t>126223578</t>
-  </si>
-  <si>
-    <t>32416367</t>
-  </si>
-  <si>
-    <t>3421601</t>
-  </si>
-  <si>
-    <t>126224092</t>
-  </si>
-  <si>
-    <t>2022-07-07 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-07 23:13</t>
-  </si>
-  <si>
-    <t>3421947</t>
-  </si>
-  <si>
-    <t>3421952</t>
-  </si>
-  <si>
     <t>RT00002344</t>
+  </si>
+  <si>
+    <t>126255438</t>
+  </si>
+  <si>
+    <t>3424784</t>
+  </si>
+  <si>
+    <t>3424785</t>
+  </si>
+  <si>
+    <t>126255461</t>
+  </si>
+  <si>
+    <t>2022-07-10 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-10 23:13</t>
+  </si>
+  <si>
+    <t>3424915</t>
+  </si>
+  <si>
+    <t>3424916</t>
+  </si>
+  <si>
+    <t>126272691</t>
+  </si>
+  <si>
+    <t>126272716</t>
+  </si>
+  <si>
+    <t>126272738</t>
+  </si>
+  <si>
+    <t>126272750</t>
+  </si>
+  <si>
+    <t>126256941</t>
+  </si>
+  <si>
+    <t>126272196</t>
+  </si>
+  <si>
+    <t>126272820</t>
+  </si>
+  <si>
+    <t>126274307</t>
+  </si>
+  <si>
+    <t>32421456</t>
+  </si>
+  <si>
+    <t>3426690</t>
+  </si>
+  <si>
+    <t>126272705</t>
+  </si>
+  <si>
+    <t>32421457</t>
+  </si>
+  <si>
+    <t>3426691</t>
+  </si>
+  <si>
+    <t>126272727</t>
+  </si>
+  <si>
+    <t>32421458</t>
+  </si>
+  <si>
+    <t>3426692</t>
+  </si>
+  <si>
+    <t>126272749</t>
+  </si>
+  <si>
+    <t>32421464</t>
+  </si>
+  <si>
+    <t>3426698</t>
+  </si>
+  <si>
+    <t>126272819</t>
+  </si>
+  <si>
+    <t>32421463</t>
+  </si>
+  <si>
+    <t>3426697</t>
+  </si>
+  <si>
+    <t>126272808</t>
+  </si>
+  <si>
+    <t>32421462</t>
+  </si>
+  <si>
+    <t>3426696</t>
+  </si>
+  <si>
+    <t>126272794</t>
+  </si>
+  <si>
+    <t>32421461</t>
+  </si>
+  <si>
+    <t>3426695</t>
+  </si>
+  <si>
+    <t>126272783</t>
+  </si>
+  <si>
+    <t>32421460</t>
+  </si>
+  <si>
+    <t>3426694</t>
+  </si>
+  <si>
+    <t>126272772</t>
+  </si>
+  <si>
+    <t>32421459</t>
+  </si>
+  <si>
+    <t>3426693</t>
+  </si>
+  <si>
+    <t>126272761</t>
+  </si>
+  <si>
+    <t>32419677</t>
+  </si>
+  <si>
+    <t>126256985</t>
+  </si>
+  <si>
+    <t>32419676</t>
+  </si>
+  <si>
+    <t>126256974</t>
+  </si>
+  <si>
+    <t>32419675</t>
+  </si>
+  <si>
+    <t>126256963</t>
+  </si>
+  <si>
+    <t>32419674</t>
+  </si>
+  <si>
+    <t>126256952</t>
+  </si>
+  <si>
+    <t>32421410</t>
+  </si>
+  <si>
+    <t>126272222</t>
+  </si>
+  <si>
+    <t>32421409</t>
+  </si>
+  <si>
+    <t>126272211</t>
+  </si>
+  <si>
+    <t>32421408</t>
+  </si>
+  <si>
+    <t>126272200</t>
+  </si>
+  <si>
+    <t>32421465</t>
+  </si>
+  <si>
+    <t>3426699</t>
+  </si>
+  <si>
+    <t>126272831</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -973,128 +966,128 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1112,7 +1105,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1194,10 +1187,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1355,7 +1348,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1364,13 +1357,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1380,7 +1373,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1389,7 +1382,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1398,7 +1391,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1408,12 +1401,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1444,7 +1437,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1463,7 +1456,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1475,19 +1468,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1512,7 +1505,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1526,7 +1519,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1540,7 +1533,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1554,7 +1547,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1567,8 +1560,8 @@
       <c r="B6" t="s">
         <v>72</v>
       </c>
-      <c r="C6">
-        <v>126184475</v>
+      <c r="C6" t="s">
+        <v>116</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1581,8 +1574,8 @@
       <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7">
-        <v>126173651</v>
+      <c r="C7" t="s">
+        <v>117</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1596,7 +1589,7 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1610,7 +1603,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1621,7 +1614,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1629,15 +1622,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
@@ -1645,12 +1638,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1675,10 +1668,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -1791,21 +1784,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1813,8 +1806,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1833,78 +1826,78 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -1912,15 +1905,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1964,10 +1957,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2466,14 +2459,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -2481,13 +2474,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2527,10 +2520,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2554,7 +2547,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>161</v>
+        <v>108</v>
       </c>
       <c r="K2" t="s">
         <v>86</v>
@@ -2585,7 +2578,7 @@
         <v>90</v>
       </c>
       <c r="J3" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="K3" t="s">
         <v>86</v>
@@ -2956,13 +2949,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -2970,11 +2963,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2999,10 +2992,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3242,13 +3235,13 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -3256,8 +3249,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3270,7 +3263,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3278,20 +3271,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -3299,9 +3292,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,76 +3313,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3447,23 +3440,23 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3482,52 +3475,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>126184475</v>
+        <v>126275005</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C2">
-        <v>3417266</v>
+        <v>3426899</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C3">
-        <v>3417267</v>
+        <v>3426900</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C4">
-        <v>3417268</v>
+        <v>3426901</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C5">
-        <v>3417269</v>
+        <v>3426902</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3597,22 +3590,22 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,41 +3623,41 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>126173651</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3416137</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>153</v>
+      <c r="A2">
+        <v>126276873</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2">
+        <v>3427103</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3416138</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>155</v>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3">
+        <v>3427104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3416139</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>157</v>
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4">
+        <v>3427105</v>
+      </c>
+      <c r="D4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3740,6 +3733,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 13th July for Many to Many and Many to One and Agent Details
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="8"/>
+    <workbookView activeTab="7" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
-    <sheet name="Rate" sheetId="3" r:id="rId3"/>
-    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
-    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
-    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
-    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
-    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
-    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
-    <sheet name="CompareCharges" sheetId="10" r:id="rId10"/>
+    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
+    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
+    <sheet name="Rate" r:id="rId3" sheetId="3"/>
+    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
+    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
+    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
+    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
+    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
+    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
+    <sheet name="CompareCharges" r:id="rId10" sheetId="10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="163">
   <si>
     <t>FileName</t>
   </si>
@@ -256,271 +256,269 @@
     <t>$760.00</t>
   </si>
   <si>
+    <t>43 Minute(s)</t>
+  </si>
+  <si>
+    <t>228927</t>
+  </si>
+  <si>
+    <t>Total :US$160.00</t>
+  </si>
+  <si>
+    <t>US$160.00</t>
+  </si>
+  <si>
+    <t>2/0</t>
+  </si>
+  <si>
+    <t>Test company order 1</t>
+  </si>
+  <si>
+    <t>Test company order 1, 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
+  </si>
+  <si>
+    <t>PickUp instruction for Automation Testing</t>
+  </si>
+  <si>
+    <t>CDT</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER</t>
+  </si>
+  <si>
+    <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>ADD - ADDITIONAL STOP</t>
+  </si>
+  <si>
+    <t>$15.00</t>
+  </si>
+  <si>
+    <t>ADDITIONAL STOP</t>
+  </si>
+  <si>
+    <t>228540</t>
+  </si>
+  <si>
+    <t>$30.00</t>
+  </si>
+  <si>
+    <t>Base Rate</t>
+  </si>
+  <si>
+    <t>SAP - Saturday Pickup</t>
+  </si>
+  <si>
+    <t>Saturday Pickup</t>
+  </si>
+  <si>
+    <t>XML - Excess Mileage</t>
+  </si>
+  <si>
+    <t>$9.90</t>
+  </si>
+  <si>
+    <t>26 Mile(s)</t>
+  </si>
+  <si>
+    <t>126292109</t>
+  </si>
+  <si>
+    <t>126292121</t>
+  </si>
+  <si>
+    <t>126292143</t>
+  </si>
+  <si>
+    <t>126292165</t>
+  </si>
+  <si>
+    <t>126291711</t>
+  </si>
+  <si>
+    <t>126292235</t>
+  </si>
+  <si>
+    <t>126293748</t>
+  </si>
+  <si>
+    <t>32423519</t>
+  </si>
+  <si>
+    <t>3428753</t>
+  </si>
+  <si>
+    <t>126292110</t>
+  </si>
+  <si>
+    <t>32423520</t>
+  </si>
+  <si>
+    <t>3428754</t>
+  </si>
+  <si>
+    <t>126292132</t>
+  </si>
+  <si>
+    <t>32423521</t>
+  </si>
+  <si>
+    <t>3428755</t>
+  </si>
+  <si>
+    <t>126292154</t>
+  </si>
+  <si>
+    <t>32423527</t>
+  </si>
+  <si>
+    <t>3428761</t>
+  </si>
+  <si>
+    <t>126292224</t>
+  </si>
+  <si>
+    <t>32423526</t>
+  </si>
+  <si>
+    <t>3428760</t>
+  </si>
+  <si>
+    <t>126292213</t>
+  </si>
+  <si>
+    <t>32423525</t>
+  </si>
+  <si>
+    <t>3428759</t>
+  </si>
+  <si>
+    <t>126292202</t>
+  </si>
+  <si>
+    <t>32423524</t>
+  </si>
+  <si>
+    <t>3428758</t>
+  </si>
+  <si>
+    <t>126292198</t>
+  </si>
+  <si>
+    <t>32423523</t>
+  </si>
+  <si>
+    <t>3428757</t>
+  </si>
+  <si>
+    <t>126292187</t>
+  </si>
+  <si>
+    <t>32423522</t>
+  </si>
+  <si>
+    <t>3428756</t>
+  </si>
+  <si>
+    <t>126292176</t>
+  </si>
+  <si>
+    <t>32421668</t>
+  </si>
+  <si>
+    <t>126275049</t>
+  </si>
+  <si>
+    <t>32421667</t>
+  </si>
+  <si>
+    <t>126275038</t>
+  </si>
+  <si>
+    <t>32421666</t>
+  </si>
+  <si>
+    <t>126275027</t>
+  </si>
+  <si>
+    <t>32421665</t>
+  </si>
+  <si>
+    <t>126275016</t>
+  </si>
+  <si>
+    <t>32423483</t>
+  </si>
+  <si>
+    <t>3428717</t>
+  </si>
+  <si>
+    <t>126291744</t>
+  </si>
+  <si>
+    <t>32423482</t>
+  </si>
+  <si>
+    <t>3428716</t>
+  </si>
+  <si>
+    <t>126291733</t>
+  </si>
+  <si>
+    <t>32423481</t>
+  </si>
+  <si>
+    <t>3428715</t>
+  </si>
+  <si>
+    <t>126291722</t>
+  </si>
+  <si>
+    <t>32423528</t>
+  </si>
+  <si>
+    <t>3428762</t>
+  </si>
+  <si>
+    <t>126292246</t>
+  </si>
+  <si>
+    <t>2022-07-12 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-12 23:13</t>
+  </si>
+  <si>
+    <t>3429054</t>
+  </si>
+  <si>
+    <t>3429064</t>
+  </si>
+  <si>
+    <t>RT00002379</t>
+  </si>
+  <si>
+    <t>$185.00</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>43 Minute(s)</t>
-  </si>
-  <si>
-    <t>228927</t>
-  </si>
-  <si>
-    <t>Total :US$160.00</t>
-  </si>
-  <si>
-    <t>US$160.00</t>
-  </si>
-  <si>
-    <t>2/0</t>
-  </si>
-  <si>
-    <t>Test company order 1</t>
-  </si>
-  <si>
-    <t>Test company order 1, 3625 Willowbend Blvd., Suite 132, Chemistry Lab Room P058, HOUSTON, TX, 77056, USA</t>
-  </si>
-  <si>
-    <t>PickUp instruction for Automation Testing</t>
-  </si>
-  <si>
-    <t>CDT</t>
-  </si>
-  <si>
-    <t>ST FRANCIS MEDICAL CENTER</t>
-  </si>
-  <si>
-    <t>ST FRANCIS MEDICAL CENTER, 23900 KATY FWY, Chemistry Laboratory, HOUSTON, TX, 77054, USA</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>ADD - ADDITIONAL STOP</t>
-  </si>
-  <si>
-    <t>$15.00</t>
-  </si>
-  <si>
-    <t>ADDITIONAL STOP</t>
-  </si>
-  <si>
-    <t>228540</t>
-  </si>
-  <si>
-    <t>$30.00</t>
-  </si>
-  <si>
-    <t>Base Rate</t>
-  </si>
-  <si>
-    <t>SAP - Saturday Pickup</t>
-  </si>
-  <si>
-    <t>Saturday Pickup</t>
-  </si>
-  <si>
-    <t>XML - Excess Mileage</t>
-  </si>
-  <si>
-    <t>$9.90</t>
-  </si>
-  <si>
-    <t>26 Mile(s)</t>
-  </si>
-  <si>
-    <t>3419933</t>
-  </si>
-  <si>
-    <t>RT00002344</t>
-  </si>
-  <si>
-    <t>126255438</t>
-  </si>
-  <si>
-    <t>3424784</t>
-  </si>
-  <si>
-    <t>3424785</t>
-  </si>
-  <si>
-    <t>126255461</t>
-  </si>
-  <si>
-    <t>2022-07-10 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-10 23:13</t>
-  </si>
-  <si>
-    <t>3424915</t>
-  </si>
-  <si>
-    <t>3424916</t>
-  </si>
-  <si>
-    <t>126272691</t>
-  </si>
-  <si>
-    <t>126272716</t>
-  </si>
-  <si>
-    <t>126272738</t>
-  </si>
-  <si>
-    <t>126272750</t>
-  </si>
-  <si>
-    <t>126256941</t>
-  </si>
-  <si>
-    <t>126272196</t>
-  </si>
-  <si>
-    <t>126272820</t>
-  </si>
-  <si>
-    <t>126274307</t>
-  </si>
-  <si>
-    <t>32421456</t>
-  </si>
-  <si>
-    <t>3426690</t>
-  </si>
-  <si>
-    <t>126272705</t>
-  </si>
-  <si>
-    <t>32421457</t>
-  </si>
-  <si>
-    <t>3426691</t>
-  </si>
-  <si>
-    <t>126272727</t>
-  </si>
-  <si>
-    <t>32421458</t>
-  </si>
-  <si>
-    <t>3426692</t>
-  </si>
-  <si>
-    <t>126272749</t>
-  </si>
-  <si>
-    <t>32421464</t>
-  </si>
-  <si>
-    <t>3426698</t>
-  </si>
-  <si>
-    <t>126272819</t>
-  </si>
-  <si>
-    <t>32421463</t>
-  </si>
-  <si>
-    <t>3426697</t>
-  </si>
-  <si>
-    <t>126272808</t>
-  </si>
-  <si>
-    <t>32421462</t>
-  </si>
-  <si>
-    <t>3426696</t>
-  </si>
-  <si>
-    <t>126272794</t>
-  </si>
-  <si>
-    <t>32421461</t>
-  </si>
-  <si>
-    <t>3426695</t>
-  </si>
-  <si>
-    <t>126272783</t>
-  </si>
-  <si>
-    <t>32421460</t>
-  </si>
-  <si>
-    <t>3426694</t>
-  </si>
-  <si>
-    <t>126272772</t>
-  </si>
-  <si>
-    <t>32421459</t>
-  </si>
-  <si>
-    <t>3426693</t>
-  </si>
-  <si>
-    <t>126272761</t>
-  </si>
-  <si>
-    <t>32419677</t>
-  </si>
-  <si>
-    <t>126256985</t>
-  </si>
-  <si>
-    <t>32419676</t>
-  </si>
-  <si>
-    <t>126256974</t>
-  </si>
-  <si>
-    <t>32419675</t>
-  </si>
-  <si>
-    <t>126256963</t>
-  </si>
-  <si>
-    <t>32419674</t>
-  </si>
-  <si>
-    <t>126256952</t>
-  </si>
-  <si>
-    <t>32421410</t>
-  </si>
-  <si>
-    <t>126272222</t>
-  </si>
-  <si>
-    <t>32421409</t>
-  </si>
-  <si>
-    <t>126272211</t>
-  </si>
-  <si>
-    <t>32421408</t>
-  </si>
-  <si>
-    <t>126272200</t>
-  </si>
-  <si>
-    <t>32421465</t>
-  </si>
-  <si>
-    <t>3426699</t>
-  </si>
-  <si>
-    <t>126272831</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -966,128 +964,128 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1105,7 +1103,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1187,10 +1185,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1348,7 +1346,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1357,13 +1355,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1373,7 +1371,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1382,7 +1380,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1391,7 +1389,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1401,12 +1399,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1437,7 +1435,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1456,7 +1454,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1468,19 +1466,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,7 +1503,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1519,7 +1517,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1533,7 +1531,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1547,7 +1545,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1560,8 +1558,8 @@
       <c r="B6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
-        <v>116</v>
+      <c r="C6">
+        <v>126295465</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1575,7 +1573,7 @@
         <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1589,7 +1587,7 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1603,7 +1601,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1614,7 +1612,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1622,15 +1620,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
@@ -1638,12 +1636,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="6" max="8" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1668,10 +1666,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -1683,7 +1681,7 @@
         <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1784,21 +1782,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1806,8 +1804,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,78 +1824,78 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
         <v>114</v>
       </c>
-      <c r="B4" t="s">
-        <v>126</v>
-      </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -1905,15 +1903,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1957,10 +1955,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -1969,25 +1967,25 @@
         <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
         <v>58</v>
       </c>
       <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>80</v>
-      </c>
-      <c r="I2" t="s">
-        <v>81</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s">
         <v>21</v>
@@ -2023,19 +2021,19 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
         <v>91</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>92</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
       </c>
       <c r="F4" t="s">
         <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2051,16 +2049,16 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
         <v>95</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
       </c>
       <c r="F5" t="s">
         <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2073,19 +2071,19 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
         <v>97</v>
-      </c>
-      <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>98</v>
       </c>
       <c r="F6" t="s">
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2098,19 +2096,19 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
         <v>99</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>100</v>
-      </c>
-      <c r="E7" t="s">
-        <v>101</v>
       </c>
       <c r="F7" t="s">
         <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2459,14 +2457,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -2474,13 +2472,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2520,25 +2518,25 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
         <v>82</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>83</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>84</v>
-      </c>
-      <c r="G2" t="s">
-        <v>85</v>
       </c>
       <c r="H2" t="s">
         <v>37</v>
@@ -2547,10 +2545,10 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2563,25 +2561,25 @@
         <v>59</v>
       </c>
       <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s">
         <v>87</v>
-      </c>
-      <c r="F3" t="s">
-        <v>88</v>
       </c>
       <c r="G3" t="s">
         <v>60</v>
       </c>
       <c r="H3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
         <v>89</v>
       </c>
-      <c r="I3" t="s">
-        <v>90</v>
-      </c>
       <c r="J3" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2949,13 +2947,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -2963,11 +2961,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2992,10 +2990,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3235,13 +3233,13 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -3249,8 +3247,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,7 +3261,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>157</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3271,20 +3269,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -3292,9 +3290,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3313,76 +3311,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3440,23 +3438,23 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3475,52 +3473,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>126275005</v>
+        <v>126295465</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C2">
-        <v>3426899</v>
+        <v>3429060</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C3">
-        <v>3426900</v>
+        <v>3429061</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C4">
-        <v>3426901</v>
+        <v>3429062</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C5">
-        <v>3426902</v>
+        <v>3429063</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3590,22 +3588,22 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,41 +3621,41 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>126276873</v>
+      <c r="A2" t="s">
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2">
-        <v>3427103</v>
+        <v>143</v>
+      </c>
+      <c r="C2" t="s">
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3">
-        <v>3427104</v>
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4">
-        <v>3427105</v>
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3733,6 +3731,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 14th July 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="7" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
-    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
-    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
-    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
-    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
-    <sheet name="CompareCharges" r:id="rId10" sheetId="10"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
+    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
+    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
+    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
+    <sheet name="CompareCharges" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="154">
   <si>
     <t>FileName</t>
   </si>
@@ -328,181 +328,154 @@
     <t>26 Mile(s)</t>
   </si>
   <si>
-    <t>126292109</t>
-  </si>
-  <si>
-    <t>126292121</t>
-  </si>
-  <si>
-    <t>126292143</t>
-  </si>
-  <si>
-    <t>126292165</t>
-  </si>
-  <si>
-    <t>126291711</t>
-  </si>
-  <si>
-    <t>126292235</t>
-  </si>
-  <si>
-    <t>126293748</t>
-  </si>
-  <si>
-    <t>32423519</t>
-  </si>
-  <si>
-    <t>3428753</t>
-  </si>
-  <si>
-    <t>126292110</t>
-  </si>
-  <si>
-    <t>32423520</t>
-  </si>
-  <si>
-    <t>3428754</t>
-  </si>
-  <si>
-    <t>126292132</t>
-  </si>
-  <si>
-    <t>32423521</t>
-  </si>
-  <si>
-    <t>3428755</t>
-  </si>
-  <si>
-    <t>126292154</t>
-  </si>
-  <si>
-    <t>32423527</t>
-  </si>
-  <si>
-    <t>3428761</t>
-  </si>
-  <si>
-    <t>126292224</t>
-  </si>
-  <si>
-    <t>32423526</t>
-  </si>
-  <si>
-    <t>3428760</t>
-  </si>
-  <si>
-    <t>126292213</t>
-  </si>
-  <si>
-    <t>32423525</t>
-  </si>
-  <si>
-    <t>3428759</t>
-  </si>
-  <si>
-    <t>126292202</t>
-  </si>
-  <si>
-    <t>32423524</t>
-  </si>
-  <si>
-    <t>3428758</t>
-  </si>
-  <si>
-    <t>126292198</t>
-  </si>
-  <si>
-    <t>32423523</t>
-  </si>
-  <si>
-    <t>3428757</t>
-  </si>
-  <si>
-    <t>126292187</t>
-  </si>
-  <si>
-    <t>32423522</t>
-  </si>
-  <si>
-    <t>3428756</t>
-  </si>
-  <si>
-    <t>126292176</t>
-  </si>
-  <si>
-    <t>32421668</t>
-  </si>
-  <si>
-    <t>126275049</t>
-  </si>
-  <si>
-    <t>32421667</t>
-  </si>
-  <si>
-    <t>126275038</t>
-  </si>
-  <si>
-    <t>32421666</t>
-  </si>
-  <si>
-    <t>126275027</t>
-  </si>
-  <si>
-    <t>32421665</t>
-  </si>
-  <si>
-    <t>126275016</t>
-  </si>
-  <si>
-    <t>32423483</t>
-  </si>
-  <si>
-    <t>3428717</t>
-  </si>
-  <si>
-    <t>126291744</t>
-  </si>
-  <si>
-    <t>32423482</t>
-  </si>
-  <si>
-    <t>3428716</t>
-  </si>
-  <si>
-    <t>126291733</t>
-  </si>
-  <si>
-    <t>32423481</t>
-  </si>
-  <si>
-    <t>3428715</t>
-  </si>
-  <si>
-    <t>126291722</t>
-  </si>
-  <si>
-    <t>32423528</t>
-  </si>
-  <si>
-    <t>3428762</t>
-  </si>
-  <si>
-    <t>126292246</t>
-  </si>
-  <si>
-    <t>2022-07-12 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-12 23:13</t>
-  </si>
-  <si>
-    <t>3429054</t>
-  </si>
-  <si>
-    <t>3429064</t>
-  </si>
-  <si>
-    <t>RT00002379</t>
+    <t>126310421</t>
+  </si>
+  <si>
+    <t>126310443</t>
+  </si>
+  <si>
+    <t>126310465</t>
+  </si>
+  <si>
+    <t>126310487</t>
+  </si>
+  <si>
+    <t>126310557</t>
+  </si>
+  <si>
+    <t>126311635</t>
+  </si>
+  <si>
+    <t>32425476</t>
+  </si>
+  <si>
+    <t>3430710</t>
+  </si>
+  <si>
+    <t>126310432</t>
+  </si>
+  <si>
+    <t>32425477</t>
+  </si>
+  <si>
+    <t>3430711</t>
+  </si>
+  <si>
+    <t>126310454</t>
+  </si>
+  <si>
+    <t>32425478</t>
+  </si>
+  <si>
+    <t>126310476</t>
+  </si>
+  <si>
+    <t>32425484</t>
+  </si>
+  <si>
+    <t>126310546</t>
+  </si>
+  <si>
+    <t>32425483</t>
+  </si>
+  <si>
+    <t>126310535</t>
+  </si>
+  <si>
+    <t>32425482</t>
+  </si>
+  <si>
+    <t>126310524</t>
+  </si>
+  <si>
+    <t>32425481</t>
+  </si>
+  <si>
+    <t>126310513</t>
+  </si>
+  <si>
+    <t>32425480</t>
+  </si>
+  <si>
+    <t>126310502</t>
+  </si>
+  <si>
+    <t>32425479</t>
+  </si>
+  <si>
+    <t>126310498</t>
+  </si>
+  <si>
+    <t>32423829</t>
+  </si>
+  <si>
+    <t>126295502</t>
+  </si>
+  <si>
+    <t>32423828</t>
+  </si>
+  <si>
+    <t>126295498</t>
+  </si>
+  <si>
+    <t>32423827</t>
+  </si>
+  <si>
+    <t>126295487</t>
+  </si>
+  <si>
+    <t>32423826</t>
+  </si>
+  <si>
+    <t>126295476</t>
+  </si>
+  <si>
+    <t>32425438</t>
+  </si>
+  <si>
+    <t>126310188</t>
+  </si>
+  <si>
+    <t>32425437</t>
+  </si>
+  <si>
+    <t>126310177</t>
+  </si>
+  <si>
+    <t>32425436</t>
+  </si>
+  <si>
+    <t>126310166</t>
+  </si>
+  <si>
+    <t>32425485</t>
+  </si>
+  <si>
+    <t>3430719</t>
+  </si>
+  <si>
+    <t>126310568</t>
+  </si>
+  <si>
+    <t>3430874</t>
+  </si>
+  <si>
+    <t>2022-07-11 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-11 23:13</t>
+  </si>
+  <si>
+    <t>126272749</t>
+  </si>
+  <si>
+    <t>3426692</t>
+  </si>
+  <si>
+    <t>3431094</t>
+  </si>
+  <si>
+    <t>3431099</t>
   </si>
   <si>
     <t>$185.00</t>
@@ -511,14 +484,13 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>RT00002407</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -964,128 +936,128 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1103,7 +1075,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1185,10 +1157,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1346,7 +1318,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1355,13 +1327,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1371,7 +1343,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1380,7 +1352,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1389,7 +1361,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1399,12 +1371,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1435,7 +1407,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1454,7 +1426,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1466,8 +1438,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
@@ -1475,10 +1447,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1559,7 +1531,7 @@
         <v>72</v>
       </c>
       <c r="C6">
-        <v>126295465</v>
+        <v>126298503</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1572,8 +1544,8 @@
       <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7" t="s">
-        <v>105</v>
+      <c r="C7">
+        <v>126296587</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1587,7 +1559,7 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1601,7 +1573,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1612,7 +1584,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1620,15 +1592,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
@@ -1636,12 +1608,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1666,10 +1638,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -1678,10 +1650,10 @@
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1782,30 +1754,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1827,13 +1799,13 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
         <v>108</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>109</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,13 +1813,13 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
         <v>111</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1855,47 +1827,47 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4">
+        <v>3426692</v>
+      </c>
+      <c r="D4" t="s">
         <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -1903,15 +1875,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1958,7 +1930,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2457,14 +2429,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -2472,13 +2444,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2521,7 +2493,7 @@
         <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2545,7 +2517,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -2576,7 +2548,7 @@
         <v>89</v>
       </c>
       <c r="J3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -2947,13 +2919,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -2961,11 +2933,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2990,10 +2962,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3233,13 +3205,13 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -3247,8 +3219,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3261,7 +3233,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3269,30 +3241,30 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3310,77 +3282,77 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>104</v>
+      <c r="A2">
+        <v>126298318</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="C2">
+        <v>3429379</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" t="s">
-        <v>121</v>
+        <v>117</v>
+      </c>
+      <c r="C3">
+        <v>3429380</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" t="s">
-        <v>124</v>
+        <v>119</v>
+      </c>
+      <c r="C4">
+        <v>3429381</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="C5">
+        <v>3429382</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+      <c r="C6">
+        <v>3429383</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
+        <v>125</v>
+      </c>
+      <c r="C7">
+        <v>3429384</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3438,23 +3410,23 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3472,57 +3444,204 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>126278361</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3429379</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3429380</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3429381</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3429382</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
+        <v>3429383</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
+        <v>3429384</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>126295465</v>
+        <v>126313237</v>
       </c>
       <c r="B2" t="s">
         <v>135</v>
       </c>
       <c r="C2">
-        <v>3429060</v>
+        <v>3431024</v>
       </c>
       <c r="D2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>137</v>
       </c>
       <c r="C3">
-        <v>3429061</v>
+        <v>3431025</v>
       </c>
       <c r="D3" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>139</v>
       </c>
       <c r="C4">
-        <v>3429062</v>
+        <v>3431026</v>
       </c>
       <c r="D4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5">
-        <v>3429063</v>
-      </c>
-      <c r="D5" t="s">
-        <v>142</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3588,149 +3707,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 18th July 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="8" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
-    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
-    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
-    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
-    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
-    <sheet name="CompareCharges" r:id="rId10" sheetId="10"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
+    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
+    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
+    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
+    <sheet name="CompareCharges" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="168">
   <si>
     <t>FileName</t>
   </si>
@@ -328,33 +328,6 @@
     <t>26 Mile(s)</t>
   </si>
   <si>
-    <t>126310443</t>
-  </si>
-  <si>
-    <t>3430711</t>
-  </si>
-  <si>
-    <t>3430874</t>
-  </si>
-  <si>
-    <t>2022-07-11 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-11 23:13</t>
-  </si>
-  <si>
-    <t>126272749</t>
-  </si>
-  <si>
-    <t>3426692</t>
-  </si>
-  <si>
-    <t>3431094</t>
-  </si>
-  <si>
-    <t>3431099</t>
-  </si>
-  <si>
     <t>$185.00</t>
   </si>
   <si>
@@ -364,191 +337,202 @@
     <t>RT00002407</t>
   </si>
   <si>
-    <t>126326262</t>
-  </si>
-  <si>
-    <t>126326284</t>
-  </si>
-  <si>
-    <t>126326309</t>
-  </si>
-  <si>
-    <t>126326321</t>
-  </si>
-  <si>
-    <t>126326398</t>
-  </si>
-  <si>
-    <t>126326446</t>
-  </si>
-  <si>
-    <t>126326480</t>
-  </si>
-  <si>
-    <t>126326228</t>
-  </si>
-  <si>
-    <t>32427114</t>
-  </si>
-  <si>
-    <t>3432348</t>
-  </si>
-  <si>
-    <t>126326273</t>
-  </si>
-  <si>
-    <t>32427115</t>
-  </si>
-  <si>
-    <t>3432349</t>
-  </si>
-  <si>
-    <t>126326295</t>
-  </si>
-  <si>
-    <t>32427116</t>
-  </si>
-  <si>
-    <t>3432350</t>
-  </si>
-  <si>
-    <t>126326310</t>
-  </si>
-  <si>
-    <t>32427122</t>
-  </si>
-  <si>
-    <t>3432356</t>
-  </si>
-  <si>
-    <t>126326387</t>
-  </si>
-  <si>
-    <t>32427121</t>
-  </si>
-  <si>
-    <t>3432355</t>
-  </si>
-  <si>
-    <t>126326376</t>
-  </si>
-  <si>
-    <t>32427120</t>
-  </si>
-  <si>
-    <t>3432354</t>
-  </si>
-  <si>
-    <t>126326365</t>
-  </si>
-  <si>
-    <t>32427119</t>
-  </si>
-  <si>
-    <t>3432353</t>
-  </si>
-  <si>
-    <t>126326354</t>
-  </si>
-  <si>
-    <t>32427118</t>
-  </si>
-  <si>
-    <t>3432352</t>
-  </si>
-  <si>
-    <t>126326343</t>
-  </si>
-  <si>
-    <t>32427117</t>
-  </si>
-  <si>
-    <t>3432351</t>
-  </si>
-  <si>
-    <t>126326332</t>
-  </si>
-  <si>
-    <t>32427126</t>
-  </si>
-  <si>
-    <t>3432360</t>
-  </si>
-  <si>
-    <t>126326435</t>
-  </si>
-  <si>
-    <t>32427125</t>
-  </si>
-  <si>
-    <t>3432359</t>
-  </si>
-  <si>
-    <t>126326424</t>
-  </si>
-  <si>
-    <t>32427124</t>
-  </si>
-  <si>
-    <t>3432358</t>
-  </si>
-  <si>
-    <t>126326413</t>
-  </si>
-  <si>
-    <t>32427123</t>
-  </si>
-  <si>
-    <t>3432357</t>
-  </si>
-  <si>
-    <t>126326402</t>
-  </si>
-  <si>
-    <t>32427129</t>
-  </si>
-  <si>
-    <t>126326479</t>
-  </si>
-  <si>
-    <t>32427128</t>
-  </si>
-  <si>
-    <t>126326468</t>
-  </si>
-  <si>
-    <t>32427127</t>
-  </si>
-  <si>
-    <t>126326457</t>
-  </si>
-  <si>
-    <t>32427130</t>
-  </si>
-  <si>
-    <t>3432364</t>
-  </si>
-  <si>
-    <t>126326491</t>
-  </si>
-  <si>
-    <t>2022-07-14 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-14 23:13</t>
-  </si>
-  <si>
-    <t>3432745</t>
-  </si>
-  <si>
-    <t>3432750</t>
+    <t>126354788</t>
+  </si>
+  <si>
+    <t>126354803</t>
+  </si>
+  <si>
+    <t>126354825</t>
+  </si>
+  <si>
+    <t>126354847</t>
+  </si>
+  <si>
+    <t>126348936</t>
+  </si>
+  <si>
+    <t>126354685</t>
+  </si>
+  <si>
+    <t>126354917</t>
+  </si>
+  <si>
+    <t>126355877</t>
+  </si>
+  <si>
+    <t>32430000</t>
+  </si>
+  <si>
+    <t>3435234</t>
+  </si>
+  <si>
+    <t>126354799</t>
+  </si>
+  <si>
+    <t>32430001</t>
+  </si>
+  <si>
+    <t>3435235</t>
+  </si>
+  <si>
+    <t>126354814</t>
+  </si>
+  <si>
+    <t>32430002</t>
+  </si>
+  <si>
+    <t>3435236</t>
+  </si>
+  <si>
+    <t>126354836</t>
+  </si>
+  <si>
+    <t>32430008</t>
+  </si>
+  <si>
+    <t>3435242</t>
+  </si>
+  <si>
+    <t>126354906</t>
+  </si>
+  <si>
+    <t>32430007</t>
+  </si>
+  <si>
+    <t>3435241</t>
+  </si>
+  <si>
+    <t>126354892</t>
+  </si>
+  <si>
+    <t>32430006</t>
+  </si>
+  <si>
+    <t>3435240</t>
+  </si>
+  <si>
+    <t>126354881</t>
+  </si>
+  <si>
+    <t>32430005</t>
+  </si>
+  <si>
+    <t>3435239</t>
+  </si>
+  <si>
+    <t>126354870</t>
+  </si>
+  <si>
+    <t>32430004</t>
+  </si>
+  <si>
+    <t>3435238</t>
+  </si>
+  <si>
+    <t>126354869</t>
+  </si>
+  <si>
+    <t>32430003</t>
+  </si>
+  <si>
+    <t>3435237</t>
+  </si>
+  <si>
+    <t>126354858</t>
+  </si>
+  <si>
+    <t>32429390</t>
+  </si>
+  <si>
+    <t>3434624</t>
+  </si>
+  <si>
+    <t>126348970</t>
+  </si>
+  <si>
+    <t>32429389</t>
+  </si>
+  <si>
+    <t>3434623</t>
+  </si>
+  <si>
+    <t>126348969</t>
+  </si>
+  <si>
+    <t>32429388</t>
+  </si>
+  <si>
+    <t>3434622</t>
+  </si>
+  <si>
+    <t>126348958</t>
+  </si>
+  <si>
+    <t>32429387</t>
+  </si>
+  <si>
+    <t>3434621</t>
+  </si>
+  <si>
+    <t>126348947</t>
+  </si>
+  <si>
+    <t>32429988</t>
+  </si>
+  <si>
+    <t>3435222</t>
+  </si>
+  <si>
+    <t>126354711</t>
+  </si>
+  <si>
+    <t>32429987</t>
+  </si>
+  <si>
+    <t>3435221</t>
+  </si>
+  <si>
+    <t>126354700</t>
+  </si>
+  <si>
+    <t>32429986</t>
+  </si>
+  <si>
+    <t>3435220</t>
+  </si>
+  <si>
+    <t>126354696</t>
+  </si>
+  <si>
+    <t>32430009</t>
+  </si>
+  <si>
+    <t>3435243</t>
+  </si>
+  <si>
+    <t>126354928</t>
+  </si>
+  <si>
+    <t>2022-07-17 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-17 23:13</t>
+  </si>
+  <si>
+    <t>3435368</t>
+  </si>
+  <si>
+    <t>3435370</t>
+  </si>
+  <si>
+    <t>Charges on TC ACK stage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -994,128 +978,128 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1133,7 +1117,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1215,10 +1199,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1376,7 +1360,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1385,13 +1369,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1401,7 +1385,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1410,7 +1394,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1419,7 +1403,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1429,12 +1413,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1465,7 +1449,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1484,7 +1468,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1496,8 +1480,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
@@ -1505,10 +1489,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1533,7 +1517,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1547,7 +1531,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1561,7 +1545,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1575,7 +1559,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1589,7 +1573,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1603,7 +1587,7 @@
         <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1617,7 +1601,7 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1631,7 +1615,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1642,7 +1626,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1650,31 +1634,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="6" max="8" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -1693,140 +1677,156 @@
       <c r="F1" s="13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G1" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3430874</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
+      <c r="G14" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
@@ -1834,8 +1834,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1854,78 +1854,78 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
         <v>113</v>
       </c>
-      <c r="B2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" t="s">
-        <v>122</v>
-      </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -1933,15 +1933,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1985,10 +1985,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2487,14 +2487,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -2502,13 +2502,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2548,10 +2548,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2575,7 +2575,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -2606,7 +2606,7 @@
         <v>89</v>
       </c>
       <c r="J3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -2977,13 +2977,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -2991,11 +2991,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3020,10 +3020,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3263,13 +3263,13 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -3277,8 +3277,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3291,7 +3291,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3299,20 +3299,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C7"/>
@@ -3320,9 +3320,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,76 +3341,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3468,14 +3468,14 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -3483,8 +3483,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3502,53 +3502,53 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>117</v>
+      <c r="A2" t="s">
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3618,22 +3618,22 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3651,41 +3651,41 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>126327959</v>
+      <c r="A2" t="s">
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2">
-        <v>3432531</v>
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3">
-        <v>3432532</v>
+        <v>154</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4">
-        <v>3432533</v>
+        <v>157</v>
+      </c>
+      <c r="C4" t="s">
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3761,6 +3761,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 19th july 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="231">
   <si>
     <t>FileName</t>
   </si>
@@ -1884,10 +1884,10 @@
       <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>102</v>
       </c>
       <c r="G2" t="s">

</xml_diff>

<commit_message>
Changes of exception handling
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="166">
   <si>
     <t>FileName</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t>AOF - Agent Order Fee</t>
+  </si>
+  <si>
+    <t>$185.00</t>
   </si>
 </sst>
 </file>
@@ -1715,8 +1718,8 @@
       <c r="D2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="16">
-        <v>185</v>
+      <c r="E2" t="s">
+        <v>165</v>
       </c>
       <c r="F2" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Changes of 20th July 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="229">
   <si>
     <t>FileName</t>
   </si>
@@ -521,6 +521,195 @@
   </si>
   <si>
     <t>$185.00</t>
+  </si>
+  <si>
+    <t>126409345</t>
+  </si>
+  <si>
+    <t>126409367</t>
+  </si>
+  <si>
+    <t>126409389</t>
+  </si>
+  <si>
+    <t>126409404</t>
+  </si>
+  <si>
+    <t>126411753</t>
+  </si>
+  <si>
+    <t>126409068</t>
+  </si>
+  <si>
+    <t>126409471</t>
+  </si>
+  <si>
+    <t>126411029</t>
+  </si>
+  <si>
+    <t>32435724</t>
+  </si>
+  <si>
+    <t>3440958</t>
+  </si>
+  <si>
+    <t>126409356</t>
+  </si>
+  <si>
+    <t>32435725</t>
+  </si>
+  <si>
+    <t>3440959</t>
+  </si>
+  <si>
+    <t>126409378</t>
+  </si>
+  <si>
+    <t>32435726</t>
+  </si>
+  <si>
+    <t>3440960</t>
+  </si>
+  <si>
+    <t>126409390</t>
+  </si>
+  <si>
+    <t>32435732</t>
+  </si>
+  <si>
+    <t>3440966</t>
+  </si>
+  <si>
+    <t>126409460</t>
+  </si>
+  <si>
+    <t>32435731</t>
+  </si>
+  <si>
+    <t>3440965</t>
+  </si>
+  <si>
+    <t>126409459</t>
+  </si>
+  <si>
+    <t>32435730</t>
+  </si>
+  <si>
+    <t>3440964</t>
+  </si>
+  <si>
+    <t>126409448</t>
+  </si>
+  <si>
+    <t>32435729</t>
+  </si>
+  <si>
+    <t>3440963</t>
+  </si>
+  <si>
+    <t>126409437</t>
+  </si>
+  <si>
+    <t>32435728</t>
+  </si>
+  <si>
+    <t>3440962</t>
+  </si>
+  <si>
+    <t>126409426</t>
+  </si>
+  <si>
+    <t>32435727</t>
+  </si>
+  <si>
+    <t>3440961</t>
+  </si>
+  <si>
+    <t>126409415</t>
+  </si>
+  <si>
+    <t>32435954</t>
+  </si>
+  <si>
+    <t>3441188</t>
+  </si>
+  <si>
+    <t>126411797</t>
+  </si>
+  <si>
+    <t>32435953</t>
+  </si>
+  <si>
+    <t>3441187</t>
+  </si>
+  <si>
+    <t>126411786</t>
+  </si>
+  <si>
+    <t>32435952</t>
+  </si>
+  <si>
+    <t>3441186</t>
+  </si>
+  <si>
+    <t>126411775</t>
+  </si>
+  <si>
+    <t>32435951</t>
+  </si>
+  <si>
+    <t>3441185</t>
+  </si>
+  <si>
+    <t>126411764</t>
+  </si>
+  <si>
+    <t>32435700</t>
+  </si>
+  <si>
+    <t>3440934</t>
+  </si>
+  <si>
+    <t>126409091</t>
+  </si>
+  <si>
+    <t>32435699</t>
+  </si>
+  <si>
+    <t>3440933</t>
+  </si>
+  <si>
+    <t>126409080</t>
+  </si>
+  <si>
+    <t>32435698</t>
+  </si>
+  <si>
+    <t>3440932</t>
+  </si>
+  <si>
+    <t>126409079</t>
+  </si>
+  <si>
+    <t>32435733</t>
+  </si>
+  <si>
+    <t>3440967</t>
+  </si>
+  <si>
+    <t>126409482</t>
+  </si>
+  <si>
+    <t>2022-07-19 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-19 23:13</t>
+  </si>
+  <si>
+    <t>3441269</t>
+  </si>
+  <si>
+    <t>3441274</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1721,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1546,7 +1735,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1559,8 +1748,8 @@
       <c r="B4" t="s">
         <v>70</v>
       </c>
-      <c r="C4">
-        <v>126347825</v>
+      <c r="C4" t="s">
+        <v>168</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1574,7 +1763,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>169</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1587,8 +1776,8 @@
       <c r="B6" t="s">
         <v>72</v>
       </c>
-      <c r="C6">
-        <v>126358144</v>
+      <c r="C6" t="s">
+        <v>170</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1601,8 +1790,8 @@
       <c r="B7" t="s">
         <v>73</v>
       </c>
-      <c r="C7">
-        <v>126394209</v>
+      <c r="C7" t="s">
+        <v>171</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1616,7 +1805,7 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1630,7 +1819,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>173</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1707,7 +1896,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="B2" s="2">
         <v>3430874</v>
@@ -1910,63 +2099,63 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>126347825</v>
-      </c>
-      <c r="B4">
-        <v>32432961</v>
-      </c>
-      <c r="C4">
-        <v>3434537</v>
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>222</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>223</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>173</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2041,10 +2230,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2604,10 +2793,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2631,7 +2820,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>158</v>
+        <v>225</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -2662,7 +2851,7 @@
         <v>89</v>
       </c>
       <c r="J3" t="s">
-        <v>159</v>
+        <v>226</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -3076,10 +3265,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3347,7 +3536,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>227</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3355,7 +3544,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
@@ -3397,76 +3586,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>199</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3558,53 +3747,53 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>126358144</v>
+      <c r="A2" t="s">
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2">
-        <v>3435561</v>
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
+        <v>202</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3">
-        <v>3435562</v>
+        <v>204</v>
+      </c>
+      <c r="C3" t="s">
+        <v>205</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4">
-        <v>3435563</v>
+        <v>207</v>
+      </c>
+      <c r="C4" t="s">
+        <v>208</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C5">
-        <v>3435564</v>
+        <v>210</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,41 +3896,41 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>126394209</v>
+      <c r="A2" t="s">
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2">
-        <v>3439289</v>
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3">
-        <v>3439290</v>
+        <v>216</v>
+      </c>
+      <c r="C3" t="s">
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4">
-        <v>3439291</v>
+        <v>219</v>
+      </c>
+      <c r="C4" t="s">
+        <v>220</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes of 21st july 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="9" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="173">
   <si>
     <t>FileName</t>
   </si>
@@ -337,388 +337,218 @@
     <t>Charges on TC ACK stage</t>
   </si>
   <si>
-    <t>126383359</t>
-  </si>
-  <si>
-    <t>126383371</t>
-  </si>
-  <si>
-    <t>126383418</t>
-  </si>
-  <si>
-    <t>126383485</t>
-  </si>
-  <si>
-    <t>126391002</t>
-  </si>
-  <si>
-    <t>32432959</t>
-  </si>
-  <si>
-    <t>3438193</t>
-  </si>
-  <si>
-    <t>126383360</t>
-  </si>
-  <si>
-    <t>32432960</t>
-  </si>
-  <si>
-    <t>3438194</t>
-  </si>
-  <si>
-    <t>126383382</t>
-  </si>
-  <si>
-    <t>3438195</t>
-  </si>
-  <si>
-    <t>126383407</t>
-  </si>
-  <si>
-    <t>32432967</t>
-  </si>
-  <si>
-    <t>3438201</t>
-  </si>
-  <si>
-    <t>126383474</t>
-  </si>
-  <si>
-    <t>32432966</t>
-  </si>
-  <si>
-    <t>3438200</t>
-  </si>
-  <si>
-    <t>126383463</t>
-  </si>
-  <si>
-    <t>32432965</t>
-  </si>
-  <si>
-    <t>3438199</t>
-  </si>
-  <si>
-    <t>126383452</t>
-  </si>
-  <si>
-    <t>32432964</t>
-  </si>
-  <si>
-    <t>3438198</t>
-  </si>
-  <si>
-    <t>126383441</t>
-  </si>
-  <si>
-    <t>32432963</t>
-  </si>
-  <si>
-    <t>3438197</t>
-  </si>
-  <si>
-    <t>126383430</t>
-  </si>
-  <si>
-    <t>32432962</t>
-  </si>
-  <si>
-    <t>3438196</t>
-  </si>
-  <si>
-    <t>126383429</t>
-  </si>
-  <si>
-    <t>32432955</t>
-  </si>
-  <si>
-    <t>126383304</t>
-  </si>
-  <si>
-    <t>32432954</t>
-  </si>
-  <si>
-    <t>126383290</t>
-  </si>
-  <si>
-    <t>32432953</t>
-  </si>
-  <si>
-    <t>126383289</t>
-  </si>
-  <si>
-    <t>32432968</t>
-  </si>
-  <si>
-    <t>3438202</t>
-  </si>
-  <si>
-    <t>126383496</t>
-  </si>
-  <si>
-    <t>2022-07-18 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-18 23:13</t>
-  </si>
-  <si>
-    <t>3439103</t>
-  </si>
-  <si>
-    <t>3439109</t>
-  </si>
-  <si>
-    <t>32433849</t>
-  </si>
-  <si>
-    <t>126392504</t>
-  </si>
-  <si>
-    <t>32433848</t>
-  </si>
-  <si>
-    <t>126392490</t>
-  </si>
-  <si>
-    <t>32433847</t>
-  </si>
-  <si>
-    <t>126392489</t>
-  </si>
-  <si>
-    <t>32433846</t>
-  </si>
-  <si>
-    <t>126392478</t>
-  </si>
-  <si>
     <t>New Add ChName</t>
   </si>
   <si>
     <t>New Add ChValue</t>
   </si>
   <si>
-    <t>2022-07-16 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-16 23:13</t>
-  </si>
-  <si>
-    <t>126347836</t>
-  </si>
-  <si>
-    <t>3434537</t>
-  </si>
-  <si>
-    <t>3439337</t>
-  </si>
-  <si>
-    <t>3439343</t>
-  </si>
-  <si>
     <t>AOF - Agent Order Fee</t>
   </si>
   <si>
     <t>$185.00</t>
   </si>
   <si>
-    <t>126409345</t>
-  </si>
-  <si>
-    <t>126409367</t>
-  </si>
-  <si>
-    <t>126409389</t>
-  </si>
-  <si>
-    <t>126409404</t>
-  </si>
-  <si>
-    <t>126411753</t>
-  </si>
-  <si>
-    <t>126409068</t>
-  </si>
-  <si>
-    <t>126409471</t>
-  </si>
-  <si>
-    <t>126411029</t>
-  </si>
-  <si>
-    <t>32435724</t>
-  </si>
-  <si>
-    <t>3440958</t>
-  </si>
-  <si>
-    <t>126409356</t>
-  </si>
-  <si>
-    <t>32435725</t>
-  </si>
-  <si>
-    <t>3440959</t>
-  </si>
-  <si>
-    <t>126409378</t>
-  </si>
-  <si>
-    <t>32435726</t>
-  </si>
-  <si>
-    <t>3440960</t>
-  </si>
-  <si>
-    <t>126409390</t>
-  </si>
-  <si>
-    <t>32435732</t>
-  </si>
-  <si>
-    <t>3440966</t>
-  </si>
-  <si>
-    <t>126409460</t>
-  </si>
-  <si>
-    <t>32435731</t>
-  </si>
-  <si>
-    <t>3440965</t>
-  </si>
-  <si>
-    <t>126409459</t>
-  </si>
-  <si>
-    <t>32435730</t>
-  </si>
-  <si>
-    <t>3440964</t>
-  </si>
-  <si>
-    <t>126409448</t>
-  </si>
-  <si>
-    <t>32435729</t>
-  </si>
-  <si>
-    <t>3440963</t>
-  </si>
-  <si>
-    <t>126409437</t>
-  </si>
-  <si>
-    <t>32435728</t>
-  </si>
-  <si>
-    <t>3440962</t>
-  </si>
-  <si>
-    <t>126409426</t>
-  </si>
-  <si>
-    <t>32435727</t>
-  </si>
-  <si>
-    <t>3440961</t>
-  </si>
-  <si>
-    <t>126409415</t>
-  </si>
-  <si>
-    <t>32435954</t>
-  </si>
-  <si>
-    <t>3441188</t>
-  </si>
-  <si>
-    <t>126411797</t>
-  </si>
-  <si>
-    <t>32435953</t>
-  </si>
-  <si>
-    <t>3441187</t>
-  </si>
-  <si>
-    <t>126411786</t>
-  </si>
-  <si>
-    <t>32435952</t>
-  </si>
-  <si>
-    <t>3441186</t>
-  </si>
-  <si>
-    <t>126411775</t>
-  </si>
-  <si>
-    <t>32435951</t>
-  </si>
-  <si>
-    <t>3441185</t>
-  </si>
-  <si>
-    <t>126411764</t>
-  </si>
-  <si>
-    <t>32435700</t>
-  </si>
-  <si>
-    <t>3440934</t>
-  </si>
-  <si>
-    <t>126409091</t>
-  </si>
-  <si>
-    <t>32435699</t>
-  </si>
-  <si>
-    <t>3440933</t>
-  </si>
-  <si>
-    <t>126409080</t>
-  </si>
-  <si>
-    <t>32435698</t>
-  </si>
-  <si>
-    <t>3440932</t>
-  </si>
-  <si>
-    <t>126409079</t>
-  </si>
-  <si>
-    <t>32435733</t>
-  </si>
-  <si>
-    <t>3440967</t>
-  </si>
-  <si>
-    <t>126409482</t>
-  </si>
-  <si>
-    <t>2022-07-19 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-19 23:13</t>
-  </si>
-  <si>
-    <t>3441269</t>
-  </si>
-  <si>
-    <t>3441274</t>
+    <t>126425796</t>
+  </si>
+  <si>
+    <t>126425811</t>
+  </si>
+  <si>
+    <t>126425833</t>
+  </si>
+  <si>
+    <t>126425855</t>
+  </si>
+  <si>
+    <t>126427907</t>
+  </si>
+  <si>
+    <t>126425372</t>
+  </si>
+  <si>
+    <t>126425925</t>
+  </si>
+  <si>
+    <t>126427398</t>
+  </si>
+  <si>
+    <t>32437415</t>
+  </si>
+  <si>
+    <t>3442649</t>
+  </si>
+  <si>
+    <t>126425800</t>
+  </si>
+  <si>
+    <t>32437416</t>
+  </si>
+  <si>
+    <t>3442650</t>
+  </si>
+  <si>
+    <t>126425822</t>
+  </si>
+  <si>
+    <t>32437417</t>
+  </si>
+  <si>
+    <t>3442651</t>
+  </si>
+  <si>
+    <t>126425844</t>
+  </si>
+  <si>
+    <t>32437423</t>
+  </si>
+  <si>
+    <t>3442657</t>
+  </si>
+  <si>
+    <t>126425914</t>
+  </si>
+  <si>
+    <t>32437422</t>
+  </si>
+  <si>
+    <t>3442656</t>
+  </si>
+  <si>
+    <t>126425903</t>
+  </si>
+  <si>
+    <t>32437421</t>
+  </si>
+  <si>
+    <t>3442655</t>
+  </si>
+  <si>
+    <t>126425899</t>
+  </si>
+  <si>
+    <t>32437420</t>
+  </si>
+  <si>
+    <t>3442654</t>
+  </si>
+  <si>
+    <t>126425888</t>
+  </si>
+  <si>
+    <t>32437419</t>
+  </si>
+  <si>
+    <t>3442653</t>
+  </si>
+  <si>
+    <t>126425877</t>
+  </si>
+  <si>
+    <t>32437418</t>
+  </si>
+  <si>
+    <t>3442652</t>
+  </si>
+  <si>
+    <t>126425866</t>
+  </si>
+  <si>
+    <t>32437598</t>
+  </si>
+  <si>
+    <t>3442832</t>
+  </si>
+  <si>
+    <t>126427941</t>
+  </si>
+  <si>
+    <t>32437597</t>
+  </si>
+  <si>
+    <t>3442831</t>
+  </si>
+  <si>
+    <t>126427930</t>
+  </si>
+  <si>
+    <t>32437596</t>
+  </si>
+  <si>
+    <t>3442830</t>
+  </si>
+  <si>
+    <t>126427929</t>
+  </si>
+  <si>
+    <t>32437595</t>
+  </si>
+  <si>
+    <t>3442829</t>
+  </si>
+  <si>
+    <t>126427918</t>
+  </si>
+  <si>
+    <t>32437377</t>
+  </si>
+  <si>
+    <t>3442611</t>
+  </si>
+  <si>
+    <t>126425408</t>
+  </si>
+  <si>
+    <t>32437376</t>
+  </si>
+  <si>
+    <t>3442610</t>
+  </si>
+  <si>
+    <t>126425394</t>
+  </si>
+  <si>
+    <t>32437375</t>
+  </si>
+  <si>
+    <t>3442609</t>
+  </si>
+  <si>
+    <t>126425383</t>
+  </si>
+  <si>
+    <t>32437424</t>
+  </si>
+  <si>
+    <t>3442658</t>
+  </si>
+  <si>
+    <t>126425936</t>
+  </si>
+  <si>
+    <t>2022-07-20 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-20 23:13</t>
+  </si>
+  <si>
+    <t>3442890</t>
+  </si>
+  <si>
+    <t>3442899</t>
+  </si>
+  <si>
+    <t>3442925</t>
+  </si>
+  <si>
+    <t>3442932</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1220,7 +1050,7 @@
     <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -1255,7 +1085,6 @@
     <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="8" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="19" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1688,7 +1517,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,7 +1550,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1735,7 +1564,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1749,7 +1578,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1763,7 +1592,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1777,7 +1606,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1791,7 +1620,7 @@
         <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1805,7 +1634,7 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1819,7 +1648,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1848,7 +1677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -1884,19 +1713,19 @@
       <c r="F1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>103</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2">
         <v>3430874</v>
@@ -1908,7 +1737,7 @@
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
         <v>101</v>
@@ -1917,10 +1746,10 @@
         <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="I2" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1930,7 +1759,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="18"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
@@ -1941,7 +1770,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="18"/>
+      <c r="G4" s="17"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
@@ -1952,7 +1781,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
@@ -1963,7 +1792,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
@@ -1974,7 +1803,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="18"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
@@ -1985,7 +1814,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
@@ -1996,7 +1825,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
@@ -2007,7 +1836,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
@@ -2018,7 +1847,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
@@ -2029,7 +1858,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="18"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
@@ -2040,7 +1869,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="18"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
@@ -2051,7 +1880,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="17"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
@@ -2073,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,63 +1928,63 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" t="s">
-        <v>181</v>
+        <v>122</v>
+      </c>
+      <c r="C4">
+        <v>3442658</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2230,10 +2059,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2793,10 +2622,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2820,7 +2649,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>225</v>
+        <v>167</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -2851,7 +2680,7 @@
         <v>89</v>
       </c>
       <c r="J3" t="s">
-        <v>226</v>
+        <v>168</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -3265,10 +3094,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3536,7 +3365,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>171</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3544,7 +3373,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>172</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
@@ -3586,76 +3415,76 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>141</v>
       </c>
       <c r="D7" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3748,52 +3577,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3873,7 +3702,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3897,40 +3726,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>218</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>220</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes of 25th july 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" tabRatio="890" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
-    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
-    <sheet name="Rate" r:id="rId3" sheetId="3"/>
-    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
-    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
-    <sheet name="LocJob" r:id="rId6" sheetId="6"/>
-    <sheet name="OneToMany" r:id="rId7" sheetId="7"/>
-    <sheet name="ManyToOne" r:id="rId8" sheetId="8"/>
-    <sheet name="ManyToMany" r:id="rId9" sheetId="9"/>
-    <sheet name="CompareCharges" r:id="rId10" sheetId="10"/>
+    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
+    <sheet name="Rate" sheetId="3" r:id="rId3"/>
+    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
+    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="LocJob" sheetId="6" r:id="rId6"/>
+    <sheet name="OneToMany" sheetId="7" r:id="rId7"/>
+    <sheet name="ManyToOne" sheetId="8" r:id="rId8"/>
+    <sheet name="ManyToMany" sheetId="9" r:id="rId9"/>
+    <sheet name="CompareCharges" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="164">
   <si>
     <t>FileName</t>
   </si>
@@ -331,9 +331,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>RT00002407</t>
-  </si>
-  <si>
     <t>Charges on TC ACK stage</t>
   </si>
   <si>
@@ -349,206 +346,181 @@
     <t>$185.00</t>
   </si>
   <si>
-    <t>126425796</t>
-  </si>
-  <si>
-    <t>126425811</t>
-  </si>
-  <si>
-    <t>126425833</t>
-  </si>
-  <si>
-    <t>126425855</t>
-  </si>
-  <si>
-    <t>126427907</t>
-  </si>
-  <si>
-    <t>126425372</t>
-  </si>
-  <si>
-    <t>126425925</t>
-  </si>
-  <si>
-    <t>126427398</t>
-  </si>
-  <si>
-    <t>32437415</t>
-  </si>
-  <si>
-    <t>3442649</t>
-  </si>
-  <si>
-    <t>126425800</t>
-  </si>
-  <si>
-    <t>32437416</t>
-  </si>
-  <si>
-    <t>3442650</t>
-  </si>
-  <si>
-    <t>126425822</t>
-  </si>
-  <si>
-    <t>32437417</t>
-  </si>
-  <si>
-    <t>3442651</t>
-  </si>
-  <si>
-    <t>126425844</t>
-  </si>
-  <si>
-    <t>32437423</t>
-  </si>
-  <si>
-    <t>3442657</t>
-  </si>
-  <si>
-    <t>126425914</t>
-  </si>
-  <si>
-    <t>32437422</t>
-  </si>
-  <si>
-    <t>3442656</t>
-  </si>
-  <si>
-    <t>126425903</t>
-  </si>
-  <si>
-    <t>32437421</t>
-  </si>
-  <si>
-    <t>3442655</t>
-  </si>
-  <si>
-    <t>126425899</t>
-  </si>
-  <si>
-    <t>32437420</t>
-  </si>
-  <si>
-    <t>3442654</t>
-  </si>
-  <si>
-    <t>126425888</t>
-  </si>
-  <si>
-    <t>32437419</t>
-  </si>
-  <si>
-    <t>3442653</t>
-  </si>
-  <si>
-    <t>126425877</t>
-  </si>
-  <si>
-    <t>32437418</t>
-  </si>
-  <si>
-    <t>3442652</t>
-  </si>
-  <si>
-    <t>126425866</t>
-  </si>
-  <si>
-    <t>32437598</t>
-  </si>
-  <si>
-    <t>3442832</t>
-  </si>
-  <si>
-    <t>126427941</t>
-  </si>
-  <si>
-    <t>32437597</t>
-  </si>
-  <si>
-    <t>3442831</t>
-  </si>
-  <si>
-    <t>126427930</t>
-  </si>
-  <si>
-    <t>32437596</t>
-  </si>
-  <si>
-    <t>3442830</t>
-  </si>
-  <si>
-    <t>126427929</t>
-  </si>
-  <si>
-    <t>32437595</t>
-  </si>
-  <si>
-    <t>3442829</t>
-  </si>
-  <si>
-    <t>126427918</t>
-  </si>
-  <si>
-    <t>32437377</t>
-  </si>
-  <si>
-    <t>3442611</t>
-  </si>
-  <si>
-    <t>126425408</t>
-  </si>
-  <si>
-    <t>32437376</t>
-  </si>
-  <si>
-    <t>3442610</t>
-  </si>
-  <si>
-    <t>126425394</t>
-  </si>
-  <si>
-    <t>32437375</t>
-  </si>
-  <si>
-    <t>3442609</t>
-  </si>
-  <si>
-    <t>126425383</t>
-  </si>
-  <si>
-    <t>32437424</t>
-  </si>
-  <si>
-    <t>3442658</t>
-  </si>
-  <si>
-    <t>126425936</t>
-  </si>
-  <si>
-    <t>2022-07-20 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-20 23:13</t>
-  </si>
-  <si>
-    <t>3442890</t>
-  </si>
-  <si>
-    <t>3442899</t>
-  </si>
-  <si>
-    <t>3442925</t>
-  </si>
-  <si>
-    <t>3442932</t>
+    <t>126475768</t>
+  </si>
+  <si>
+    <t>126475780</t>
+  </si>
+  <si>
+    <t>126475805</t>
+  </si>
+  <si>
+    <t>126475827</t>
+  </si>
+  <si>
+    <t>126470187</t>
+  </si>
+  <si>
+    <t>126475643</t>
+  </si>
+  <si>
+    <t>126475894</t>
+  </si>
+  <si>
+    <t>126469880</t>
+  </si>
+  <si>
+    <t>32442423</t>
+  </si>
+  <si>
+    <t>3447657</t>
+  </si>
+  <si>
+    <t>126475779</t>
+  </si>
+  <si>
+    <t>32442424</t>
+  </si>
+  <si>
+    <t>3447658</t>
+  </si>
+  <si>
+    <t>126475791</t>
+  </si>
+  <si>
+    <t>32442425</t>
+  </si>
+  <si>
+    <t>126475816</t>
+  </si>
+  <si>
+    <t>32442431</t>
+  </si>
+  <si>
+    <t>126475883</t>
+  </si>
+  <si>
+    <t>32442430</t>
+  </si>
+  <si>
+    <t>126475872</t>
+  </si>
+  <si>
+    <t>32442429</t>
+  </si>
+  <si>
+    <t>126475861</t>
+  </si>
+  <si>
+    <t>32442428</t>
+  </si>
+  <si>
+    <t>126475850</t>
+  </si>
+  <si>
+    <t>32442427</t>
+  </si>
+  <si>
+    <t>126475849</t>
+  </si>
+  <si>
+    <t>32442426</t>
+  </si>
+  <si>
+    <t>126475838</t>
+  </si>
+  <si>
+    <t>32441886</t>
+  </si>
+  <si>
+    <t>3447120</t>
+  </si>
+  <si>
+    <t>126470224</t>
+  </si>
+  <si>
+    <t>32441885</t>
+  </si>
+  <si>
+    <t>3447119</t>
+  </si>
+  <si>
+    <t>126470213</t>
+  </si>
+  <si>
+    <t>32441884</t>
+  </si>
+  <si>
+    <t>3447118</t>
+  </si>
+  <si>
+    <t>126470202</t>
+  </si>
+  <si>
+    <t>32441883</t>
+  </si>
+  <si>
+    <t>3447117</t>
+  </si>
+  <si>
+    <t>126470198</t>
+  </si>
+  <si>
+    <t>32442415</t>
+  </si>
+  <si>
+    <t>126475676</t>
+  </si>
+  <si>
+    <t>32442414</t>
+  </si>
+  <si>
+    <t>126475665</t>
+  </si>
+  <si>
+    <t>32442413</t>
+  </si>
+  <si>
+    <t>126475654</t>
+  </si>
+  <si>
+    <t>32442432</t>
+  </si>
+  <si>
+    <t>3447666</t>
+  </si>
+  <si>
+    <t>126475908</t>
+  </si>
+  <si>
+    <t>3447853</t>
+  </si>
+  <si>
+    <t>RT00002485</t>
+  </si>
+  <si>
+    <t>2022-07-21 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-21 23:13</t>
+  </si>
+  <si>
+    <t>126443417</t>
+  </si>
+  <si>
+    <t>3444471</t>
+  </si>
+  <si>
+    <t>3448016</t>
+  </si>
+  <si>
+    <t>3448017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1007,132 +979,132 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="20" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="27" fontId="21" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="19" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1150,7 +1122,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1232,10 +1204,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1393,7 +1365,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1402,13 +1374,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1418,7 +1390,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1427,7 +1399,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1436,7 +1408,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1446,12 +1418,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1482,7 +1454,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1501,7 +1473,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1513,19 +1485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1550,7 +1522,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>47</v>
@@ -1564,7 +1536,7 @@
         <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>47</v>
@@ -1578,7 +1550,7 @@
         <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>47</v>
@@ -1592,7 +1564,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>48</v>
@@ -1606,7 +1578,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>49</v>
@@ -1620,7 +1592,7 @@
         <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>50</v>
@@ -1634,7 +1606,7 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>47</v>
@@ -1648,7 +1620,7 @@
         <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -1659,7 +1631,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1667,15 +1639,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
@@ -1683,15 +1655,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1714,30 +1686,30 @@
         <v>64</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3430874</v>
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
         <v>101</v>
@@ -1746,10 +1718,10 @@
         <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1886,30 +1858,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F14">
-    <cfRule dxfId="1" operator="equal" priority="1" type="cellIs">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule dxfId="0" operator="equal" priority="2" type="cellIs">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1928,78 +1900,78 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>116</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
         <v>119</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>120</v>
-      </c>
-      <c r="D3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4">
+        <v>3444471</v>
+      </c>
+      <c r="D4" t="s">
         <v>122</v>
-      </c>
-      <c r="C4">
-        <v>3442658</v>
-      </c>
-      <c r="D4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
@@ -2007,15 +1979,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2059,10 +2031,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2561,14 +2533,14 @@
       <c r="L31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -2576,13 +2548,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2622,10 +2594,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2649,7 +2621,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -2680,7 +2652,7 @@
         <v>89</v>
       </c>
       <c r="J3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -3051,13 +3023,13 @@
       <c r="K31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
@@ -3065,11 +3037,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3094,10 +3066,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3337,13 +3309,13 @@
       <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
@@ -3351,8 +3323,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3365,7 +3337,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3373,30 +3345,30 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3414,77 +3386,77 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>111</v>
+      <c r="A2">
+        <v>126475827</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="C2">
+        <v>3444472</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <v>3444473</v>
       </c>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" t="s">
-        <v>132</v>
+        <v>127</v>
+      </c>
+      <c r="C4">
+        <v>3444474</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>135</v>
+        <v>129</v>
+      </c>
+      <c r="C5">
+        <v>3444475</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" t="s">
-        <v>138</v>
+        <v>131</v>
+      </c>
+      <c r="C6">
+        <v>3444476</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" t="s">
-        <v>141</v>
+        <v>133</v>
+      </c>
+      <c r="C7">
+        <v>3444477</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3542,14 +3514,14 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
@@ -3557,8 +3529,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3577,52 +3549,52 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3692,22 +3664,24 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3726,40 +3700,40 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" t="s">
-        <v>156</v>
+        <v>147</v>
+      </c>
+      <c r="C2">
+        <v>3448004</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" t="s">
-        <v>159</v>
+        <v>149</v>
+      </c>
+      <c r="C3">
+        <v>3448005</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
+        <v>151</v>
+      </c>
+      <c r="C4">
+        <v>3448006</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,6 +3809,6 @@
       <c r="D16" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of OtoM and MtoO for search btn click event
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="228">
   <si>
     <t>FileName</t>
   </si>
@@ -692,6 +692,21 @@
   </si>
   <si>
     <t>126499746</t>
+  </si>
+  <si>
+    <t>2022-07-25 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-25 23:13</t>
+  </si>
+  <si>
+    <t>3450480</t>
+  </si>
+  <si>
+    <t>3450485</t>
+  </si>
+  <si>
+    <t>RT00002495</t>
   </si>
 </sst>
 </file>
@@ -1809,7 +1824,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>227</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1878,7 +1893,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>226</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -2209,10 +2224,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2772,10 +2787,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
@@ -2799,7 +2814,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>158</v>
+        <v>223</v>
       </c>
       <c r="K2" t="s">
         <v>85</v>
@@ -2830,7 +2845,7 @@
         <v>89</v>
       </c>
       <c r="J3" t="s">
-        <v>159</v>
+        <v>224</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -3244,10 +3259,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3515,7 +3530,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>225</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
@@ -3523,7 +3538,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>226</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Changes of 29th july 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_STG.xlsx
+++ b/RTE/src/main/resources/RTE_STG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="8" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
+    <workbookView activeTab="6" tabRatio="890" windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="227">
   <si>
     <t>FileName</t>
   </si>
@@ -346,367 +346,364 @@
     <t>$185.00</t>
   </si>
   <si>
-    <t>126475768</t>
-  </si>
-  <si>
-    <t>126475780</t>
-  </si>
-  <si>
-    <t>126475805</t>
-  </si>
-  <si>
-    <t>126475827</t>
-  </si>
-  <si>
-    <t>126470187</t>
-  </si>
-  <si>
-    <t>126475643</t>
-  </si>
-  <si>
-    <t>126475894</t>
-  </si>
-  <si>
-    <t>126469880</t>
-  </si>
-  <si>
-    <t>32442423</t>
-  </si>
-  <si>
-    <t>3447657</t>
-  </si>
-  <si>
-    <t>126475779</t>
-  </si>
-  <si>
-    <t>32442424</t>
-  </si>
-  <si>
-    <t>3447658</t>
-  </si>
-  <si>
-    <t>126475791</t>
-  </si>
-  <si>
-    <t>32442425</t>
-  </si>
-  <si>
-    <t>126475816</t>
-  </si>
-  <si>
-    <t>32442431</t>
-  </si>
-  <si>
-    <t>126475883</t>
-  </si>
-  <si>
-    <t>32442430</t>
-  </si>
-  <si>
-    <t>126475872</t>
-  </si>
-  <si>
-    <t>32442429</t>
-  </si>
-  <si>
-    <t>126475861</t>
-  </si>
-  <si>
-    <t>32442428</t>
-  </si>
-  <si>
-    <t>126475850</t>
-  </si>
-  <si>
-    <t>32442427</t>
-  </si>
-  <si>
-    <t>126475849</t>
-  </si>
-  <si>
-    <t>32442426</t>
-  </si>
-  <si>
-    <t>126475838</t>
-  </si>
-  <si>
-    <t>32441886</t>
-  </si>
-  <si>
-    <t>3447120</t>
-  </si>
-  <si>
-    <t>126470224</t>
-  </si>
-  <si>
-    <t>32441885</t>
-  </si>
-  <si>
-    <t>3447119</t>
-  </si>
-  <si>
-    <t>126470213</t>
-  </si>
-  <si>
-    <t>32441884</t>
-  </si>
-  <si>
-    <t>3447118</t>
-  </si>
-  <si>
-    <t>126470202</t>
-  </si>
-  <si>
-    <t>32441883</t>
-  </si>
-  <si>
-    <t>3447117</t>
-  </si>
-  <si>
-    <t>126470198</t>
-  </si>
-  <si>
-    <t>32442415</t>
-  </si>
-  <si>
-    <t>126475676</t>
-  </si>
-  <si>
-    <t>32442414</t>
-  </si>
-  <si>
-    <t>126475665</t>
-  </si>
-  <si>
-    <t>32442413</t>
-  </si>
-  <si>
-    <t>126475654</t>
-  </si>
-  <si>
-    <t>32442432</t>
-  </si>
-  <si>
-    <t>3447666</t>
-  </si>
-  <si>
-    <t>126475908</t>
-  </si>
-  <si>
-    <t>3447853</t>
-  </si>
-  <si>
-    <t>RT00002485</t>
-  </si>
-  <si>
-    <t>2022-07-21 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-21 23:13</t>
-  </si>
-  <si>
-    <t>126443417</t>
-  </si>
-  <si>
-    <t>3444471</t>
-  </si>
-  <si>
-    <t>3448016</t>
-  </si>
-  <si>
-    <t>3448017</t>
-  </si>
-  <si>
-    <t>126499609</t>
-  </si>
-  <si>
-    <t>126499621</t>
-  </si>
-  <si>
-    <t>126499643</t>
-  </si>
-  <si>
-    <t>126499665</t>
-  </si>
-  <si>
-    <t>126501939</t>
-  </si>
-  <si>
-    <t>126497317</t>
-  </si>
-  <si>
-    <t>126499735</t>
-  </si>
-  <si>
-    <t>126500895</t>
-  </si>
-  <si>
-    <t>32444924</t>
-  </si>
-  <si>
-    <t>3450158</t>
-  </si>
-  <si>
-    <t>126499610</t>
-  </si>
-  <si>
-    <t>32444925</t>
-  </si>
-  <si>
-    <t>3450159</t>
-  </si>
-  <si>
-    <t>126499632</t>
-  </si>
-  <si>
-    <t>32444926</t>
-  </si>
-  <si>
-    <t>3450160</t>
-  </si>
-  <si>
-    <t>126499654</t>
-  </si>
-  <si>
-    <t>32444932</t>
-  </si>
-  <si>
-    <t>3450166</t>
-  </si>
-  <si>
-    <t>126499724</t>
-  </si>
-  <si>
-    <t>32444931</t>
-  </si>
-  <si>
-    <t>3450165</t>
-  </si>
-  <si>
-    <t>126499713</t>
-  </si>
-  <si>
-    <t>32444930</t>
-  </si>
-  <si>
-    <t>3450164</t>
-  </si>
-  <si>
-    <t>126499702</t>
-  </si>
-  <si>
-    <t>32444929</t>
-  </si>
-  <si>
-    <t>3450163</t>
-  </si>
-  <si>
-    <t>126499698</t>
-  </si>
-  <si>
-    <t>32444928</t>
-  </si>
-  <si>
-    <t>3450162</t>
-  </si>
-  <si>
-    <t>126499687</t>
-  </si>
-  <si>
-    <t>32444927</t>
-  </si>
-  <si>
-    <t>3450161</t>
-  </si>
-  <si>
-    <t>126499676</t>
-  </si>
-  <si>
-    <t>32445129</t>
-  </si>
-  <si>
-    <t>3450363</t>
-  </si>
-  <si>
-    <t>126501973</t>
-  </si>
-  <si>
-    <t>32445128</t>
-  </si>
-  <si>
-    <t>3450362</t>
-  </si>
-  <si>
-    <t>126501962</t>
-  </si>
-  <si>
-    <t>32445127</t>
-  </si>
-  <si>
-    <t>3450361</t>
-  </si>
-  <si>
-    <t>126501951</t>
-  </si>
-  <si>
-    <t>32445126</t>
-  </si>
-  <si>
-    <t>3450360</t>
-  </si>
-  <si>
-    <t>126501940</t>
-  </si>
-  <si>
-    <t>32444699</t>
-  </si>
-  <si>
-    <t>3449933</t>
-  </si>
-  <si>
-    <t>126497340</t>
-  </si>
-  <si>
-    <t>32444698</t>
-  </si>
-  <si>
-    <t>3449932</t>
-  </si>
-  <si>
-    <t>126497339</t>
-  </si>
-  <si>
-    <t>32444697</t>
-  </si>
-  <si>
-    <t>3449931</t>
-  </si>
-  <si>
-    <t>126497328</t>
-  </si>
-  <si>
-    <t>32444933</t>
-  </si>
-  <si>
-    <t>3450167</t>
-  </si>
-  <si>
-    <t>126499746</t>
-  </si>
-  <si>
-    <t>2022-07-25 22:30</t>
-  </si>
-  <si>
-    <t>2022-07-25 23:13</t>
-  </si>
-  <si>
-    <t>3450480</t>
-  </si>
-  <si>
     <t>3450485</t>
   </si>
   <si>
     <t>RT00002495</t>
+  </si>
+  <si>
+    <t>126518881</t>
+  </si>
+  <si>
+    <t>3452254</t>
+  </si>
+  <si>
+    <t>3452255</t>
+  </si>
+  <si>
+    <t>126518917</t>
+  </si>
+  <si>
+    <t>2022-07-26 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-26 23:13</t>
+  </si>
+  <si>
+    <t>3452558</t>
+  </si>
+  <si>
+    <t>3452561</t>
+  </si>
+  <si>
+    <t>126536096</t>
+  </si>
+  <si>
+    <t>126536111</t>
+  </si>
+  <si>
+    <t>126536133</t>
+  </si>
+  <si>
+    <t>126536155</t>
+  </si>
+  <si>
+    <t>126538573</t>
+  </si>
+  <si>
+    <t>126535527</t>
+  </si>
+  <si>
+    <t>126536225</t>
+  </si>
+  <si>
+    <t>126537794</t>
+  </si>
+  <si>
+    <t>32448836</t>
+  </si>
+  <si>
+    <t>3454070</t>
+  </si>
+  <si>
+    <t>126536100</t>
+  </si>
+  <si>
+    <t>32448837</t>
+  </si>
+  <si>
+    <t>3454071</t>
+  </si>
+  <si>
+    <t>126536122</t>
+  </si>
+  <si>
+    <t>32448838</t>
+  </si>
+  <si>
+    <t>3454072</t>
+  </si>
+  <si>
+    <t>126536144</t>
+  </si>
+  <si>
+    <t>126536214</t>
+  </si>
+  <si>
+    <t>126536203</t>
+  </si>
+  <si>
+    <t>126536199</t>
+  </si>
+  <si>
+    <t>126536188</t>
+  </si>
+  <si>
+    <t>126536177</t>
+  </si>
+  <si>
+    <t>126536166</t>
+  </si>
+  <si>
+    <t>32449053</t>
+  </si>
+  <si>
+    <t>3454287</t>
+  </si>
+  <si>
+    <t>126538610</t>
+  </si>
+  <si>
+    <t>32449052</t>
+  </si>
+  <si>
+    <t>3454286</t>
+  </si>
+  <si>
+    <t>126538609</t>
+  </si>
+  <si>
+    <t>32449051</t>
+  </si>
+  <si>
+    <t>3454285</t>
+  </si>
+  <si>
+    <t>126538595</t>
+  </si>
+  <si>
+    <t>32449050</t>
+  </si>
+  <si>
+    <t>3454284</t>
+  </si>
+  <si>
+    <t>126538584</t>
+  </si>
+  <si>
+    <t>32448783</t>
+  </si>
+  <si>
+    <t>3454017</t>
+  </si>
+  <si>
+    <t>126535550</t>
+  </si>
+  <si>
+    <t>32448782</t>
+  </si>
+  <si>
+    <t>3454016</t>
+  </si>
+  <si>
+    <t>126535549</t>
+  </si>
+  <si>
+    <t>32448781</t>
+  </si>
+  <si>
+    <t>3454015</t>
+  </si>
+  <si>
+    <t>126535538</t>
+  </si>
+  <si>
+    <t>32448845</t>
+  </si>
+  <si>
+    <t>3454079</t>
+  </si>
+  <si>
+    <t>126536236</t>
+  </si>
+  <si>
+    <t>126560134</t>
+  </si>
+  <si>
+    <t>126560156</t>
+  </si>
+  <si>
+    <t>126560178</t>
+  </si>
+  <si>
+    <t>126560190</t>
+  </si>
+  <si>
+    <t>126564213</t>
+  </si>
+  <si>
+    <t>126559745</t>
+  </si>
+  <si>
+    <t>126560260</t>
+  </si>
+  <si>
+    <t>126561511</t>
+  </si>
+  <si>
+    <t>32451230</t>
+  </si>
+  <si>
+    <t>3456464</t>
+  </si>
+  <si>
+    <t>126560145</t>
+  </si>
+  <si>
+    <t>32451231</t>
+  </si>
+  <si>
+    <t>3456465</t>
+  </si>
+  <si>
+    <t>126560167</t>
+  </si>
+  <si>
+    <t>32451232</t>
+  </si>
+  <si>
+    <t>3456466</t>
+  </si>
+  <si>
+    <t>126560189</t>
+  </si>
+  <si>
+    <t>32451238</t>
+  </si>
+  <si>
+    <t>3456472</t>
+  </si>
+  <si>
+    <t>126560259</t>
+  </si>
+  <si>
+    <t>32451237</t>
+  </si>
+  <si>
+    <t>3456471</t>
+  </si>
+  <si>
+    <t>126560248</t>
+  </si>
+  <si>
+    <t>32451236</t>
+  </si>
+  <si>
+    <t>3456470</t>
+  </si>
+  <si>
+    <t>126560237</t>
+  </si>
+  <si>
+    <t>32451235</t>
+  </si>
+  <si>
+    <t>3456469</t>
+  </si>
+  <si>
+    <t>126560226</t>
+  </si>
+  <si>
+    <t>32451234</t>
+  </si>
+  <si>
+    <t>3456468</t>
+  </si>
+  <si>
+    <t>126560215</t>
+  </si>
+  <si>
+    <t>32451233</t>
+  </si>
+  <si>
+    <t>3456467</t>
+  </si>
+  <si>
+    <t>126560204</t>
+  </si>
+  <si>
+    <t>32451612</t>
+  </si>
+  <si>
+    <t>3456846</t>
+  </si>
+  <si>
+    <t>126564257</t>
+  </si>
+  <si>
+    <t>32451611</t>
+  </si>
+  <si>
+    <t>3456845</t>
+  </si>
+  <si>
+    <t>126564246</t>
+  </si>
+  <si>
+    <t>32451610</t>
+  </si>
+  <si>
+    <t>3456844</t>
+  </si>
+  <si>
+    <t>126564235</t>
+  </si>
+  <si>
+    <t>32451609</t>
+  </si>
+  <si>
+    <t>3456843</t>
+  </si>
+  <si>
+    <t>126564224</t>
+  </si>
+  <si>
+    <t>32451195</t>
+  </si>
+  <si>
+    <t>3456429</t>
+  </si>
+  <si>
+    <t>126559778</t>
+  </si>
+  <si>
+    <t>32451194</t>
+  </si>
+  <si>
+    <t>3456428</t>
+  </si>
+  <si>
+    <t>126559767</t>
+  </si>
+  <si>
+    <t>32451193</t>
+  </si>
+  <si>
+    <t>3456427</t>
+  </si>
+  <si>
+    <t>126559756</t>
+  </si>
+  <si>
+    <t>32451239</t>
+  </si>
+  <si>
+    <t>3456473</t>
+  </si>
+  <si>
+    <t>126560271</t>
+  </si>
+  <si>
+    <t>2022-07-28 22:30</t>
+  </si>
+  <si>
+    <t>2022-07-28 23:13</t>
+  </si>
+  <si>
+    <t>3476927</t>
+  </si>
+  <si>
+    <t>3476929</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1821,7 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>108</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="8" t="s">
@@ -1893,7 +1890,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -3553,8 +3550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,8 +3863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>